<commit_message>
Add private equity sheet to Airlines, more updates
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7288EFC7-862C-48F9-A92D-1531CD32A35E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A37F56-55F3-4D0C-B0CF-8641C6509245}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="1" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
+    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
   <sheets>
     <sheet name="Industry Screening" sheetId="2" r:id="rId1"/>
     <sheet name="Main" sheetId="1" r:id="rId2"/>
+    <sheet name="Private Equity" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
     <author>Charlie George</author>
   </authors>
   <commentList>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
       <text>
         <r>
           <rPr>
@@ -63,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
+    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
       <text>
         <r>
           <rPr>
@@ -76,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
       <text>
         <r>
           <rPr>
@@ -89,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
+    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
       <text>
         <r>
           <rPr>
@@ -102,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
       <text>
         <r>
           <rPr>
@@ -115,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
+    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
       <text>
         <r>
           <rPr>
@@ -128,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
       <text>
         <r>
           <rPr>
@@ -141,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
+    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
       <text>
         <r>
           <rPr>
@@ -154,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
+    <comment ref="P9" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
       <text>
         <r>
           <rPr>
@@ -219,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="426">
   <si>
     <t>Ticker</t>
   </si>
@@ -290,9 +291,6 @@
     <t>TUI AG</t>
   </si>
   <si>
-    <t>No. Aircraft</t>
-  </si>
-  <si>
     <t>Aircraft Orders</t>
   </si>
   <si>
@@ -1425,6 +1423,81 @@
   </si>
   <si>
     <t>Flag carrier for China, 1/3 of "Big Three" chinese airlines</t>
+  </si>
+  <si>
+    <t>$DAL</t>
+  </si>
+  <si>
+    <t>US legacy carrier &amp; one of the world's oldest airlines, 2nd largest airline</t>
+  </si>
+  <si>
+    <t>S/O</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Valuation</t>
+  </si>
+  <si>
+    <t>Founded</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Flybe</t>
+  </si>
+  <si>
+    <t>Thyme Investco Ltd. (Affiliate of Cyrus Capital Partners)</t>
+  </si>
+  <si>
+    <t>Fleet Size</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>No Destinations</t>
+  </si>
+  <si>
+    <t>Virgin Atlantic</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Wiki</t>
+  </si>
+  <si>
+    <t>Inent to join SkyTeam airline alliance in 2023</t>
+  </si>
+  <si>
+    <t>51% Virgin Group, 49% Delta Air Lines</t>
+  </si>
+  <si>
+    <t>Investors/Ownership</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Eastern Airways</t>
+  </si>
+  <si>
+    <t>10~</t>
+  </si>
+  <si>
+    <t>Regional short-haul airline</t>
+  </si>
+  <si>
+    <t>Long-haul airline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flybe 1979-2020 collapsed in March 2020, brand bought out by Cyrus Capital with a plan to relaunch </t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1641,13 +1714,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1710,7 +1801,16 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1720,6 +1820,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1754,6 +1857,11 @@
         <row r="6">
           <cell r="C6">
             <v>1.2050000000000001</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>4950</v>
           </cell>
         </row>
         <row r="8">
@@ -1794,6 +1902,11 @@
             <v>4.5199999999999996</v>
           </cell>
         </row>
+        <row r="7">
+          <cell r="C7">
+            <v>758</v>
+          </cell>
+        </row>
         <row r="8">
           <cell r="C8">
             <v>3426.16</v>
@@ -1817,7 +1930,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1838,6 +1951,11 @@
             <v>23.2</v>
           </cell>
         </row>
+        <row r="7">
+          <cell r="C7">
+            <v>103.7</v>
+          </cell>
+        </row>
         <row r="8">
           <cell r="C8">
             <v>2405.84</v>
@@ -1854,13 +1972,11 @@
           </cell>
         </row>
         <row r="21">
-          <cell r="D21">
-            <v>153</v>
-          </cell>
+          <cell r="D21"/>
         </row>
         <row r="22">
           <cell r="D22">
-            <v>315</v>
+            <v>153</v>
           </cell>
         </row>
       </sheetData>
@@ -1871,7 +1987,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1890,6 +2006,11 @@
         <row r="6">
           <cell r="C6">
             <v>10.029999999999999</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>214.62</v>
           </cell>
         </row>
         <row r="8">
@@ -2282,8 +2403,8 @@
   </sheetPr>
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C21" sqref="B7:C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2295,63 +2416,63 @@
     <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>43</v>
-      </c>
       <c r="D2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="G2" s="8">
         <v>45.94</v>
@@ -2363,7 +2484,7 @@
         <v>17.64</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="9">
         <v>0.64759999999999995</v>
@@ -2372,7 +2493,7 @@
         <v>44756</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N2" s="11">
         <v>-1.8700000000000001E-2</v>
@@ -2380,22 +2501,22 @@
     </row>
     <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="D3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="G3" s="8">
         <v>51.16</v>
@@ -2407,7 +2528,7 @@
         <v>17.64</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K3" s="9">
         <v>0.66100000000000003</v>
@@ -2424,22 +2545,22 @@
     </row>
     <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="G4" s="8">
         <v>43.53</v>
@@ -2468,22 +2589,22 @@
     </row>
     <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="G5" s="8">
         <v>45.33</v>
@@ -2495,7 +2616,7 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K5" s="9">
         <v>0.77129999999999999</v>
@@ -2504,7 +2625,7 @@
         <v>44770</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N5" s="11">
         <v>-3.6799999999999999E-2</v>
@@ -2512,34 +2633,34 @@
     </row>
     <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="D6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="F6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" s="7">
         <v>16.739999999999998</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6" s="8">
         <v>1.65</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K6" s="13">
         <v>0.4516</v>
@@ -2548,7 +2669,7 @@
         <v>44767</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N6" s="11">
         <v>-2.86E-2</v>
@@ -2556,40 +2677,40 @@
     </row>
     <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="D7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="F7" s="14">
         <v>-171</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" s="8">
         <v>1.65</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K7" s="13">
         <v>0.3901</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M7" s="12">
         <v>14.414999999999999</v>
@@ -2600,40 +2721,40 @@
     </row>
     <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="21" t="s">
+      <c r="D8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="F8" s="14">
         <v>-171</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="8">
         <v>1.65</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K8" s="13">
         <v>0.29320000000000002</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M8" s="12">
         <v>14.164999999999999</v>
@@ -2644,25 +2765,25 @@
     </row>
     <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>81</v>
-      </c>
       <c r="G9" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H9" s="8">
         <v>189.59</v>
@@ -2671,13 +2792,13 @@
         <v>1.65</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" s="13">
         <v>0.435</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M9" s="12">
         <v>14.135</v>
@@ -2688,28 +2809,28 @@
     </row>
     <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="D10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="G10" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10" s="8">
         <v>3.79</v>
@@ -2721,10 +2842,10 @@
         <v>0</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N10" s="9">
         <v>2.1499999999999998E-2</v>
@@ -2735,40 +2856,40 @@
         <v>753</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="D11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="F11" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="7">
         <v>10.95</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I11" s="8">
         <v>3.86</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K11" s="11">
         <v>7.9399999999999998E-2</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N11" s="9">
         <v>1.24E-2</v>
@@ -2776,34 +2897,34 @@
     </row>
     <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="G12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12" s="8">
         <v>12.56</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K12" s="9">
         <v>0.58950000000000002</v>
@@ -2812,7 +2933,7 @@
         <v>44669</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N12" s="11">
         <v>-2.93E-2</v>
@@ -2820,34 +2941,34 @@
     </row>
     <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="G13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I13" s="8">
         <v>12.56</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K13" s="9">
         <v>0.5917</v>
@@ -2856,7 +2977,7 @@
         <v>44762</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N13" s="11">
         <v>-2.2499999999999999E-2</v>
@@ -2864,34 +2985,34 @@
     </row>
     <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I14" s="8">
         <v>12.56</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K14" s="9">
         <v>0.58950000000000002</v>
@@ -2911,40 +3032,40 @@
         <v>1055</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="G15" s="7">
         <v>17.61</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I15" s="8">
         <v>3.76</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="13">
         <v>0.14680000000000001</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N15" s="11">
         <v>-9.1999999999999998E-3</v>
@@ -2952,34 +3073,34 @@
     </row>
     <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="F16" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="7">
         <v>4.28</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I16" s="8">
         <v>3.53</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K16" s="11">
         <v>7.0000000000000001E-3</v>
@@ -2988,7 +3109,7 @@
         <v>44799</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N16" s="11">
         <v>-4.4900000000000002E-2</v>
@@ -2999,40 +3120,40 @@
         <v>670</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="G17" s="7">
         <v>11.89</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I17" s="8">
         <v>4.3899999999999997</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K17" s="11">
         <v>6.7599999999999993E-2</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N17" s="9">
         <v>7.1999999999999998E-3</v>
@@ -3040,34 +3161,34 @@
     </row>
     <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>126</v>
-      </c>
       <c r="G18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I18" s="7">
         <v>-10.06</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K18" s="9">
         <v>0.55430000000000001</v>
@@ -3084,43 +3205,43 @@
     </row>
     <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="F19" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G19" s="7">
         <v>4.13</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I19" s="8">
         <v>4.51</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K19" s="11">
         <v>1.9E-3</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="11">
         <v>-2.5399999999999999E-2</v>
@@ -3128,34 +3249,34 @@
     </row>
     <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>136</v>
-      </c>
       <c r="G20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I20" s="7">
         <v>-10.06</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K20" s="9">
         <v>0.55430000000000001</v>
@@ -3164,7 +3285,7 @@
         <v>44763</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N20" s="11">
         <v>-2.07E-2</v>
@@ -3172,43 +3293,43 @@
     </row>
     <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="D21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="G21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I21" s="8">
         <v>409.03</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K21" s="13">
         <v>0.1454</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N21" s="9">
         <v>4.0000000000000001E-3</v>
@@ -3216,34 +3337,34 @@
     </row>
     <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="F22" s="14">
         <v>-25</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I22" s="8">
         <v>8.5500000000000007</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K22" s="13">
         <v>0.17899999999999999</v>
@@ -3260,43 +3381,43 @@
     </row>
     <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>140</v>
-      </c>
       <c r="C23" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="G23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I23" s="8">
         <v>6.17</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K23" s="13">
         <v>0.16120000000000001</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N23" s="11">
         <v>-7.1000000000000004E-3</v>
@@ -3307,40 +3428,40 @@
         <v>12</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="F24" s="14">
         <v>-2.25</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I24" s="8">
         <v>39.950000000000003</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K24" s="13">
         <v>0.1384</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N24" s="11">
         <v>-4.53E-2</v>
@@ -3348,43 +3469,43 @@
     </row>
     <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="F25" s="14">
         <v>-2.25</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I25" s="8">
         <v>39.950000000000003</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K25" s="11">
         <v>1E-4</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N25" s="11">
         <v>-2.4500000000000001E-2</v>
@@ -3392,44 +3513,44 @@
     </row>
     <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="D26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="F26" s="8" t="e" cm="1" vm="1">
         <f t="array" ref="F26">-_FV(AUD$353,"00")</f>
         <v>#VALUE!</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I26" s="8">
         <v>39.47</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K26" s="13">
         <v>0.1694</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N26" s="11">
         <v>-3.1E-2</v>
@@ -3440,19 +3561,19 @@
         <v>293</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C27" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="G27" s="7">
         <v>19.07</v>
@@ -3464,7 +3585,7 @@
         <v>1.72</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K27" s="11">
         <v>4.2099999999999999E-2</v>
@@ -3473,7 +3594,7 @@
         <v>44783</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N27" s="11">
         <v>-1.09E-2</v>
@@ -3481,25 +3602,25 @@
     </row>
     <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>176</v>
-      </c>
       <c r="F28" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H28" s="8">
         <v>18.88</v>
@@ -3508,16 +3629,16 @@
         <v>2.36</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K28" s="11">
         <v>0</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N28" s="9">
         <v>4.7399999999999998E-2</v>
@@ -3525,22 +3646,22 @@
     </row>
     <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C29" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="G29" s="15">
         <v>12.52</v>
@@ -3552,7 +3673,7 @@
         <v>2.67</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K29" s="9">
         <v>0.80210000000000004</v>
@@ -3561,7 +3682,7 @@
         <v>44763</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N29" s="11">
         <v>-3.04E-2</v>
@@ -3569,44 +3690,44 @@
     </row>
     <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="D30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="F30" s="8" t="e" cm="1" vm="2">
         <f t="array" ref="F30">-_FV(#REF!,"52")</f>
         <v>#VALUE!</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I30" s="16">
         <v>3400.56</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K30" s="13">
         <v>0.2258</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N30" s="9">
         <v>1.5299999999999999E-2</v>
@@ -3620,37 +3741,37 @@
         <v>14</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F31" s="17">
         <v>-772</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I31" s="8">
         <v>2.7</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K31" s="13">
         <v>0.4672</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N31" s="11">
         <v>-3.85E-2</v>
@@ -3664,37 +3785,37 @@
         <v>13</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F32" s="14">
         <v>-377.7</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I32" s="8">
         <v>4.2</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K32" s="9">
         <v>0.54359999999999997</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N32" s="11">
         <v>-6.9500000000000006E-2</v>
@@ -3702,34 +3823,34 @@
     </row>
     <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="F33" s="8" t="s">
-        <v>200</v>
-      </c>
       <c r="G33" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I33" s="8">
         <v>2.54</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K33" s="9">
         <v>0.79769999999999996</v>
@@ -3746,34 +3867,34 @@
     </row>
     <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C34" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>205</v>
-      </c>
       <c r="G34" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I34" s="8">
         <v>2.54</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K34" s="9">
         <v>0.81630000000000003</v>
@@ -3782,7 +3903,7 @@
         <v>44768</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N34" s="11">
         <v>-9.5999999999999992E-3</v>
@@ -3790,40 +3911,40 @@
     </row>
     <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="F35" s="14">
         <v>-247</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I35" s="7">
         <v>-4.95</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K35" s="13">
         <v>0.1099</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M35" s="12">
         <v>1.798</v>
@@ -3834,22 +3955,22 @@
     </row>
     <row r="36" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C36" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="7" t="s">
+      <c r="F36" s="7" t="s">
         <v>214</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>215</v>
       </c>
       <c r="G36" s="8">
         <v>33.75</v>
@@ -3861,7 +3982,7 @@
         <v>2.27</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K36" s="9">
         <v>1</v>
@@ -3870,7 +3991,7 @@
         <v>44776</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N36" s="9">
         <v>2.5000000000000001E-3</v>
@@ -3878,22 +3999,22 @@
     </row>
     <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="C37" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="G37" s="7">
         <v>19</v>
@@ -3905,7 +4026,7 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K37" s="9">
         <v>0.88719999999999999</v>
@@ -3914,7 +4035,7 @@
         <v>44769</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N37" s="11">
         <v>-4.1000000000000002E-2</v>
@@ -3922,43 +4043,43 @@
     </row>
     <row r="38" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>224</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>225</v>
       </c>
       <c r="F38" s="14">
         <v>-247</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I38" s="7">
         <v>-9.02</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K38" s="11">
         <v>1.5299999999999999E-2</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N38" s="9">
         <v>0</v>
@@ -3966,28 +4087,28 @@
     </row>
     <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C39" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>231</v>
-      </c>
       <c r="G39" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I39" s="8">
         <v>3.04</v>
@@ -4010,34 +4131,34 @@
     </row>
     <row r="40" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="C40" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="7" t="s">
+      <c r="F40" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="F40" s="8" t="s">
-        <v>235</v>
-      </c>
       <c r="G40" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I40" s="8">
         <v>3.04</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K40" s="9">
         <v>0.63200000000000001</v>
@@ -4046,7 +4167,7 @@
         <v>44768</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N40" s="9">
         <v>1.84E-2</v>
@@ -4054,34 +4175,34 @@
     </row>
     <row r="41" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C41" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>240</v>
-      </c>
       <c r="G41" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I41" s="8">
         <v>3.04</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K41" s="9">
         <v>0.68369999999999997</v>
@@ -4090,7 +4211,7 @@
         <v>44769</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N41" s="9">
         <v>1.5299999999999999E-2</v>
@@ -4098,22 +4219,22 @@
     </row>
     <row r="42" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="C42" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>245</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>246</v>
       </c>
       <c r="G42" s="7">
         <v>16.329999999999998</v>
@@ -4125,7 +4246,7 @@
         <v>11.72</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K42" s="9">
         <v>0.58279999999999998</v>
@@ -4134,7 +4255,7 @@
         <v>44756</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N42" s="11">
         <v>-3.85E-2</v>
@@ -4142,22 +4263,22 @@
     </row>
     <row r="43" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" s="15" t="s">
+      <c r="F43" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="G43" s="7">
         <v>9.67</v>
@@ -4169,16 +4290,16 @@
         <v>1.98</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K43" s="13">
         <v>0.41289999999999999</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N43" s="11">
         <v>-3.2000000000000002E-3</v>
@@ -4186,34 +4307,34 @@
     </row>
     <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>256</v>
-      </c>
       <c r="C44" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G44" s="7">
         <v>14.45</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I44" s="7">
         <v>-2.0099999999999998</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K44" s="13">
         <v>0.3846</v>
@@ -4222,7 +4343,7 @@
         <v>44784</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N44" s="11">
         <v>-4.36E-2</v>
@@ -4230,22 +4351,22 @@
     </row>
     <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E45" s="15" t="s">
+      <c r="F45" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>262</v>
       </c>
       <c r="G45" s="8">
         <v>26.04</v>
@@ -4257,16 +4378,16 @@
         <v>2.23</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K45" s="11">
         <v>6.0100000000000001E-2</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N45" s="9">
         <v>5.8999999999999999E-3</v>
@@ -4274,34 +4395,34 @@
     </row>
     <row r="46" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="C46" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="C46" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>267</v>
-      </c>
       <c r="F46" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G46" s="8">
         <v>62.13</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I46" s="7">
         <v>-1.68</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K46" s="13">
         <v>0.1178</v>
@@ -4310,7 +4431,7 @@
         <v>44770</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N46" s="11">
         <v>-4.1200000000000001E-2</v>
@@ -4318,22 +4439,22 @@
     </row>
     <row r="47" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="C47" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="15" t="s">
+      <c r="F47" s="7" t="s">
         <v>272</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="G47" s="7">
         <v>14.47</v>
@@ -4345,7 +4466,7 @@
         <v>2.14</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K47" s="9">
         <v>0.87429999999999997</v>
@@ -4354,7 +4475,7 @@
         <v>44770</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N47" s="11">
         <v>-5.2600000000000001E-2</v>
@@ -4362,40 +4483,40 @@
     </row>
     <row r="48" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>276</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>277</v>
       </c>
       <c r="F48" s="14">
         <v>-247</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I48" s="7">
         <v>-4.95</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K48" s="13">
         <v>0.1062</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M48" s="12">
         <v>1.8149999999999999</v>
@@ -4406,43 +4527,43 @@
     </row>
     <row r="49" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="C49" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="C49" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>281</v>
-      </c>
       <c r="F49" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G49" s="7">
         <v>16.87</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K49" s="11">
         <v>4.0500000000000001E-2</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N49" s="9">
         <v>0</v>
@@ -4450,44 +4571,44 @@
     </row>
     <row r="50" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="C50" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="15" t="s">
         <v>285</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>286</v>
       </c>
       <c r="F50" s="8" t="e" cm="1" vm="1">
         <f t="array" ref="F50">-_FV(NZD$261,"00")</f>
         <v>#VALUE!</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I50" s="8">
         <v>5.0599999999999996</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K50" s="11">
         <v>2.2800000000000001E-2</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N50" s="11">
         <v>-1.4E-3</v>
@@ -4495,44 +4616,44 @@
     </row>
     <row r="51" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="15" t="s">
         <v>290</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>291</v>
       </c>
       <c r="F51" s="8" t="e" cm="1" vm="1">
         <f t="array" ref="F51">-_FV(NZD$261,"00")</f>
         <v>#VALUE!</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I51" s="8">
         <v>5.0599999999999996</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K51" s="11">
         <v>2.2800000000000001E-2</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N51" s="11">
         <v>-3.3300000000000003E-2</v>
@@ -4540,34 +4661,34 @@
     </row>
     <row r="52" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="C52" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="C52" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E52" s="15" t="s">
+      <c r="F52" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>297</v>
-      </c>
       <c r="G52" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I52" s="8">
         <v>7.14</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K52" s="9">
         <v>0.82489999999999997</v>
@@ -4576,7 +4697,7 @@
         <v>44768</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N52" s="11">
         <v>-5.5E-2</v>
@@ -4584,25 +4705,25 @@
     </row>
     <row r="53" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="C53" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E53" s="15" t="s">
+      <c r="F53" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="F53" s="7" t="s">
-        <v>303</v>
-      </c>
       <c r="G53" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H53" s="15">
         <v>10.99</v>
@@ -4617,10 +4738,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N53" s="9">
         <v>0</v>
@@ -4628,22 +4749,22 @@
     </row>
     <row r="54" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="C54" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="C54" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E54" s="15" t="s">
+      <c r="F54" s="7" t="s">
         <v>307</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>308</v>
       </c>
       <c r="G54" s="8">
         <v>275.27999999999997</v>
@@ -4655,7 +4776,7 @@
         <v>3.61</v>
       </c>
       <c r="J54" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K54" s="11">
         <v>8.4599999999999995E-2</v>
@@ -4664,7 +4785,7 @@
         <v>44656</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N54" s="9">
         <v>2.7699999999999999E-2</v>
@@ -4672,22 +4793,22 @@
     </row>
     <row r="55" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="C55" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="C55" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E55" s="8" t="s">
+      <c r="F55" s="15" t="s">
         <v>313</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>314</v>
       </c>
       <c r="G55" s="15">
         <v>19.47</v>
@@ -4699,16 +4820,16 @@
         <v>0.9</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K55" s="13">
         <v>0.1381</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M55" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N55" s="9">
         <v>9.9000000000000008E-3</v>
@@ -4716,43 +4837,43 @@
     </row>
     <row r="56" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="C56" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="C56" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E56" s="8" t="s">
+      <c r="F56" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>320</v>
-      </c>
       <c r="G56" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I56" s="7">
         <v>-5.37</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K56" s="11">
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N56" s="11">
         <v>-1.2699999999999999E-2</v>
@@ -4760,25 +4881,25 @@
     </row>
     <row r="57" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="C57" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E57" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="F57" s="7" t="s">
-        <v>324</v>
-      </c>
       <c r="G57" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H57" s="8">
         <v>16.399999999999999</v>
@@ -4787,16 +4908,16 @@
         <v>-9.1999999999999993</v>
       </c>
       <c r="J57" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K57" s="13">
         <v>0.12870000000000001</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N57" s="11">
         <v>-2.0899999999999998E-2</v>
@@ -4804,43 +4925,43 @@
     </row>
     <row r="58" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="C58" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="C58" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E58" s="8" t="s">
+      <c r="F58" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="F58" s="8" t="s">
-        <v>330</v>
-      </c>
       <c r="G58" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I58" s="7">
         <v>-2.89</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K58" s="11">
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N58" s="11">
         <v>-2.7799999999999998E-2</v>
@@ -4848,28 +4969,28 @@
     </row>
     <row r="59" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="C59" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="C59" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E59" s="8" t="s">
+      <c r="F59" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="F59" s="8" t="s">
-        <v>336</v>
-      </c>
       <c r="G59" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I59" s="7">
         <v>-6.15</v>
@@ -4881,10 +5002,10 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M59" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N59" s="9">
         <v>0</v>
@@ -4892,43 +5013,43 @@
     </row>
     <row r="60" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="C60" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="C60" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E60" s="8" t="s">
+      <c r="F60" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="G60" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J60" s="8" t="s">
         <v>341</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I60" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J60" s="8" t="s">
-        <v>342</v>
       </c>
       <c r="K60" s="11">
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N60" s="9">
         <v>3.0999999999999999E-3</v>
@@ -4936,34 +5057,34 @@
     </row>
     <row r="61" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="C61" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="C61" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>346</v>
-      </c>
       <c r="F61" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G61" s="7">
         <v>0</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I61" s="8">
         <v>1.98</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K61" s="9">
         <v>0.5343</v>
@@ -4972,7 +5093,7 @@
         <v>44781</v>
       </c>
       <c r="M61" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N61" s="11">
         <v>-3.7199999999999997E-2</v>
@@ -4980,44 +5101,44 @@
     </row>
     <row r="62" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="C62" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>350</v>
-      </c>
-      <c r="C62" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>351</v>
       </c>
       <c r="F62" s="8" t="e" cm="1" vm="2">
         <f t="array" ref="F62">-_FV(AUD$68,"52")</f>
         <v>#VALUE!</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I62" s="8">
         <v>1.38</v>
       </c>
       <c r="J62" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K62" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M62" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N62" s="11">
         <v>-4.4000000000000003E-3</v>
@@ -5025,28 +5146,28 @@
     </row>
     <row r="63" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="C63" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="D63" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="D63" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E63" s="8" t="s">
+      <c r="F63" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="F63" s="8" t="s">
-        <v>358</v>
-      </c>
       <c r="G63" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I63" s="8">
         <v>105.95</v>
@@ -5058,10 +5179,10 @@
         <v>1E-4</v>
       </c>
       <c r="L63" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M63" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N63" s="11">
         <v>-4.9000000000000002E-2</v>
@@ -5069,43 +5190,43 @@
     </row>
     <row r="64" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="C64" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E64" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="C64" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E64" s="8" t="s">
+      <c r="F64" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="F64" s="8" t="s">
-        <v>363</v>
-      </c>
       <c r="G64" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I64" s="7">
         <v>-6.32</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K64" s="11">
         <v>1.18E-2</v>
       </c>
       <c r="L64" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N64" s="9">
         <v>0</v>
@@ -5113,25 +5234,25 @@
     </row>
     <row r="65" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="C65" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="C65" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E65" s="8" t="s">
+      <c r="F65" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="F65" s="7" t="s">
-        <v>369</v>
-      </c>
       <c r="G65" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H65" s="7">
         <v>7.69</v>
@@ -5140,16 +5261,16 @@
         <v>-3.44</v>
       </c>
       <c r="J65" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K65" s="11">
         <v>5.5500000000000001E-2</v>
       </c>
       <c r="L65" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M65" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N65" s="11">
         <v>-0.88419999999999999</v>
@@ -5157,43 +5278,43 @@
     </row>
     <row r="66" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="C66" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="C66" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E66" s="8" t="s">
+      <c r="F66" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="F66" s="8" t="s">
-        <v>375</v>
-      </c>
       <c r="G66" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I66" s="8">
         <v>81.900000000000006</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K66" s="13">
         <v>0.3634</v>
       </c>
       <c r="L66" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M66" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N66" s="11">
         <v>-9.0899999999999995E-2</v>
@@ -5286,13 +5407,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:P21"/>
+  <dimension ref="B1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5303,34 +5424,36 @@
     <col min="4" max="4" width="8.875" style="4"/>
     <col min="5" max="5" width="8.875" style="1"/>
     <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.875" style="1"/>
-    <col min="10" max="10" width="63.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.875" style="1"/>
-    <col min="14" max="14" width="10.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.875" style="1"/>
+    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="8.875" style="1"/>
+    <col min="11" max="11" width="63.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.875" style="1"/>
+    <col min="15" max="15" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="39" t="s">
-        <v>399</v>
-      </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="N1" s="1"/>
+      <c r="F1" s="42" t="s">
+        <v>398</v>
+      </c>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -5340,37 +5463,40 @@
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>388</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="27" t="s">
         <v>12</v>
       </c>
@@ -5381,37 +5507,41 @@
         <v>18</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F3" s="1">
         <f>[1]Main!$C$6</f>
         <v>1.2050000000000001</v>
       </c>
       <c r="G3" s="28">
+        <f>[1]Main!$C$7</f>
+        <v>4950</v>
+      </c>
+      <c r="H3" s="28">
         <f>[1]Main!$C$8</f>
         <v>5964.75</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <f>[1]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="I3" s="28">
+      <c r="J3" s="28">
         <f>[1]Main!$C$12</f>
         <v>5964.75</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="L3" s="4"/>
-      <c r="N3" s="4">
+      <c r="M3" s="4"/>
+      <c r="O3" s="4">
         <v>531</v>
       </c>
-      <c r="P3" s="4">
+      <c r="Q3" s="4">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="s">
         <v>11</v>
       </c>
@@ -5422,43 +5552,47 @@
         <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F4" s="1">
         <f>[2]Main!$C$6</f>
         <v>4.5199999999999996</v>
       </c>
       <c r="G4" s="28">
+        <f>[2]Main!$C$7</f>
+        <v>758</v>
+      </c>
+      <c r="H4" s="28">
         <f>[2]Main!$C$8</f>
         <v>3426.16</v>
       </c>
-      <c r="H4" s="29">
+      <c r="I4" s="29">
         <f>[2]Main!$C$11</f>
         <v>478</v>
       </c>
-      <c r="I4" s="28">
+      <c r="J4" s="28">
         <f>[2]Main!$C$12</f>
         <v>2948.16</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="K4" s="22">
+      <c r="K4" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="L4" s="22">
         <f>'[2]Financial Model'!$I$31</f>
         <v>2.4699599465954607E-2</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="N4" s="4">
+      <c r="M4" s="4"/>
+      <c r="O4" s="4">
         <v>310</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <v>106</v>
       </c>
-      <c r="P4" s="4">
+      <c r="Q4" s="4">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="27" t="s">
         <v>10</v>
       </c>
@@ -5469,44 +5603,48 @@
         <v>18</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F5" s="1">
         <f>[3]Main!$C$6</f>
         <v>23.2</v>
       </c>
       <c r="G5" s="28">
+        <f>[3]Main!$C$7</f>
+        <v>103.7</v>
+      </c>
+      <c r="H5" s="28">
         <f>[3]Main!$C$8</f>
         <v>2405.84</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <f>[3]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="I5" s="28">
+      <c r="J5" s="28">
         <f>[3]Main!$C$12</f>
         <v>2405.84</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="22">
+      <c r="L5" s="22">
         <f>'[3]Financial Model'!$L$25</f>
         <v>0.47730688307784791</v>
       </c>
-      <c r="L5" s="22"/>
       <c r="M5" s="22"/>
-      <c r="N5" s="4">
+      <c r="N5" s="22"/>
+      <c r="O5" s="4">
         <f>[3]Main!$D$21</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <f>[3]Main!$D$22</f>
         <v>153</v>
       </c>
-      <c r="O5" s="4">
-        <f>[3]Main!$D$22</f>
-        <v>315</v>
-      </c>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="27" t="s">
         <v>16</v>
       </c>
@@ -5517,67 +5655,72 @@
         <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F6" s="1">
         <f>[4]Main!$C$6</f>
         <v>10.029999999999999</v>
       </c>
       <c r="G6" s="28">
+        <f>[4]Main!$C$7</f>
+        <v>214.62</v>
+      </c>
+      <c r="H6" s="28">
         <f>[4]Main!$C$8</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="H6" s="29">
+      <c r="I6" s="29">
         <f>[4]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="I6" s="28">
+      <c r="J6" s="28">
         <f>[4]Main!$C$12</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="1" t="s">
+        <v>393</v>
+      </c>
       <c r="L6" s="4"/>
-      <c r="N6" s="4">
+      <c r="M6" s="4"/>
+      <c r="O6" s="4">
         <v>96</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <v>57</v>
       </c>
-      <c r="P6" s="4">
+      <c r="Q6" s="4">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" s="27"/>
       <c r="E7" s="4"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="29"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="29"/>
-      <c r="K7" s="4"/>
+      <c r="J7" s="29"/>
       <c r="L7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="M7" s="4"/>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -5587,176 +5730,198 @@
       <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="J9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="4"/>
+      <c r="H9" s="33"/>
+      <c r="K9" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="L9" s="4"/>
-      <c r="N9" s="4">
+      <c r="M9" s="4"/>
+      <c r="O9" s="4">
         <v>130</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="4">
         <v>44</v>
       </c>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="35">
         <v>753</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="H10" s="33"/>
+      <c r="K10" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="J10" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="M10" s="4"/>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>383</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>384</v>
       </c>
       <c r="F11" s="1">
         <v>40.14</v>
       </c>
-      <c r="G11" s="34">
-        <f>(F11*G19)*592.96</f>
+      <c r="H11" s="34">
+        <f>(F11*H19)*592.96</f>
         <v>19279.145664000003</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="K11" s="4"/>
+      <c r="K11" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F12" s="1">
         <v>76.38</v>
       </c>
-      <c r="G12" s="34">
-        <f>(F12*G19)*226.92</f>
+      <c r="H12" s="34">
+        <f>(F12*H19)*226.92</f>
         <v>14039.041176000001</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="K12" s="4"/>
+      <c r="K12" s="1" t="s">
+        <v>396</v>
+      </c>
       <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="31">
         <v>9201</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>390</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>391</v>
       </c>
       <c r="F13" s="32">
         <v>2357</v>
       </c>
-      <c r="G13" s="34">
-        <f>(F13*G21)*320.79</f>
+      <c r="G13" s="32"/>
+      <c r="H13" s="34">
+        <f>(F13*H21)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="K13" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F14" s="1">
         <v>9.5399999999999991</v>
       </c>
-      <c r="G14" s="34">
-        <f>(F14*G19)*320.79</f>
+      <c r="H14" s="34">
+        <f>(F14*H19)*320.79</f>
         <v>2478.8726459999998</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="1" t="s">
+        <v>395</v>
+      </c>
       <c r="L14" s="4"/>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F18" s="36" t="s">
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F18" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F19" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="G18" s="37"/>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F19" s="23" t="s">
+      <c r="G19" s="36"/>
+      <c r="H19" s="25">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F20" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="G19" s="25">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F20" s="23" t="s">
-        <v>381</v>
-      </c>
-      <c r="G20" s="25">
+      <c r="G20" s="36"/>
+      <c r="H20" s="25">
         <v>0.85</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F21" s="24" t="s">
-        <v>392</v>
-      </c>
-      <c r="G21" s="26">
+        <v>391</v>
+      </c>
+      <c r="G21" s="37"/>
+      <c r="H21" s="26">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B8:P8"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B8:Q8"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
@@ -5768,4 +5933,165 @@
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
   <legacyDrawing r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA0EDE9-69E3-4DB1-A599-3D030985D0D0}">
+  <dimension ref="B2:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="1"/>
+    <col min="7" max="7" width="41.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1"/>
+    <col min="10" max="10" width="13.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" style="1"/>
+    <col min="12" max="12" width="33.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2020</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4">
+        <v>5</v>
+      </c>
+      <c r="J3" s="4">
+        <v>16</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>415</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1984</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="H4" s="4">
+        <v>36</v>
+      </c>
+      <c r="I4" s="4">
+        <v>21</v>
+      </c>
+      <c r="J4" s="4">
+        <v>32</v>
+      </c>
+      <c r="K4" s="43" t="s">
+        <v>415</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1997</v>
+      </c>
+      <c r="H5" s="4">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="K5" s="43" t="s">
+        <v>415</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" display="Link" xr:uid="{705A33A3-71BB-4320-B698-2F78CD2A8AFC}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{02883213-BF38-4D93-A318-299B713A430A}"/>
+    <hyperlink ref="K5" r:id="rId3" location="Fleet" xr:uid="{31B6035D-A419-4044-A1AE-78B68CC43A46}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add $ALK to Airlines Overview sheet prep for model
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A37F56-55F3-4D0C-B0CF-8641C6509245}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D020FAFE-8C6A-0148-BFC8-27B1D352CADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
+    <workbookView xWindow="680" yWindow="500" windowWidth="32400" windowHeight="18900" activeTab="1" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
   <sheets>
     <sheet name="Industry Screening" sheetId="2" r:id="rId1"/>
@@ -27,6 +27,16 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -142,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
       <text>
         <r>
           <rPr>
@@ -155,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P9" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
+    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
       <text>
         <r>
           <rPr>
@@ -173,7 +183,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -181,7 +191,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -190,14 +200,14 @@
   <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
@@ -220,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="429">
   <si>
     <t>Ticker</t>
   </si>
@@ -1498,6 +1508,15 @@
   </si>
   <si>
     <t xml:space="preserve">Flybe 1979-2020 collapsed in March 2020, brand bought out by Cyrus Capital with a plan to relaunch </t>
+  </si>
+  <si>
+    <t>$ALK</t>
+  </si>
+  <si>
+    <t>Holding company (Alaska Air &amp; Horizon Air) + ground handler McGee Air Services</t>
+  </si>
+  <si>
+    <t>Alaska Air Group, Inc.</t>
   </si>
 </sst>
 </file>
@@ -1505,8 +1524,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;0&quot;#"/>
@@ -1736,7 +1755,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1760,7 +1779,7 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1776,12 +1795,6 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1795,16 +1808,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1822,7 +1832,16 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2403,17 +2422,17 @@
   </sheetPr>
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="20"/>
-    <col min="2" max="2" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="20"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
         <v>27</v>
@@ -2455,7 +2474,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
@@ -2499,7 +2518,7 @@
         <v>-1.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>48</v>
       </c>
@@ -2543,7 +2562,7 @@
         <v>-1.49E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>53</v>
       </c>
@@ -2587,7 +2606,7 @@
         <v>-9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>57</v>
       </c>
@@ -2631,7 +2650,7 @@
         <v>-3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>63</v>
       </c>
@@ -2675,7 +2694,7 @@
         <v>-2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>70</v>
       </c>
@@ -2719,7 +2738,7 @@
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>75</v>
       </c>
@@ -2763,7 +2782,7 @@
         <v>1.11E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>75</v>
       </c>
@@ -2807,7 +2826,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>82</v>
       </c>
@@ -2851,7 +2870,7 @@
         <v>2.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
         <v>753</v>
       </c>
@@ -2895,7 +2914,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>93</v>
       </c>
@@ -2939,7 +2958,7 @@
         <v>-2.93E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>93</v>
       </c>
@@ -2983,7 +3002,7 @@
         <v>-2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>103</v>
       </c>
@@ -3027,7 +3046,7 @@
         <v>-1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="19">
         <v>1055</v>
       </c>
@@ -3071,7 +3090,7 @@
         <v>-9.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>112</v>
       </c>
@@ -3115,7 +3134,7 @@
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="19">
         <v>670</v>
       </c>
@@ -3159,7 +3178,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>122</v>
       </c>
@@ -3203,7 +3222,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>127</v>
       </c>
@@ -3247,7 +3266,7 @@
         <v>-2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>132</v>
       </c>
@@ -3291,7 +3310,7 @@
         <v>-2.07E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>138</v>
       </c>
@@ -3335,7 +3354,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>145</v>
       </c>
@@ -3379,7 +3398,7 @@
         <v>-2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>138</v>
       </c>
@@ -3423,7 +3442,7 @@
         <v>-7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>12</v>
       </c>
@@ -3467,7 +3486,7 @@
         <v>-4.53E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>158</v>
       </c>
@@ -3511,7 +3530,7 @@
         <v>-2.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>162</v>
       </c>
@@ -3556,7 +3575,7 @@
         <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="19">
         <v>293</v>
       </c>
@@ -3600,7 +3619,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>173</v>
       </c>
@@ -3644,7 +3663,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>178</v>
       </c>
@@ -3688,7 +3707,7 @@
         <v>-3.04E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>184</v>
       </c>
@@ -3733,7 +3752,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>11</v>
       </c>
@@ -3777,7 +3796,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>10</v>
       </c>
@@ -3821,7 +3840,7 @@
         <v>-6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>196</v>
       </c>
@@ -3865,7 +3884,7 @@
         <v>7.5399999999999995E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>201</v>
       </c>
@@ -3909,7 +3928,7 @@
         <v>-9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>207</v>
       </c>
@@ -3953,7 +3972,7 @@
         <v>-1.61E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>211</v>
       </c>
@@ -3997,7 +4016,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>217</v>
       </c>
@@ -4041,7 +4060,7 @@
         <v>-4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>223</v>
       </c>
@@ -4085,7 +4104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
         <v>227</v>
       </c>
@@ -4129,7 +4148,7 @@
         <v>-1.8200000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
         <v>231</v>
       </c>
@@ -4173,7 +4192,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>231</v>
       </c>
@@ -4217,7 +4236,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
         <v>242</v>
       </c>
@@ -4261,7 +4280,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>248</v>
       </c>
@@ -4305,7 +4324,7 @@
         <v>-3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
         <v>254</v>
       </c>
@@ -4349,7 +4368,7 @@
         <v>-4.36E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
         <v>258</v>
       </c>
@@ -4393,7 +4412,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
         <v>264</v>
       </c>
@@ -4437,7 +4456,7 @@
         <v>-4.1200000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
         <v>269</v>
       </c>
@@ -4481,7 +4500,7 @@
         <v>-5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
         <v>275</v>
       </c>
@@ -4525,7 +4544,7 @@
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
         <v>278</v>
       </c>
@@ -4569,7 +4588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>283</v>
       </c>
@@ -4614,7 +4633,7 @@
         <v>-1.4E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
         <v>288</v>
       </c>
@@ -4659,7 +4678,7 @@
         <v>-3.3300000000000003E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
         <v>293</v>
       </c>
@@ -4703,7 +4722,7 @@
         <v>-5.5E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
         <v>299</v>
       </c>
@@ -4747,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
         <v>304</v>
       </c>
@@ -4791,7 +4810,7 @@
         <v>2.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
         <v>310</v>
       </c>
@@ -4835,7 +4854,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
         <v>316</v>
       </c>
@@ -4879,7 +4898,7 @@
         <v>-1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
         <v>316</v>
       </c>
@@ -4923,7 +4942,7 @@
         <v>-2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>326</v>
       </c>
@@ -4967,7 +4986,7 @@
         <v>-2.7799999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
         <v>332</v>
       </c>
@@ -5011,7 +5030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
         <v>337</v>
       </c>
@@ -5055,7 +5074,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
         <v>343</v>
       </c>
@@ -5099,7 +5118,7 @@
         <v>-3.7199999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
         <v>348</v>
       </c>
@@ -5144,7 +5163,7 @@
         <v>-4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
         <v>353</v>
       </c>
@@ -5188,7 +5207,7 @@
         <v>-4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="s">
         <v>359</v>
       </c>
@@ -5232,7 +5251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="s">
         <v>365</v>
       </c>
@@ -5276,7 +5295,7 @@
         <v>-0.88419999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
         <v>371</v>
       </c>
@@ -5407,46 +5426,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:Q21"/>
+  <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="1"/>
-    <col min="3" max="3" width="37.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="4"/>
-    <col min="5" max="5" width="8.875" style="1"/>
-    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
-    <col min="8" max="10" width="8.875" style="1"/>
-    <col min="11" max="11" width="63.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.875" style="1"/>
-    <col min="15" max="15" width="10.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="4"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
+    <col min="8" max="10" width="8.83203125" style="1"/>
+    <col min="11" max="11" width="65.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.83203125" style="1"/>
+    <col min="15" max="15" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.875" style="1"/>
+    <col min="18" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="39" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5496,8 +5515,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B3" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -5513,11 +5532,11 @@
         <f>[1]Main!$C$6</f>
         <v>1.2050000000000001</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="26">
         <f>[1]Main!$C$7</f>
         <v>4950</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="26">
         <f>[1]Main!$C$8</f>
         <v>5964.75</v>
       </c>
@@ -5525,7 +5544,7 @@
         <f>[1]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="26">
         <f>[1]Main!$C$12</f>
         <v>5964.75</v>
       </c>
@@ -5541,8 +5560,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="27" t="s">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B4" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -5558,19 +5577,19 @@
         <f>[2]Main!$C$6</f>
         <v>4.5199999999999996</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="26">
         <f>[2]Main!$C$7</f>
         <v>758</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="26">
         <f>[2]Main!$C$8</f>
         <v>3426.16</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="27">
         <f>[2]Main!$C$11</f>
         <v>478</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="26">
         <f>[2]Main!$C$12</f>
         <v>2948.16</v>
       </c>
@@ -5592,8 +5611,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B5" s="25" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -5609,11 +5628,11 @@
         <f>[3]Main!$C$6</f>
         <v>23.2</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="26">
         <f>[3]Main!$C$7</f>
         <v>103.7</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="26">
         <f>[3]Main!$C$8</f>
         <v>2405.84</v>
       </c>
@@ -5621,7 +5640,7 @@
         <f>[3]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="26">
         <f>[3]Main!$C$12</f>
         <v>2405.84</v>
       </c>
@@ -5644,8 +5663,8 @@
       </c>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="27" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B6" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -5661,19 +5680,19 @@
         <f>[4]Main!$C$6</f>
         <v>10.029999999999999</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="26">
         <f>[4]Main!$C$7</f>
         <v>214.62</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="26">
         <f>[4]Main!$C$8</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="27">
         <f>[4]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="26">
         <f>[4]Main!$C$12</f>
         <v>2152.6385999999998</v>
       </c>
@@ -5692,236 +5711,263 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="27"/>
-      <c r="E7" s="4"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B7" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="1" t="s">
+        <v>427</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B8" s="25"/>
+      <c r="E8" s="4"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="K9" s="1" t="s">
+      <c r="H10" s="31"/>
+      <c r="K10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="O9" s="4">
-        <v>130</v>
-      </c>
-      <c r="P9" s="4">
-        <v>44</v>
-      </c>
-      <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="35">
-        <v>753</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="H10" s="33"/>
-      <c r="K10" s="1" t="s">
-        <v>400</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
+      <c r="O10" s="4">
+        <v>130</v>
+      </c>
+      <c r="P10" s="4">
+        <v>44</v>
+      </c>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>382</v>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B11" s="33">
+        <v>753</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F11" s="1">
-        <v>40.14</v>
-      </c>
-      <c r="H11" s="34">
-        <f>(F11*H19)*592.96</f>
-        <v>19279.145664000003</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="H11" s="31"/>
       <c r="K11" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="Q11" s="4"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>383</v>
       </c>
       <c r="F12" s="1">
-        <v>76.38</v>
-      </c>
-      <c r="H12" s="34">
-        <f>(F12*H19)*226.92</f>
-        <v>14039.041176000001</v>
+        <v>40.14</v>
+      </c>
+      <c r="H12" s="32">
+        <f>(F12*H20)*592.96</f>
+        <v>19279.145664000003</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B13" s="31">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B13" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F13" s="1">
+        <v>76.38</v>
+      </c>
+      <c r="H13" s="32">
+        <f>(F13*H20)*226.92</f>
+        <v>14039.041176000001</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B14" s="29">
         <v>9201</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F14" s="30">
         <v>2357</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="34">
-        <f>(F13*H21)*320.79</f>
+      <c r="G14" s="30"/>
+      <c r="H14" s="32">
+        <f>(F14*H22)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B15" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F14" s="1">
-        <v>9.5399999999999991</v>
-      </c>
-      <c r="H14" s="34">
-        <f>(F14*H19)*320.79</f>
-        <v>2478.8726459999998</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>383</v>
       </c>
+      <c r="F15" s="1">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="H15" s="32">
+        <f>(F15*H20)*320.79</f>
+        <v>2478.8726459999998</v>
+      </c>
       <c r="K15" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="B16" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F18" s="38" t="s">
+    <row r="19" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="F19" s="35" t="s">
         <v>378</v>
       </c>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40"/>
-    </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F19" s="23" t="s">
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="F20" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="25">
+      <c r="G20" s="41"/>
+      <c r="H20" s="23">
         <v>0.81</v>
       </c>
     </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F20" s="23" t="s">
+    <row r="21" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="F21" s="40" t="s">
         <v>380</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="25">
+      <c r="G21" s="41"/>
+      <c r="H21" s="23">
         <v>0.85</v>
       </c>
     </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F21" s="24" t="s">
+    <row r="22" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="F22" s="42" t="s">
         <v>391</v>
       </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="26">
+      <c r="G22" s="43"/>
+      <c r="H22" s="24">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="B8:Q8"/>
+  <mergeCells count="6">
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="B9:Q9"/>
     <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
@@ -5939,31 +5985,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA0EDE9-69E3-4DB1-A599-3D030985D0D0}">
   <dimension ref="B2:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1"/>
-    <col min="7" max="7" width="41.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1"/>
-    <col min="10" max="10" width="13.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="1"/>
-    <col min="12" max="12" width="33.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>404</v>
       </c>
@@ -5998,7 +6044,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>408</v>
       </c>
@@ -6020,14 +6066,14 @@
       <c r="J3" s="4">
         <v>16</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="34" t="s">
         <v>415</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>413</v>
       </c>
@@ -6052,14 +6098,14 @@
       <c r="J4" s="4">
         <v>32</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="34" t="s">
         <v>415</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>421</v>
       </c>
@@ -6081,7 +6127,7 @@
       <c r="J5" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="34" t="s">
         <v>415</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start $ALK model, update Airlines Overview doc with $ALK key data
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D020FAFE-8C6A-0148-BFC8-27B1D352CADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61557CE-1FAC-4504-9D2C-6C6CE942ED5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="32400" windowHeight="18900" activeTab="1" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
+    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="1" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
   <sheets>
     <sheet name="Industry Screening" sheetId="2" r:id="rId1"/>
@@ -22,21 +22,12 @@
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -61,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
+    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
       <text>
         <r>
           <rPr>
@@ -74,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
       <text>
         <r>
           <rPr>
@@ -87,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
       <text>
         <r>
           <rPr>
@@ -100,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
+    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
       <text>
         <r>
           <rPr>
@@ -113,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
       <text>
         <r>
           <rPr>
@@ -126,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
+    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
       <text>
         <r>
           <rPr>
@@ -139,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
       <text>
         <r>
           <rPr>
@@ -183,7 +174,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -191,7 +182,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -200,14 +191,14 @@
   <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
@@ -230,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="432">
   <si>
     <t>Ticker</t>
   </si>
@@ -1517,18 +1508,28 @@
   </si>
   <si>
     <t>Alaska Air Group, Inc.</t>
+  </si>
+  <si>
+    <t>P/B</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;0&quot;#"/>
+    <numFmt numFmtId="168" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1755,9 +1756,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1779,7 +1780,7 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1808,13 +1809,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1838,10 +1845,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1949,7 +1956,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1989,9 +1996,6 @@
           <cell r="C12">
             <v>2405.84</v>
           </cell>
-        </row>
-        <row r="21">
-          <cell r="D21"/>
         </row>
         <row r="22">
           <cell r="D22">
@@ -2050,6 +2054,66 @@
       </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>41.83</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>126.5</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>5291.4949999999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>1122</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>4169.4949999999999</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>Q222</v>
+          </cell>
+          <cell r="D30">
+            <v>44378</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>1.3933386917609896</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="41">
+          <cell r="V41">
+            <v>0.73137697516930023</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2426,13 +2490,13 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="20"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="20"/>
+    <col min="2" max="2" width="42.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
         <v>27</v>
@@ -2474,7 +2538,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
@@ -2518,7 +2582,7 @@
         <v>-1.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>48</v>
       </c>
@@ -2562,7 +2626,7 @@
         <v>-1.49E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>53</v>
       </c>
@@ -2606,7 +2670,7 @@
         <v>-9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>57</v>
       </c>
@@ -2650,7 +2714,7 @@
         <v>-3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>63</v>
       </c>
@@ -2694,7 +2758,7 @@
         <v>-2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>70</v>
       </c>
@@ -2738,7 +2802,7 @@
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>75</v>
       </c>
@@ -2782,7 +2846,7 @@
         <v>1.11E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>75</v>
       </c>
@@ -2826,7 +2890,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>82</v>
       </c>
@@ -2870,7 +2934,7 @@
         <v>2.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>753</v>
       </c>
@@ -2914,7 +2978,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>93</v>
       </c>
@@ -2958,7 +3022,7 @@
         <v>-2.93E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>93</v>
       </c>
@@ -3002,7 +3066,7 @@
         <v>-2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>103</v>
       </c>
@@ -3046,7 +3110,7 @@
         <v>-1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>1055</v>
       </c>
@@ -3090,7 +3154,7 @@
         <v>-9.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>112</v>
       </c>
@@ -3134,7 +3198,7 @@
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>670</v>
       </c>
@@ -3178,7 +3242,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>122</v>
       </c>
@@ -3222,7 +3286,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>127</v>
       </c>
@@ -3266,7 +3330,7 @@
         <v>-2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>132</v>
       </c>
@@ -3310,7 +3374,7 @@
         <v>-2.07E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>138</v>
       </c>
@@ -3354,7 +3418,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>145</v>
       </c>
@@ -3398,7 +3462,7 @@
         <v>-2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>138</v>
       </c>
@@ -3442,7 +3506,7 @@
         <v>-7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>12</v>
       </c>
@@ -3486,7 +3550,7 @@
         <v>-4.53E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>158</v>
       </c>
@@ -3530,7 +3594,7 @@
         <v>-2.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>162</v>
       </c>
@@ -3575,7 +3639,7 @@
         <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>293</v>
       </c>
@@ -3619,7 +3683,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>173</v>
       </c>
@@ -3663,7 +3727,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>178</v>
       </c>
@@ -3707,7 +3771,7 @@
         <v>-3.04E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>184</v>
       </c>
@@ -3752,7 +3816,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>11</v>
       </c>
@@ -3796,7 +3860,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>10</v>
       </c>
@@ -3840,7 +3904,7 @@
         <v>-6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>196</v>
       </c>
@@ -3884,7 +3948,7 @@
         <v>7.5399999999999995E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>201</v>
       </c>
@@ -3928,7 +3992,7 @@
         <v>-9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>207</v>
       </c>
@@ -3972,7 +4036,7 @@
         <v>-1.61E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>211</v>
       </c>
@@ -4016,7 +4080,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>217</v>
       </c>
@@ -4060,7 +4124,7 @@
         <v>-4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>223</v>
       </c>
@@ -4104,7 +4168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>227</v>
       </c>
@@ -4148,7 +4212,7 @@
         <v>-1.8200000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>231</v>
       </c>
@@ -4192,7 +4256,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>231</v>
       </c>
@@ -4236,7 +4300,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>242</v>
       </c>
@@ -4280,7 +4344,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>248</v>
       </c>
@@ -4324,7 +4388,7 @@
         <v>-3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>254</v>
       </c>
@@ -4368,7 +4432,7 @@
         <v>-4.36E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>258</v>
       </c>
@@ -4412,7 +4476,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>264</v>
       </c>
@@ -4456,7 +4520,7 @@
         <v>-4.1200000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>269</v>
       </c>
@@ -4500,7 +4564,7 @@
         <v>-5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>275</v>
       </c>
@@ -4544,7 +4608,7 @@
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>278</v>
       </c>
@@ -4588,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>283</v>
       </c>
@@ -4633,7 +4697,7 @@
         <v>-1.4E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>288</v>
       </c>
@@ -4678,7 +4742,7 @@
         <v>-3.3300000000000003E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>293</v>
       </c>
@@ -4722,7 +4786,7 @@
         <v>-5.5E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>299</v>
       </c>
@@ -4766,7 +4830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>304</v>
       </c>
@@ -4810,7 +4874,7 @@
         <v>2.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>310</v>
       </c>
@@ -4854,7 +4918,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>316</v>
       </c>
@@ -4898,7 +4962,7 @@
         <v>-1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>316</v>
       </c>
@@ -4942,7 +5006,7 @@
         <v>-2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>326</v>
       </c>
@@ -4986,7 +5050,7 @@
         <v>-2.7799999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>332</v>
       </c>
@@ -5030,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>337</v>
       </c>
@@ -5074,7 +5138,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>343</v>
       </c>
@@ -5118,7 +5182,7 @@
         <v>-3.7199999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>348</v>
       </c>
@@ -5163,7 +5227,7 @@
         <v>-4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
         <v>353</v>
       </c>
@@ -5207,7 +5271,7 @@
         <v>-4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>359</v>
       </c>
@@ -5251,7 +5315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>365</v>
       </c>
@@ -5295,7 +5359,7 @@
         <v>-0.88419999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>371</v>
       </c>
@@ -5426,46 +5490,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:Q22"/>
+  <dimension ref="B1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="4"/>
-    <col min="5" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="8.83203125" style="1"/>
-    <col min="11" max="11" width="65.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.83203125" style="1"/>
-    <col min="15" max="15" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="1"/>
+    <col min="3" max="3" width="37.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="4"/>
+    <col min="5" max="5" width="8.875" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="8.875" style="1"/>
+    <col min="11" max="11" width="65.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.875" style="1"/>
+    <col min="15" max="15" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.375" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.83203125" style="1"/>
+    <col min="18" max="20" width="8.875" style="1"/>
+    <col min="21" max="22" width="8.875" style="4"/>
+    <col min="23" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="41" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5514,8 +5580,17 @@
       <c r="Q2" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S2" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>12</v>
       </c>
@@ -5559,183 +5634,218 @@
       <c r="Q3" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F4" s="26">
+        <f>[5]Main!$C$6*H20</f>
+        <v>37.646999999999998</v>
+      </c>
+      <c r="G4" s="26">
+        <f>[5]Main!$C$7</f>
+        <v>126.5</v>
+      </c>
+      <c r="H4" s="26">
+        <f>[5]Main!$C$8*H20</f>
+        <v>4762.3455000000004</v>
+      </c>
+      <c r="I4" s="27">
+        <f>[5]Main!$C$11*H20</f>
+        <v>1009.8000000000001</v>
+      </c>
+      <c r="J4" s="26">
+        <f>[5]Main!$C$12*H20</f>
+        <v>3752.5455000000002</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="L4" s="22">
+        <f>'[5]Financial Model'!$V$41</f>
+        <v>0.73137697516930023</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="S4" s="44">
+        <f>[5]Main!$C$35</f>
+        <v>1.3933386917609896</v>
+      </c>
+      <c r="U4" s="4" t="str">
+        <f>[5]Main!$C$30</f>
+        <v>Q222</v>
+      </c>
+      <c r="V4" s="45">
+        <f>[5]Main!$D$30</f>
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F5" s="1">
         <f>[2]Main!$C$6</f>
         <v>4.5199999999999996</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G5" s="26">
         <f>[2]Main!$C$7</f>
         <v>758</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H5" s="26">
         <f>[2]Main!$C$8</f>
         <v>3426.16</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I5" s="26">
         <f>[2]Main!$C$11</f>
         <v>478</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J5" s="26">
         <f>[2]Main!$C$12</f>
         <v>2948.16</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L5" s="22">
         <f>'[2]Financial Model'!$I$31</f>
         <v>2.4699599465954607E-2</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="O4" s="4">
+      <c r="M5" s="4"/>
+      <c r="O5" s="4">
         <v>310</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P5" s="4">
         <v>106</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q5" s="4">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B5" s="25" t="s">
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F6" s="1">
         <f>[3]Main!$C$6</f>
         <v>23.2</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G6" s="26">
         <f>[3]Main!$C$7</f>
         <v>103.7</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H6" s="26">
         <f>[3]Main!$C$8</f>
         <v>2405.84</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I6" s="1">
         <f>[3]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J6" s="26">
         <f>[3]Main!$C$12</f>
         <v>2405.84</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L6" s="22">
         <f>'[3]Financial Model'!$L$25</f>
         <v>0.47730688307784791</v>
       </c>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="4">
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="4">
         <f>[3]Main!$D$21</f>
         <v>0</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P6" s="4">
         <f>[3]Main!$D$22</f>
         <v>153</v>
       </c>
-      <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B6" s="25" t="s">
+      <c r="Q6" s="4"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <f>[4]Main!$C$6</f>
         <v>10.029999999999999</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G7" s="26">
         <f>[4]Main!$C$7</f>
         <v>214.62</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H7" s="26">
         <f>[4]Main!$C$8</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I7" s="27">
         <f>[4]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J7" s="26">
         <f>[4]Main!$C$12</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="O6" s="4">
-        <v>96</v>
-      </c>
-      <c r="P6" s="4">
-        <v>57</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B7" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="1" t="s">
-        <v>427</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="O7" s="4">
+        <v>96</v>
+      </c>
+      <c r="P7" s="4">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>82</v>
+      </c>
+      <c r="S7" s="4"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B8" s="25"/>
       <c r="E8" s="4"/>
       <c r="H8" s="28"/>
@@ -5744,26 +5854,28 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S8" s="4"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="S9" s="4"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
@@ -5786,8 +5898,9 @@
         <v>44</v>
       </c>
       <c r="Q10" s="4"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S10" s="4"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="33">
         <v>753</v>
       </c>
@@ -5804,8 +5917,9 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="Q11" s="4"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S11" s="4"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>382</v>
       </c>
@@ -5823,15 +5937,16 @@
       </c>
       <c r="H12" s="32">
         <f>(F12*H20)*592.96</f>
-        <v>19279.145664000003</v>
+        <v>21421.272960000006</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>397</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>384</v>
       </c>
@@ -5849,15 +5964,16 @@
       </c>
       <c r="H13" s="32">
         <f>(F13*H20)*226.92</f>
-        <v>14039.041176000001</v>
+        <v>15598.934639999999</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>396</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S13" s="4"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="29">
         <v>9201</v>
       </c>
@@ -5882,8 +5998,9 @@
         <v>392</v>
       </c>
       <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S14" s="4"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>385</v>
       </c>
@@ -5901,15 +6018,16 @@
       </c>
       <c r="H15" s="32">
         <f>(F15*H20)*320.79</f>
-        <v>2478.8726459999998</v>
+        <v>2754.3029400000005</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>395</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.15">
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>401</v>
       </c>
@@ -5925,40 +6043,49 @@
       <c r="K16" s="1" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F19" s="35" t="s">
+      <c r="S16" s="4"/>
+    </row>
+    <row r="19" spans="6:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="37" t="s">
         <v>378</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F20" s="40" t="s">
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+    </row>
+    <row r="20" spans="6:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="42" t="s">
         <v>379</v>
       </c>
-      <c r="G20" s="41"/>
+      <c r="G20" s="43"/>
       <c r="H20" s="23">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F21" s="40" t="s">
+        <v>0.9</v>
+      </c>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+    </row>
+    <row r="21" spans="6:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="42" t="s">
         <v>380</v>
       </c>
-      <c r="G21" s="41"/>
+      <c r="G21" s="43"/>
       <c r="H21" s="23">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F22" s="42" t="s">
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+    </row>
+    <row r="22" spans="6:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="35" t="s">
         <v>391</v>
       </c>
-      <c r="G22" s="43"/>
+      <c r="G22" s="36"/>
       <c r="H22" s="24">
         <v>6.0000000000000001E-3</v>
       </c>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5970,14 +6097,15 @@
     <mergeCell ref="F21:G21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{176C962A-9F96-4539-8149-82E34F7BBB40}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{56F8AAB4-AB88-4816-A70A-66823F4EBD86}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{176C962A-9F96-4539-8149-82E34F7BBB40}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{56F8AAB4-AB88-4816-A70A-66823F4EBD86}"/>
     <hyperlink ref="B3" r:id="rId4" xr:uid="{593208B0-BF4C-4E7C-9DA3-9FABEC41EED7}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{5BD026C6-209C-4F8D-96F9-0D20474E4F7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -5992,24 +6120,24 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1"/>
-    <col min="7" max="7" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1"/>
-    <col min="10" max="10" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="1"/>
-    <col min="12" max="12" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>404</v>
       </c>
@@ -6044,7 +6172,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>408</v>
       </c>
@@ -6073,7 +6201,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>413</v>
       </c>
@@ -6105,7 +6233,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>421</v>
       </c>

</xml_diff>

<commit_message>
Add $INDIGO model & update Airlines Overview
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDE3ED2-8D00-4398-8F12-4AB5AF07E5A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED7857D-A344-4D10-8181-89325D96D703}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="1" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
     <author>Charlie George</author>
   </authors>
   <commentList>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
+    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
       <text>
         <r>
           <rPr>
@@ -65,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
       <text>
         <r>
           <rPr>
@@ -78,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
+    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
       <text>
         <r>
           <rPr>
@@ -91,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
+    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
       <text>
         <r>
           <rPr>
@@ -104,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
       <text>
         <r>
           <rPr>
@@ -117,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
       <text>
         <r>
           <rPr>
@@ -130,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
+    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
       <text>
         <r>
           <rPr>
@@ -143,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
+    <comment ref="O11" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
       <text>
         <r>
           <rPr>
@@ -156,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
+    <comment ref="P11" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
       <text>
         <r>
           <rPr>
@@ -221,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="437">
   <si>
     <t>Ticker</t>
   </si>
@@ -1517,6 +1518,21 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>InterGlobe Aviation Ltd.</t>
+  </si>
+  <si>
+    <t>Low-cost Indian airline &amp; largest Airline in India by passenger numbers</t>
+  </si>
+  <si>
+    <t>$INDIGO</t>
+  </si>
+  <si>
+    <t>₹</t>
+  </si>
+  <si>
+    <t>INRGBP</t>
   </si>
 </sst>
 </file>
@@ -2122,6 +2138,45 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>1779.1</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>385.26</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>685416.06599999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>685416.06599999999</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <global>
@@ -2489,8 +2544,8 @@
   </sheetPr>
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="A23:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5493,13 +5548,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:V22"/>
+  <dimension ref="B1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5595,520 +5650,576 @@
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="F3" s="28">
+        <f>[6]Main!$C$6*H24</f>
+        <v>19.570099999999996</v>
+      </c>
+      <c r="G3" s="26">
+        <f>[6]Main!$C$7</f>
+        <v>385.26</v>
+      </c>
+      <c r="H3" s="26">
+        <f>[6]Main!$C$8*H24</f>
+        <v>7539.5767259999993</v>
+      </c>
+      <c r="I3" s="27">
+        <f>[6]Main!$C$11*H24</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="26">
+        <f>[6]Main!$C$12*H24</f>
+        <v>7539.5767259999993</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F4" s="1">
         <f>[1]Main!$C$6</f>
         <v>1.2050000000000001</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G4" s="26">
         <f>[1]Main!$C$7</f>
         <v>4950</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H4" s="26">
         <f>[1]Main!$C$8</f>
         <v>5964.75</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I4" s="1">
         <f>[1]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J4" s="26">
         <f>[1]Main!$C$12</f>
         <v>5964.75</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="O3" s="4">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="O4" s="4">
         <v>531</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q4" s="4">
         <v>200</v>
       </c>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B5" s="25" t="s">
         <v>426</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="F4" s="26">
-        <f>[2]Main!$C$6*H20</f>
+      <c r="F5" s="26">
+        <f>[2]Main!$C$6*H21</f>
         <v>37.646999999999998</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G5" s="26">
         <f>[2]Main!$C$7</f>
         <v>126.5</v>
       </c>
-      <c r="H4" s="26">
-        <f>[2]Main!$C$8*H20</f>
+      <c r="H5" s="26">
+        <f>[2]Main!$C$8*H21</f>
         <v>4762.3455000000004</v>
       </c>
-      <c r="I4" s="27">
-        <f>[2]Main!$C$11*H20</f>
+      <c r="I5" s="27">
+        <f>[2]Main!$C$11*H21</f>
         <v>1009.8000000000001</v>
       </c>
-      <c r="J4" s="26">
-        <f>[2]Main!$C$12*H20</f>
+      <c r="J5" s="26">
+        <f>[2]Main!$C$12*H21</f>
         <v>3752.5455000000002</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L5" s="22">
         <f>'[2]Financial Model'!$V$42</f>
         <v>0.26862302483069977</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="S4" s="35">
+      <c r="M5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="S5" s="35">
         <f>[2]Main!$C$35</f>
         <v>1.3933386917609896</v>
       </c>
-      <c r="U4" s="4" t="str">
+      <c r="U5" s="4" t="str">
         <f>[2]Main!$C$30</f>
         <v>Q222</v>
       </c>
-      <c r="V4" s="36">
+      <c r="V5" s="36">
         <f>[2]Main!$D$30</f>
         <v>44378</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F6" s="1">
         <f>[3]Main!$C$6</f>
         <v>4.5199999999999996</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G6" s="26">
         <f>[3]Main!$C$7</f>
         <v>758</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H6" s="26">
         <f>[3]Main!$C$8</f>
         <v>3426.16</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I6" s="26">
         <f>[3]Main!$C$11</f>
         <v>478</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J6" s="26">
         <f>[3]Main!$C$12</f>
         <v>2948.16</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L6" s="22">
         <f>'[3]Financial Model'!$I$31</f>
         <v>2.4699599465954607E-2</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="O5" s="4">
+      <c r="M6" s="4"/>
+      <c r="O6" s="4">
         <v>310</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P6" s="4">
         <v>106</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q6" s="4">
         <v>136</v>
       </c>
-      <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B6" s="25" t="s">
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <f>[4]Main!$C$6</f>
         <v>23.2</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G7" s="26">
         <f>[4]Main!$C$7</f>
         <v>103.7</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H7" s="26">
         <f>[4]Main!$C$8</f>
         <v>2405.84</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I7" s="1">
         <f>[4]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J7" s="26">
         <f>[4]Main!$C$12</f>
         <v>2405.84</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L7" s="22">
         <f>'[4]Financial Model'!$L$25</f>
         <v>0.47730688307784791</v>
       </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="4">
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="4">
         <f>[4]Main!$D$21</f>
         <v>0</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P7" s="4">
         <f>[4]Main!$D$22</f>
         <v>153</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B7" s="25" t="s">
+      <c r="Q7" s="4"/>
+      <c r="S7" s="4"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B8" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <f>[5]Main!$C$6</f>
         <v>10.029999999999999</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G8" s="26">
         <f>[5]Main!$C$7</f>
         <v>214.62</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H8" s="26">
         <f>[5]Main!$C$8</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I8" s="27">
         <f>[5]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J8" s="26">
         <f>[5]Main!$C$12</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="O7" s="4">
-        <v>96</v>
-      </c>
-      <c r="P7" s="4">
-        <v>57</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>82</v>
-      </c>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B8" s="25"/>
-      <c r="E8" s="4"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="Q8" s="4"/>
+      <c r="O8" s="4">
+        <v>96</v>
+      </c>
+      <c r="P8" s="4">
+        <v>57</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>82</v>
+      </c>
       <c r="S8" s="4"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
+      <c r="B9" s="25"/>
+      <c r="E9" s="4"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="Q9" s="4"/>
       <c r="S9" s="4"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="S10" s="4"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="H10" s="31"/>
-      <c r="K10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="O10" s="4">
-        <v>130</v>
-      </c>
-      <c r="P10" s="4">
-        <v>44</v>
-      </c>
-      <c r="Q10" s="4"/>
-      <c r="S10" s="4"/>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B11" s="33">
-        <v>753</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>399</v>
       </c>
       <c r="H11" s="31"/>
       <c r="K11" s="1" t="s">
-        <v>400</v>
+        <v>24</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
+      <c r="O11" s="4">
+        <v>130</v>
+      </c>
+      <c r="P11" s="4">
+        <v>44</v>
+      </c>
       <c r="Q11" s="4"/>
       <c r="S11" s="4"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>382</v>
+      <c r="B12" s="33">
+        <v>753</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F12" s="1">
-        <v>40.14</v>
-      </c>
-      <c r="H12" s="32">
-        <f>(F12*H20)*592.96</f>
-        <v>21421.272960000006</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="H12" s="31"/>
       <c r="K12" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
+      <c r="Q12" s="4"/>
       <c r="S12" s="4"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>383</v>
       </c>
       <c r="F13" s="1">
-        <v>76.38</v>
+        <v>40.14</v>
       </c>
       <c r="H13" s="32">
-        <f>(F13*H20)*226.92</f>
-        <v>15598.934639999999</v>
+        <f>(F13*H21)*592.96</f>
+        <v>21421.272960000006</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="S13" s="4"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B14" s="29">
+      <c r="B14" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F14" s="1">
+        <v>76.38</v>
+      </c>
+      <c r="H14" s="32">
+        <f>(F14*H21)*226.92</f>
+        <v>15598.934639999999</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="S14" s="4"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B15" s="29">
         <v>9201</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F15" s="30">
         <v>2357</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="32">
-        <f>(F14*H22)*320.79</f>
+      <c r="G15" s="30"/>
+      <c r="H15" s="32">
+        <f>(F15*H23)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F15" s="1">
-        <v>9.5399999999999991</v>
-      </c>
-      <c r="H15" s="32">
-        <f>(F15*H20)*320.79</f>
-        <v>2754.3029400000005</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>395</v>
-      </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
       <c r="S15" s="4"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>197</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>383</v>
       </c>
+      <c r="F16" s="1">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="H16" s="32">
+        <f>(F16*H21)*320.79</f>
+        <v>2754.3029400000005</v>
+      </c>
       <c r="K16" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="S16" s="4"/>
-    </row>
-    <row r="19" spans="6:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F19" s="39" t="s">
+      <c r="S17" s="4"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D20" s="1"/>
+      <c r="F20" s="39" t="s">
         <v>378</v>
       </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-    </row>
-    <row r="20" spans="6:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="44" t="s">
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D21" s="1"/>
+      <c r="F21" s="44" t="s">
         <v>379</v>
-      </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="23">
-        <v>0.9</v>
-      </c>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-    </row>
-    <row r="21" spans="6:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="44" t="s">
-        <v>380</v>
       </c>
       <c r="G21" s="45"/>
       <c r="H21" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D22" s="1"/>
+      <c r="F22" s="44" t="s">
+        <v>380</v>
+      </c>
+      <c r="G22" s="45"/>
+      <c r="H22" s="23">
         <v>0.85</v>
       </c>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-    </row>
-    <row r="22" spans="6:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F22" s="37" t="s">
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D23" s="1"/>
+      <c r="F23" s="44" t="s">
         <v>391</v>
       </c>
-      <c r="G22" s="38"/>
-      <c r="H22" s="24">
+      <c r="G23" s="45"/>
+      <c r="H23" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="F24" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="G24" s="38"/>
+      <c r="H24" s="24">
+        <v>1.0999999999999999E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="B9:Q9"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{176C962A-9F96-4539-8149-82E34F7BBB40}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{56F8AAB4-AB88-4816-A70A-66823F4EBD86}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{593208B0-BF4C-4E7C-9DA3-9FABEC41EED7}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{5BD026C6-209C-4F8D-96F9-0D20474E4F7F}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{176C962A-9F96-4539-8149-82E34F7BBB40}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{56F8AAB4-AB88-4816-A70A-66823F4EBD86}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{593208B0-BF4C-4E7C-9DA3-9FABEC41EED7}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{5BD026C6-209C-4F8D-96F9-0D20474E4F7F}"/>
+    <hyperlink ref="B3" r:id="rId6" xr:uid="{28605697-2E3F-4D0E-BA6A-013F294DB301}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Minor update to airlines
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED7857D-A344-4D10-8181-89325D96D703}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42418073-9C06-4020-86D2-F87326E44985}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="1" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
@@ -1846,6 +1846,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1859,12 +1865,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1887,6 +1887,45 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>1779.1</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>385.26</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>685416.06599999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>685416.06599999999</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1929,7 +1968,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1992,7 +2031,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2041,7 +2080,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2095,7 +2134,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2133,45 +2172,6 @@
       </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>1779.1</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>385.26</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>685416.06599999999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>685416.06599999999</v>
-          </cell>
-        </row>
-      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5554,7 +5554,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5579,13 +5579,13 @@
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="45" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
@@ -5662,23 +5662,23 @@
         <v>435</v>
       </c>
       <c r="F3" s="28">
-        <f>[6]Main!$C$6*H24</f>
+        <f>[1]Main!$C$6*H24</f>
         <v>19.570099999999996</v>
       </c>
       <c r="G3" s="26">
-        <f>[6]Main!$C$7</f>
+        <f>[1]Main!$C$7</f>
         <v>385.26</v>
       </c>
       <c r="H3" s="26">
-        <f>[6]Main!$C$8*H24</f>
+        <f>[1]Main!$C$8*H24</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="I3" s="27">
-        <f>[6]Main!$C$11*H24</f>
+        <f>[1]Main!$C$11*H24</f>
         <v>0</v>
       </c>
       <c r="J3" s="26">
-        <f>[6]Main!$C$12*H24</f>
+        <f>[1]Main!$C$12*H24</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -5703,23 +5703,23 @@
         <v>377</v>
       </c>
       <c r="F4" s="1">
-        <f>[1]Main!$C$6</f>
+        <f>[2]Main!$C$6</f>
         <v>1.2050000000000001</v>
       </c>
       <c r="G4" s="26">
-        <f>[1]Main!$C$7</f>
+        <f>[2]Main!$C$7</f>
         <v>4950</v>
       </c>
       <c r="H4" s="26">
-        <f>[1]Main!$C$8</f>
+        <f>[2]Main!$C$8</f>
         <v>5964.75</v>
       </c>
       <c r="I4" s="1">
-        <f>[1]Main!$C$11</f>
+        <f>[2]Main!$C$11</f>
         <v>0</v>
       </c>
       <c r="J4" s="26">
-        <f>[1]Main!$C$12</f>
+        <f>[2]Main!$C$12</f>
         <v>5964.75</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -5749,44 +5749,44 @@
         <v>383</v>
       </c>
       <c r="F5" s="26">
-        <f>[2]Main!$C$6*H21</f>
+        <f>[3]Main!$C$6*H21</f>
         <v>37.646999999999998</v>
       </c>
       <c r="G5" s="26">
-        <f>[2]Main!$C$7</f>
+        <f>[3]Main!$C$7</f>
         <v>126.5</v>
       </c>
       <c r="H5" s="26">
-        <f>[2]Main!$C$8*H21</f>
+        <f>[3]Main!$C$8*H21</f>
         <v>4762.3455000000004</v>
       </c>
       <c r="I5" s="27">
-        <f>[2]Main!$C$11*H21</f>
+        <f>[3]Main!$C$11*H21</f>
         <v>1009.8000000000001</v>
       </c>
       <c r="J5" s="26">
-        <f>[2]Main!$C$12*H21</f>
+        <f>[3]Main!$C$12*H21</f>
         <v>3752.5455000000002</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>427</v>
       </c>
       <c r="L5" s="22">
-        <f>'[2]Financial Model'!$V$42</f>
+        <f>'[3]Financial Model'!$V$42</f>
         <v>0.26862302483069977</v>
       </c>
       <c r="M5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="S5" s="35">
-        <f>[2]Main!$C$35</f>
+        <f>[3]Main!$C$35</f>
         <v>1.3933386917609896</v>
       </c>
       <c r="U5" s="4" t="str">
-        <f>[2]Main!$C$30</f>
+        <f>[3]Main!$C$30</f>
         <v>Q222</v>
       </c>
       <c r="V5" s="36">
-        <f>[2]Main!$D$30</f>
+        <f>[3]Main!$D$30</f>
         <v>44378</v>
       </c>
     </row>
@@ -5804,30 +5804,30 @@
         <v>381</v>
       </c>
       <c r="F6" s="1">
-        <f>[3]Main!$C$6</f>
+        <f>[4]Main!$C$6</f>
         <v>4.5199999999999996</v>
       </c>
       <c r="G6" s="26">
-        <f>[3]Main!$C$7</f>
+        <f>[4]Main!$C$7</f>
         <v>758</v>
       </c>
       <c r="H6" s="26">
-        <f>[3]Main!$C$8</f>
+        <f>[4]Main!$C$8</f>
         <v>3426.16</v>
       </c>
       <c r="I6" s="26">
-        <f>[3]Main!$C$11</f>
+        <f>[4]Main!$C$11</f>
         <v>478</v>
       </c>
       <c r="J6" s="26">
-        <f>[3]Main!$C$12</f>
+        <f>[4]Main!$C$12</f>
         <v>2948.16</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>394</v>
       </c>
       <c r="L6" s="22">
-        <f>'[3]Financial Model'!$I$31</f>
+        <f>'[4]Financial Model'!$I$31</f>
         <v>2.4699599465954607E-2</v>
       </c>
       <c r="M6" s="4"/>
@@ -5856,40 +5856,40 @@
         <v>377</v>
       </c>
       <c r="F7" s="1">
-        <f>[4]Main!$C$6</f>
+        <f>[5]Main!$C$6</f>
         <v>23.2</v>
       </c>
       <c r="G7" s="26">
-        <f>[4]Main!$C$7</f>
+        <f>[5]Main!$C$7</f>
         <v>103.7</v>
       </c>
       <c r="H7" s="26">
-        <f>[4]Main!$C$8</f>
+        <f>[5]Main!$C$8</f>
         <v>2405.84</v>
       </c>
       <c r="I7" s="1">
-        <f>[4]Main!$C$11</f>
+        <f>[5]Main!$C$11</f>
         <v>0</v>
       </c>
       <c r="J7" s="26">
-        <f>[4]Main!$C$12</f>
+        <f>[5]Main!$C$12</f>
         <v>2405.84</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="22">
-        <f>'[4]Financial Model'!$L$25</f>
+        <f>'[5]Financial Model'!$L$25</f>
         <v>0.47730688307784791</v>
       </c>
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
       <c r="O7" s="4">
-        <f>[4]Main!$D$21</f>
+        <f>[5]Main!$D$21</f>
         <v>0</v>
       </c>
       <c r="P7" s="4">
-        <f>[4]Main!$D$22</f>
+        <f>[5]Main!$D$22</f>
         <v>153</v>
       </c>
       <c r="Q7" s="4"/>
@@ -5909,23 +5909,23 @@
         <v>381</v>
       </c>
       <c r="F8" s="1">
-        <f>[5]Main!$C$6</f>
+        <f>[6]Main!$C$6</f>
         <v>10.029999999999999</v>
       </c>
       <c r="G8" s="26">
-        <f>[5]Main!$C$7</f>
+        <f>[6]Main!$C$7</f>
         <v>214.62</v>
       </c>
       <c r="H8" s="26">
-        <f>[5]Main!$C$8</f>
+        <f>[6]Main!$C$8</f>
         <v>2152.6385999999998</v>
       </c>
       <c r="I8" s="27">
-        <f>[5]Main!$C$11</f>
+        <f>[6]Main!$C$11</f>
         <v>0</v>
       </c>
       <c r="J8" s="26">
-        <f>[5]Main!$C$12</f>
+        <f>[6]Main!$C$12</f>
         <v>2152.6385999999998</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -5956,22 +5956,22 @@
       <c r="S9" s="4"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
       <c r="S10" s="4"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
@@ -6146,20 +6146,20 @@
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D20" s="1"/>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="41" t="s">
         <v>378</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="43"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D21" s="1"/>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="39" t="s">
         <v>379</v>
       </c>
-      <c r="G21" s="45"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="23">
         <v>0.9</v>
       </c>
@@ -6168,10 +6168,10 @@
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
-      <c r="F22" s="44" t="s">
+      <c r="F22" s="39" t="s">
         <v>380</v>
       </c>
-      <c r="G22" s="45"/>
+      <c r="G22" s="40"/>
       <c r="H22" s="23">
         <v>0.85</v>
       </c>
@@ -6180,10 +6180,10 @@
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="F23" s="44" t="s">
+      <c r="F23" s="39" t="s">
         <v>391</v>
       </c>
-      <c r="G23" s="45"/>
+      <c r="G23" s="40"/>
       <c r="H23" s="23">
         <v>6.0000000000000001E-3</v>
       </c>

</xml_diff>

<commit_message>
Add Airline Services screening
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F53974-6417-494A-BE58-96E2704B2F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8139792B-174C-3B4B-A05B-245906AB11D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="32400" windowHeight="18900" activeTab="1" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
+    <workbookView xWindow="680" yWindow="500" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
   <sheets>
-    <sheet name="Industry Screening" sheetId="2" r:id="rId1"/>
-    <sheet name="Main" sheetId="1" r:id="rId2"/>
-    <sheet name="Private Equity" sheetId="3" r:id="rId3"/>
+    <sheet name="Airlines Screening" sheetId="2" r:id="rId1"/>
+    <sheet name="Airport Services Screen" sheetId="4" r:id="rId2"/>
+    <sheet name="Main" sheetId="1" r:id="rId3"/>
+    <sheet name="Private Equity" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -199,7 +200,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="3">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -214,25 +215,35 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="3">
     <bk>
       <rc t="2" v="0"/>
     </bk>
     <bk>
       <rc t="2" v="1"/>
     </bk>
+    <bk>
+      <rc t="2" v="2"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="610">
   <si>
     <t>Ticker</t>
   </si>
@@ -1549,6 +1560,519 @@
   </si>
   <si>
     <t>No. Airlines</t>
+  </si>
+  <si>
+    <t>$ATSG</t>
+  </si>
+  <si>
+    <t>Air Transport Services Group, Inc.</t>
+  </si>
+  <si>
+    <t>Worldwide cargo &amp; combi charters for freight as well as US DoD</t>
+  </si>
+  <si>
+    <t>SYD</t>
+  </si>
+  <si>
+    <t>Sydney Airport Limited Stapled Securities</t>
+  </si>
+  <si>
+    <t>Airport Services</t>
+  </si>
+  <si>
+    <t>$35.06B</t>
+  </si>
+  <si>
+    <t>AUD$508.100M</t>
+  </si>
+  <si>
+    <t>AUD$8.72</t>
+  </si>
+  <si>
+    <t>SYDDF</t>
+  </si>
+  <si>
+    <t>Sydney Airport Limited</t>
+  </si>
+  <si>
+    <t>$31.75B</t>
+  </si>
+  <si>
+    <t>AUD$371.100M</t>
+  </si>
+  <si>
+    <t>$5.46</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>Aeroports de Paris SA</t>
+  </si>
+  <si>
+    <t>$13.93B</t>
+  </si>
+  <si>
+    <t>€1.250B</t>
+  </si>
+  <si>
+    <t>59.922k</t>
+  </si>
+  <si>
+    <t>AER</t>
+  </si>
+  <si>
+    <t>Aercap Holdings N.V.</t>
+  </si>
+  <si>
+    <t>$13.63B</t>
+  </si>
+  <si>
+    <t>$4.553B</t>
+  </si>
+  <si>
+    <t>926.820k</t>
+  </si>
+  <si>
+    <t>$55.66</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>Grupo Aeroportuario Del Pacifico SAB de CV</t>
+  </si>
+  <si>
+    <t>$8.33B</t>
+  </si>
+  <si>
+    <t>45.475k</t>
+  </si>
+  <si>
+    <t>$160.56</t>
+  </si>
+  <si>
+    <t>AIA</t>
+  </si>
+  <si>
+    <t>Auckland International Airport Limited</t>
+  </si>
+  <si>
+    <t>$7.08B</t>
+  </si>
+  <si>
+    <t>NZD$139.100M</t>
+  </si>
+  <si>
+    <t>657.927k</t>
+  </si>
+  <si>
+    <t>AUD$6.93</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>Grupo Aeroportuario Del Sureste S.A.</t>
+  </si>
+  <si>
+    <t>$6.91B</t>
+  </si>
+  <si>
+    <t>43.133k</t>
+  </si>
+  <si>
+    <t>$228.91</t>
+  </si>
+  <si>
+    <t>AUKNY</t>
+  </si>
+  <si>
+    <t>Auckland International Airport Ltd.</t>
+  </si>
+  <si>
+    <t>$6.53B</t>
+  </si>
+  <si>
+    <t>$21.41</t>
+  </si>
+  <si>
+    <t>BOC Aviation Limited</t>
+  </si>
+  <si>
+    <t>$5.21B</t>
+  </si>
+  <si>
+    <t>$1.233B</t>
+  </si>
+  <si>
+    <t>423.346k</t>
+  </si>
+  <si>
+    <t>HKD$58.90</t>
+  </si>
+  <si>
+    <t>FLGZY</t>
+  </si>
+  <si>
+    <t>Flughafen Zurich AG</t>
+  </si>
+  <si>
+    <t>$4.83B</t>
+  </si>
+  <si>
+    <t>CHF291.600M</t>
+  </si>
+  <si>
+    <t>$5.98</t>
+  </si>
+  <si>
+    <t>SIG</t>
+  </si>
+  <si>
+    <t>Signature Aviation plc</t>
+  </si>
+  <si>
+    <t>$4.58B</t>
+  </si>
+  <si>
+    <t>$264.400M</t>
+  </si>
+  <si>
+    <t>GBX396.00</t>
+  </si>
+  <si>
+    <t>OMAB</t>
+  </si>
+  <si>
+    <t>Grupo Aeroportuario del Centro Norte S.A.B de C.V.</t>
+  </si>
+  <si>
+    <t>36.520k</t>
+  </si>
+  <si>
+    <t>$65.19</t>
+  </si>
+  <si>
+    <t>AAWW</t>
+  </si>
+  <si>
+    <t>Atlas Air Worldwide Holdings Inc.</t>
+  </si>
+  <si>
+    <t>$990.159M</t>
+  </si>
+  <si>
+    <t>962.867k</t>
+  </si>
+  <si>
+    <t>$100.44</t>
+  </si>
+  <si>
+    <t>BJCHF</t>
+  </si>
+  <si>
+    <t>Beijing Capital International Airport Co., Ltd.</t>
+  </si>
+  <si>
+    <t>-¥1.49</t>
+  </si>
+  <si>
+    <t>$0.59</t>
+  </si>
+  <si>
+    <t>Beijing Capital International Airport Company Limited</t>
+  </si>
+  <si>
+    <t>$2.71B</t>
+  </si>
+  <si>
+    <t>3.494M</t>
+  </si>
+  <si>
+    <t>HKD$4.64</t>
+  </si>
+  <si>
+    <t>ATSG</t>
+  </si>
+  <si>
+    <t>Air Transport Services Group Inc</t>
+  </si>
+  <si>
+    <t>$2.11B</t>
+  </si>
+  <si>
+    <t>$592.921M</t>
+  </si>
+  <si>
+    <t>271.567k</t>
+  </si>
+  <si>
+    <t>$28.47</t>
+  </si>
+  <si>
+    <t>CAAP</t>
+  </si>
+  <si>
+    <t>Corporacion America Airports S.A.</t>
+  </si>
+  <si>
+    <t>$1.30B</t>
+  </si>
+  <si>
+    <t>76.240k</t>
+  </si>
+  <si>
+    <t>$8.12</t>
+  </si>
+  <si>
+    <t>HNA Infrastructure Company Limited</t>
+  </si>
+  <si>
+    <t>$904.24M</t>
+  </si>
+  <si>
+    <t>¥732.842M</t>
+  </si>
+  <si>
+    <t>844.922k</t>
+  </si>
+  <si>
+    <t>HKD$15.00</t>
+  </si>
+  <si>
+    <t>ASLE</t>
+  </si>
+  <si>
+    <t>AerSale Corporation</t>
+  </si>
+  <si>
+    <t>$852.46M</t>
+  </si>
+  <si>
+    <t>$70.682M</t>
+  </si>
+  <si>
+    <t>212.868k</t>
+  </si>
+  <si>
+    <t>$18.95</t>
+  </si>
+  <si>
+    <t>MIC</t>
+  </si>
+  <si>
+    <t>Macquarie Infrastructure Holdings LLC</t>
+  </si>
+  <si>
+    <t>$363.95M</t>
+  </si>
+  <si>
+    <t>-$94.84</t>
+  </si>
+  <si>
+    <t>$4.09</t>
+  </si>
+  <si>
+    <t>China Aircraft Leasing Group Holdings Limited</t>
+  </si>
+  <si>
+    <t>$298.69M</t>
+  </si>
+  <si>
+    <t>152.689k</t>
+  </si>
+  <si>
+    <t>HKD$3.16</t>
+  </si>
+  <si>
+    <t>ERA</t>
+  </si>
+  <si>
+    <t>Era Group, Inc.</t>
+  </si>
+  <si>
+    <t>$111.07M</t>
+  </si>
+  <si>
+    <t>205.700k</t>
+  </si>
+  <si>
+    <t>$5.15</t>
+  </si>
+  <si>
+    <t>AIR</t>
+  </si>
+  <si>
+    <t>Air Partner Plc</t>
+  </si>
+  <si>
+    <t>$99.40M</t>
+  </si>
+  <si>
+    <t>£4.479M</t>
+  </si>
+  <si>
+    <t>GBX124.50</t>
+  </si>
+  <si>
+    <t>AVAP</t>
+  </si>
+  <si>
+    <t>Avation Plc</t>
+  </si>
+  <si>
+    <t>$83.61M</t>
+  </si>
+  <si>
+    <t>$87.275M</t>
+  </si>
+  <si>
+    <t>54.494k</t>
+  </si>
+  <si>
+    <t>GBX98.30</t>
+  </si>
+  <si>
+    <t>TAALENT</t>
+  </si>
+  <si>
+    <t>TAAL Enterprises Limited</t>
+  </si>
+  <si>
+    <t>$61.72M</t>
+  </si>
+  <si>
+    <t>₨254.017M</t>
+  </si>
+  <si>
+    <t>1.632k</t>
+  </si>
+  <si>
+    <t>₨1,620.00</t>
+  </si>
+  <si>
+    <t>GVKPIL</t>
+  </si>
+  <si>
+    <t>GVK Power &amp; Infrastructure Limited</t>
+  </si>
+  <si>
+    <t>$61.35M</t>
+  </si>
+  <si>
+    <t>₨732.175M</t>
+  </si>
+  <si>
+    <t>3.584M</t>
+  </si>
+  <si>
+    <t>₨2.90</t>
+  </si>
+  <si>
+    <t>$58.18M</t>
+  </si>
+  <si>
+    <t>$16.682B</t>
+  </si>
+  <si>
+    <t>3.418M</t>
+  </si>
+  <si>
+    <t>₨2.89</t>
+  </si>
+  <si>
+    <t>GMAA</t>
+  </si>
+  <si>
+    <t>Gama Aviation Plc</t>
+  </si>
+  <si>
+    <t>$48.69M</t>
+  </si>
+  <si>
+    <t>$3.928M</t>
+  </si>
+  <si>
+    <t>6.999k</t>
+  </si>
+  <si>
+    <t>GBX62.00</t>
+  </si>
+  <si>
+    <t>Asia-express Logistics Holdings Limited</t>
+  </si>
+  <si>
+    <t>$10.40M</t>
+  </si>
+  <si>
+    <t>449.630k</t>
+  </si>
+  <si>
+    <t>HKD$0.17</t>
+  </si>
+  <si>
+    <t>GLOBALVECT</t>
+  </si>
+  <si>
+    <t>Global Vectra Helicorp Limited</t>
+  </si>
+  <si>
+    <t>$9.51M</t>
+  </si>
+  <si>
+    <t>₨455.833M</t>
+  </si>
+  <si>
+    <t>68.141k</t>
+  </si>
+  <si>
+    <t>₨54.65</t>
+  </si>
+  <si>
+    <t>$9.49M</t>
+  </si>
+  <si>
+    <t>₨756.139M</t>
+  </si>
+  <si>
+    <t>9.364k</t>
+  </si>
+  <si>
+    <t>₨54.00</t>
+  </si>
+  <si>
+    <t>MLAAE</t>
+  </si>
+  <si>
+    <t>Caire</t>
+  </si>
+  <si>
+    <t>$3.56M</t>
+  </si>
+  <si>
+    <t>PJT</t>
+  </si>
+  <si>
+    <t>Partner Jet Corp.</t>
+  </si>
+  <si>
+    <t>$2.89M</t>
+  </si>
+  <si>
+    <t>-1.19CAD$</t>
+  </si>
+  <si>
+    <t>CAD$5.27</t>
+  </si>
+  <si>
+    <t>CHHCF</t>
+  </si>
+  <si>
+    <t>CHC Group LLC</t>
+  </si>
+  <si>
+    <t>$0.01</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +2087,7 @@
     <numFmt numFmtId="167" formatCode="&quot;0&quot;#"/>
     <numFmt numFmtId="168" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1657,8 +2181,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF3F51B5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1692,6 +2222,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1790,7 +2326,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1853,6 +2389,9 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1880,8 +2419,10 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1997,8 +2538,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2140,7 +2681,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2181,6 +2722,9 @@
             <v>1799.1950000000002</v>
           </cell>
         </row>
+        <row r="21">
+          <cell r="D21"/>
+        </row>
         <row r="22">
           <cell r="D22">
             <v>153</v>
@@ -2204,7 +2748,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2256,8 +2800,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2304,7 +2848,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
   <rv s="0">
     <v>12</v>
     <v>00</v>
@@ -2313,6 +2857,11 @@
   <rv s="0">
     <v>12</v>
     <v>52</v>
+    <v>0</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>22</v>
     <v>0</v>
   </rv>
 </rvData>
@@ -2630,8 +3179,8 @@
   </sheetPr>
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5633,14 +6182,1624 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1929FE-0BC2-6848-BD0A-9E287659518B}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:N35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="20"/>
+    <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="48"/>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="8">
+        <v>111.27</v>
+      </c>
+      <c r="I2" s="7">
+        <v>-3.01</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0</v>
+      </c>
+      <c r="K2" s="13">
+        <v>0.36730000000000002</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="N2" s="9">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="8">
+        <v>154.27000000000001</v>
+      </c>
+      <c r="I3" s="8">
+        <v>808.78</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0.3669</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="N3" s="11">
+        <v>-0.11940000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="8">
+        <v>16.829999999999998</v>
+      </c>
+      <c r="I4" s="8">
+        <v>4.22</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0.1336</v>
+      </c>
+      <c r="L4" s="10">
+        <v>44861</v>
+      </c>
+      <c r="M4" s="12">
+        <v>137.44999999999999</v>
+      </c>
+      <c r="N4" s="11">
+        <v>-1.8E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="G5" s="7">
+        <v>7.14</v>
+      </c>
+      <c r="H5" s="8">
+        <v>13.01</v>
+      </c>
+      <c r="I5" s="8">
+        <v>3.5</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="N5" s="9">
+        <v>3.2800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>464</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="8">
+        <v>33.520000000000003</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1.81</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0.17630000000000001</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="N6" s="9">
+        <v>4.6100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>472</v>
+      </c>
+      <c r="G7" s="8">
+        <v>138.6</v>
+      </c>
+      <c r="H7" s="8">
+        <v>88.1</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="K7" s="13">
+        <v>0.21</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="N7" s="9">
+        <v>5.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="15">
+        <v>23.6</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0.54</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0.22090000000000001</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="N8" s="9">
+        <v>2.46E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>472</v>
+      </c>
+      <c r="G9" s="8">
+        <v>56.34</v>
+      </c>
+      <c r="H9" s="8">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="J9" s="8">
+        <v>667</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="N9" s="11">
+        <v>-1.5599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="19">
+        <v>2588</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="G10" s="7">
+        <v>9.24</v>
+      </c>
+      <c r="H10" s="8">
+        <v>16.79</v>
+      </c>
+      <c r="I10" s="8">
+        <v>3.53</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="L10" s="10">
+        <v>44791</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="N10" s="9">
+        <v>4.1599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="G11" s="8">
+        <v>50.5</v>
+      </c>
+      <c r="H11" s="8">
+        <v>19.41</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="J11" s="8">
+        <v>255</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="N11" s="9">
+        <v>8.3999999999999995E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="8">
+        <v>25.25</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1.89</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0.87319999999999998</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="N12" s="9">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="7">
+        <v>19.059999999999999</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1.05</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="K13" s="11">
+        <v>9.4200000000000006E-2</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="N13" s="9">
+        <v>1.5299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="G14" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="H14" s="7">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="I14" s="8">
+        <v>1.29</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="K14" s="9">
+        <v>1</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="N14" s="9">
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="G15" s="7">
+        <v>5.96</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0.74</v>
+      </c>
+      <c r="J15" s="8">
+        <v>667</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="N15" s="9">
+        <v>0.1346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="19">
+        <v>694</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="G16" s="7">
+        <v>7.55</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="15">
+        <v>0.74</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="L16" s="10">
+        <v>44803</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="N16" s="9">
+        <v>6.4199999999999993E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="G17" s="7">
+        <v>9.92</v>
+      </c>
+      <c r="H17" s="7">
+        <v>5.58</v>
+      </c>
+      <c r="I17" s="8">
+        <v>1.47</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>520</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="N17" s="9">
+        <v>3.1099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>522</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>524</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="15">
+        <v>13.53</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="8">
+        <v>6.06</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="K18" s="13">
+        <v>0.1188</v>
+      </c>
+      <c r="L18" s="47">
+        <v>44882</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="N18" s="11">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="19">
+        <v>357</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="G19" s="7">
+        <v>11</v>
+      </c>
+      <c r="H19" s="15">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="I19" s="8">
+        <v>1.46</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0.58440000000000003</v>
+      </c>
+      <c r="L19" s="10">
+        <v>44799</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="N19" s="9">
+        <v>6.8400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>534</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>535</v>
+      </c>
+      <c r="G20" s="7">
+        <v>18.05</v>
+      </c>
+      <c r="H20" s="8">
+        <v>15.01</v>
+      </c>
+      <c r="I20" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0.65839999999999999</v>
+      </c>
+      <c r="L20" s="47">
+        <v>44873</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="N20" s="9">
+        <v>5.3E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="15">
+        <v>0.79</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0.85389999999999999</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="N21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="19">
+        <v>1848</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="H22" s="8">
+        <v>15.45</v>
+      </c>
+      <c r="I22" s="8">
+        <v>7.28</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0.4017</v>
+      </c>
+      <c r="L22" s="10">
+        <v>44862</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="N22" s="11">
+        <v>-6.3E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>547</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>550</v>
+      </c>
+      <c r="K23" s="11">
+        <v>0</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="N23" s="11">
+        <v>-0.16120000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>552</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>555</v>
+      </c>
+      <c r="G24" s="8">
+        <v>31.13</v>
+      </c>
+      <c r="H24" s="15">
+        <v>12.41</v>
+      </c>
+      <c r="I24" s="8">
+        <v>22.32</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0</v>
+      </c>
+      <c r="K24" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="N24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="15">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="I25" s="8">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>561</v>
+      </c>
+      <c r="K25" s="13">
+        <v>0.48430000000000001</v>
+      </c>
+      <c r="L25" s="10">
+        <v>44833</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="N25" s="9">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="G26" s="8">
+        <v>30.08</v>
+      </c>
+      <c r="H26" s="8">
+        <v>16.34</v>
+      </c>
+      <c r="I26" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="K26" s="11">
+        <v>0</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="N26" s="9">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="H27" s="8">
+        <v>124.51</v>
+      </c>
+      <c r="I27" s="7">
+        <v>-3.82</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="K27" s="11">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="L27" s="10">
+        <v>44785</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="N27" s="9">
+        <v>3.5700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="I28" s="8">
+        <v>971.61</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="K28" s="11">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="N28" s="9">
+        <v>2.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>579</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="8">
+        <v>35.93</v>
+      </c>
+      <c r="I29" s="8">
+        <v>3.53</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="K29" s="11">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="L29" s="10">
+        <v>44832</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="N29" s="11">
+        <v>-3.8800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="19">
+        <v>8620</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>585</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="F30" s="8" t="e" cm="1" vm="3">
+        <f t="array" ref="F30">-_FV(HKD$7,"22")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G30" s="8">
+        <v>30.21</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I30" s="8">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="K30" s="11">
+        <v>0</v>
+      </c>
+      <c r="L30" s="10">
+        <v>44785</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="N30" s="11">
+        <v>-4.4900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>589</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" s="7">
+        <v>7.09</v>
+      </c>
+      <c r="I31" s="8">
+        <v>15.56</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="K31" s="11">
+        <v>0</v>
+      </c>
+      <c r="L31" s="47">
+        <v>44874</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="N31" s="9">
+        <v>2.63E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="19" t="s">
+        <v>589</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" s="7">
+        <v>4.92</v>
+      </c>
+      <c r="I32" s="8">
+        <v>9.19</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="K32" s="11">
+        <v>0</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="N32" s="9">
+        <v>2.3699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="8">
+        <v>18</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M33" s="12">
+        <v>4</v>
+      </c>
+      <c r="N33" s="9">
+        <v>6.9500000000000006E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="G34" s="8">
+        <v>69.41</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="J34" s="8">
+        <v>0</v>
+      </c>
+      <c r="K34" s="11">
+        <v>0</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="N34" s="11">
+        <v>-1.8599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
+        <v>607</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J35" s="8">
+        <v>0</v>
+      </c>
+      <c r="K35" s="9">
+        <v>1</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="N35" s="9">
+        <v>49.000100000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=n&amp;r=o" xr:uid="{5EEDAC1C-E068-564D-B3B1-575C737A32AC}"/>
+    <hyperlink ref="C1" r:id="rId2" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=e&amp;r=o" xr:uid="{4A1BCDA7-16EA-9B4D-A933-BDCD94BF419B}"/>
+    <hyperlink ref="D1" r:id="rId3" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=i&amp;r=o" xr:uid="{6432D915-440A-7740-B367-DDC8996495BE}"/>
+    <hyperlink ref="E1" r:id="rId4" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=m&amp;r=o" xr:uid="{3B9D2FA6-1C60-124A-8AAE-BD601E55CC3B}"/>
+    <hyperlink ref="F1" r:id="rId5" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=eb&amp;r=o" xr:uid="{C426136B-C2E6-E44E-A40A-2F0D644EE0EF}"/>
+    <hyperlink ref="G1" r:id="rId6" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=pe&amp;r=o" xr:uid="{8CCF48CE-2FC8-AE4C-A46F-609542395785}"/>
+    <hyperlink ref="H1" r:id="rId7" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=ee&amp;r=o" xr:uid="{68413D75-DA6B-E844-BA05-73163BB202C2}"/>
+    <hyperlink ref="I1" r:id="rId8" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=d2e&amp;r=o" xr:uid="{9BD6A3CF-A7B6-3041-9D0B-EE262A7BFBBD}"/>
+    <hyperlink ref="J1" r:id="rId9" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=av&amp;r=o" xr:uid="{2A765050-E79B-814A-A358-88D07BB32DF7}"/>
+    <hyperlink ref="K1" r:id="rId10" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=ito&amp;r=o" xr:uid="{9CCEF475-A3F3-A44B-AEB0-9E5BCC9CE22F}"/>
+    <hyperlink ref="L1" r:id="rId11" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=ed&amp;r=o" xr:uid="{A1841BF9-A215-964B-842A-3B7139F3AE96}"/>
+    <hyperlink ref="M1" r:id="rId12" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=p&amp;r=o" xr:uid="{80F94D19-8DB8-2C43-8556-AEA85272AC07}"/>
+    <hyperlink ref="N1" r:id="rId13" display="https://wallmine.com/screener?d=a&amp;i%5B%5D=224255&amp;o=pc&amp;r=o" xr:uid="{1D79533D-53E5-E847-993E-B3EEC19792A3}"/>
+    <hyperlink ref="A2" r:id="rId14" display="https://wallmine.com/asx/syd" xr:uid="{ACEFE15D-0F43-BA41-9074-3D8439AB38F9}"/>
+    <hyperlink ref="A3" r:id="rId15" display="https://wallmine.com/otc/syddf" xr:uid="{484585F0-B6B4-F34B-8801-EA9809F25B10}"/>
+    <hyperlink ref="A4" r:id="rId16" display="https://wallmine.com/euronext/adp" xr:uid="{EE5A7097-889F-BD43-81B7-D07D267B5419}"/>
+    <hyperlink ref="A5" r:id="rId17" display="https://wallmine.com/nyse/aer" xr:uid="{21F7F95B-7E54-3F40-A34D-E9561DE16FFF}"/>
+    <hyperlink ref="A6" r:id="rId18" display="https://wallmine.com/nyse/pac" xr:uid="{897EEFD9-2299-6C43-9632-2D4D8DB10446}"/>
+    <hyperlink ref="A7" r:id="rId19" display="https://wallmine.com/asx/aia" xr:uid="{7AF352FA-508A-8242-9D2C-3B67B6B4BF4B}"/>
+    <hyperlink ref="A8" r:id="rId20" display="https://wallmine.com/nyse/asr" xr:uid="{F1B22823-3FCF-2643-92C4-C486B810340E}"/>
+    <hyperlink ref="A9" r:id="rId21" display="https://wallmine.com/otc/aukny" xr:uid="{4A71F4EB-C807-3F47-BC51-2D309A2D4C4A}"/>
+    <hyperlink ref="A10" r:id="rId22" display="https://wallmine.com/hkse/2588" xr:uid="{A1471AB8-12E0-234C-A984-0457B11B3CA3}"/>
+    <hyperlink ref="A11" r:id="rId23" display="https://wallmine.com/otc/flgzy" xr:uid="{CA63580E-5A7B-5046-9268-C0F3FEDEFA93}"/>
+    <hyperlink ref="A12" r:id="rId24" display="https://wallmine.com/lse/sig" xr:uid="{D0FAD076-D295-A543-93D3-B4A4218CA502}"/>
+    <hyperlink ref="A13" r:id="rId25" display="https://wallmine.com/nasdaq/omab" xr:uid="{A44A8779-5DC6-2F43-99A2-C8BA610E7950}"/>
+    <hyperlink ref="A14" r:id="rId26" display="https://wallmine.com/nasdaq/aaww" xr:uid="{636E58F4-7645-2445-9225-BF2A7281766E}"/>
+    <hyperlink ref="A15" r:id="rId27" display="https://wallmine.com/otc/bjchf" xr:uid="{2362827F-6A59-9C40-80B2-A0733B68E670}"/>
+    <hyperlink ref="A16" r:id="rId28" display="https://wallmine.com/hkse/0694" xr:uid="{14F59A96-B9B3-FE43-836C-ABF59D1016D4}"/>
+    <hyperlink ref="A17" r:id="rId29" display="https://wallmine.com/nasdaq/atsg" xr:uid="{EFC2EA58-4F1D-2540-8E15-1AF598C81499}"/>
+    <hyperlink ref="A18" r:id="rId30" display="https://wallmine.com/nyse/caap" xr:uid="{DD78D168-9C20-2343-AA7D-700DB2696513}"/>
+    <hyperlink ref="A19" r:id="rId31" display="https://wallmine.com/hkse/0357" xr:uid="{5AC96315-7250-9C45-B1C6-F0FD4504DDB7}"/>
+    <hyperlink ref="A20" r:id="rId32" display="https://wallmine.com/nasdaq/asle" xr:uid="{41C592AE-9ED0-E241-99C8-32D41C74D20E}"/>
+    <hyperlink ref="A21" r:id="rId33" display="https://wallmine.com/nyse/mic" xr:uid="{26D614EA-E6A4-DC40-9DDF-1D5FCAD6D894}"/>
+    <hyperlink ref="A22" r:id="rId34" display="https://wallmine.com/hkse/1848" xr:uid="{826079C5-E80C-5A41-A5F8-8FC6141EC5F8}"/>
+    <hyperlink ref="A23" r:id="rId35" display="https://wallmine.com/nyse/era" xr:uid="{B92FF20E-A8FF-684D-8F2A-D6D545BB15CA}"/>
+    <hyperlink ref="A24" r:id="rId36" display="https://wallmine.com/lse/air" xr:uid="{C079862B-61D3-FB46-885D-C6D69C049EC3}"/>
+    <hyperlink ref="A25" r:id="rId37" display="https://wallmine.com/lse/avap" xr:uid="{98875337-6499-2043-8441-5EE737A3A19F}"/>
+    <hyperlink ref="A26" r:id="rId38" display="https://wallmine.com/bse/taalent" xr:uid="{4B1FC939-133B-B94E-BDFC-E74AFE21D693}"/>
+    <hyperlink ref="A27" r:id="rId39" display="https://wallmine.com/nse/gvkpil" xr:uid="{FEADC03D-6C95-2948-B0E0-B750860080EF}"/>
+    <hyperlink ref="A28" r:id="rId40" display="https://wallmine.com/bse/gvkpil" xr:uid="{0030123D-CC3F-154F-8776-9E22BD21621A}"/>
+    <hyperlink ref="A29" r:id="rId41" display="https://wallmine.com/lse/gmaa" xr:uid="{5ED9ADE3-6FD1-D845-92C2-4629FFDC5055}"/>
+    <hyperlink ref="A30" r:id="rId42" display="https://wallmine.com/hkse/8620" xr:uid="{1B7AAF6E-FF34-D244-A9E0-9A605C169D2C}"/>
+    <hyperlink ref="A31" r:id="rId43" display="https://wallmine.com/nse/globalvect" xr:uid="{3252F405-3989-334D-BE1D-62F7DF30811E}"/>
+    <hyperlink ref="A32" r:id="rId44" display="https://wallmine.com/bse/globalvect" xr:uid="{2907CC5F-0F78-534D-8D2F-329E8B687322}"/>
+    <hyperlink ref="A33" r:id="rId45" display="https://wallmine.com/euronext/mlaae" xr:uid="{158C297F-A542-5C4F-9672-5DCBFB4D42CB}"/>
+    <hyperlink ref="A34" r:id="rId46" display="https://wallmine.com/tsxv/pjt" xr:uid="{FEA2224D-C48E-CC44-BE75-66C16AB92D87}"/>
+    <hyperlink ref="A35" r:id="rId47" display="https://wallmine.com/otc/chhcf" xr:uid="{B4B69CD1-BA34-6741-8B68-847309AA6F77}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:X24"/>
+  <dimension ref="B1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H44" sqref="H44"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5668,13 +7827,13 @@
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.15">
       <c r="D1" s="1"/>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="45" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
@@ -5760,7 +7919,7 @@
         <v>435</v>
       </c>
       <c r="F3" s="28">
-        <f>[1]Main!$C$6*H24</f>
+        <f>[1]Main!$C$6*H25</f>
         <v>19.570099999999996</v>
       </c>
       <c r="G3" s="26">
@@ -5768,15 +7927,15 @@
         <v>385.26</v>
       </c>
       <c r="H3" s="26">
-        <f>[1]Main!$C$8*H24</f>
+        <f>[1]Main!$C$8*H25</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="I3" s="27">
-        <f>[1]Main!$C$11*H24</f>
+        <f>[1]Main!$C$11*H25</f>
         <v>0</v>
       </c>
       <c r="J3" s="26">
-        <f>[1]Main!$C$12*H24</f>
+        <f>[1]Main!$C$12*H25</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -5863,7 +8022,7 @@
         <v>383</v>
       </c>
       <c r="F5" s="26">
-        <f>[3]Main!$C$6*H21</f>
+        <f>[3]Main!$C$6*H22</f>
         <v>37.646999999999998</v>
       </c>
       <c r="G5" s="26">
@@ -5871,15 +8030,15 @@
         <v>126.5</v>
       </c>
       <c r="H5" s="26">
-        <f>[3]Main!$C$8*H21</f>
+        <f>[3]Main!$C$8*H22</f>
         <v>4762.3455000000004</v>
       </c>
       <c r="I5" s="27">
-        <f>[3]Main!$C$11*H21</f>
+        <f>[3]Main!$C$11*H22</f>
         <v>1009.8000000000001</v>
       </c>
       <c r="J5" s="26">
-        <f>[3]Main!$C$12*H21</f>
+        <f>[3]Main!$C$12*H22</f>
         <v>3752.5455000000002</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -5899,7 +8058,7 @@
         <f>[3]Main!$C$30</f>
         <v>Q222</v>
       </c>
-      <c r="V5" s="45">
+      <c r="V5" s="36">
         <f>[3]Main!$D$30</f>
         <v>44378</v>
       </c>
@@ -5970,7 +8129,7 @@
         <f>[4]Main!$C$31</f>
         <v>H122</v>
       </c>
-      <c r="V6" s="45">
+      <c r="V6" s="36">
         <f>[4]Main!$D$31</f>
         <v>44700</v>
       </c>
@@ -6113,22 +8272,22 @@
       <c r="S9" s="4"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
       <c r="S10" s="4"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.15">
@@ -6192,7 +8351,7 @@
         <v>40.14</v>
       </c>
       <c r="H13" s="32">
-        <f>(F13*H21)*592.96</f>
+        <f>(F13*H22)*592.96</f>
         <v>21421.272960000006</v>
       </c>
       <c r="K13" s="1" t="s">
@@ -6219,7 +8378,7 @@
         <v>76.38</v>
       </c>
       <c r="H14" s="32">
-        <f>(F14*H21)*226.92</f>
+        <f>(F14*H22)*226.92</f>
         <v>15598.934639999999</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -6247,7 +8406,7 @@
       </c>
       <c r="G15" s="30"/>
       <c r="H15" s="32">
-        <f>(F15*H23)*320.79</f>
+        <f>(F15*H24)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -6273,7 +8432,7 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="H16" s="32">
-        <f>(F16*H21)*320.79</f>
+        <f>(F16*H22)*320.79</f>
         <v>2754.3029400000005</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -6301,70 +8460,96 @@
       </c>
       <c r="S17" s="4"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="D20" s="1"/>
-      <c r="F20" s="40" t="s">
-        <v>378</v>
-      </c>
-      <c r="G20" s="41"/>
-      <c r="H20" s="42"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B18" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F18" s="46">
+        <v>28.47</v>
+      </c>
+      <c r="H18" s="32">
+        <v>2117</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="H19" s="32"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.15">
       <c r="D21" s="1"/>
-      <c r="F21" s="38" t="s">
-        <v>379</v>
-      </c>
-      <c r="G21" s="39"/>
-      <c r="H21" s="23">
-        <v>0.9</v>
-      </c>
+      <c r="F21" s="41" t="s">
+        <v>378</v>
+      </c>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.15">
       <c r="D22" s="1"/>
-      <c r="F22" s="38" t="s">
-        <v>380</v>
-      </c>
-      <c r="G22" s="39"/>
+      <c r="F22" s="39" t="s">
+        <v>379</v>
+      </c>
+      <c r="G22" s="40"/>
       <c r="H22" s="23">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.15">
       <c r="D23" s="1"/>
-      <c r="F23" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="G23" s="39"/>
+      <c r="F23" s="39" t="s">
+        <v>380</v>
+      </c>
+      <c r="G23" s="40"/>
       <c r="H23" s="23">
-        <v>6.0000000000000001E-3</v>
+        <v>0.85</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="F24" s="36" t="s">
+      <c r="D24" s="1"/>
+      <c r="F24" s="39" t="s">
+        <v>391</v>
+      </c>
+      <c r="G24" s="40"/>
+      <c r="H24" s="23">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="F25" s="37" t="s">
         <v>436</v>
       </c>
-      <c r="G24" s="37"/>
-      <c r="H24" s="24">
+      <c r="G25" s="38"/>
+      <c r="H25" s="24">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="F25:G25"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
     <mergeCell ref="B10:Q10"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
@@ -6380,7 +8565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA0EDE9-69E3-4DB1-A599-3D030985D0D0}">
   <dimension ref="B2:L5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Create $ATSG model, add latest FQ financial data
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8139792B-174C-3B4B-A05B-245906AB11D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BCCAAF-2CA9-490D-A293-9DE3FC7D70A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
+    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
   <sheets>
     <sheet name="Airlines Screening" sheetId="2" r:id="rId1"/>
@@ -25,21 +25,12 @@
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -49,6 +40,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Charlie George</author>
+    <author>me</author>
   </authors>
   <commentList>
     <comment ref="O4" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
@@ -103,7 +95,105 @@
         </r>
       </text>
     </comment>
-    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
+    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>As of May 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>As of May 2022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O8" authorId="1" shapeId="0" xr:uid="{6707E1A1-B9D2-4817-8DE3-181D10B4D7FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>me:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Primarily Cargo A/C</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P8" authorId="1" shapeId="0" xr:uid="{9CECB1AB-BF64-4D62-80D4-8FDC2F945662}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>me:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Primarily Cargo A/C</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q8" authorId="1" shapeId="0" xr:uid="{F023898F-9365-4C97-A256-586C010E62F1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>me:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Primarily Cargo A/C</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
       <text>
         <r>
           <rPr>
@@ -116,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
+    <comment ref="P9" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
       <text>
         <r>
           <rPr>
@@ -129,33 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>As of May 2022</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>As of May 2022</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O11" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
+    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
       <text>
         <r>
           <rPr>
@@ -168,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P11" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
+    <comment ref="P12" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
       <text>
         <r>
           <rPr>
@@ -186,7 +250,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -194,7 +258,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -203,21 +267,21 @@
   <futureMetadata name="XLRICHVALUE" count="3">
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
@@ -1445,9 +1509,6 @@
     <t>SEHK</t>
   </si>
   <si>
-    <t>Flag carrier for China, 1/3 of "Big Three" chinese airlines</t>
-  </si>
-  <si>
     <t>$DAL</t>
   </si>
   <si>
@@ -1568,9 +1629,6 @@
     <t>Air Transport Services Group, Inc.</t>
   </si>
   <si>
-    <t>Worldwide cargo &amp; combi charters for freight as well as US DoD</t>
-  </si>
-  <si>
     <t>SYD</t>
   </si>
   <si>
@@ -2073,6 +2131,12 @@
   </si>
   <si>
     <t>$0.01</t>
+  </si>
+  <si>
+    <t>Flag carrier for China, 1/3 of "Big Three" Chinese airlines</t>
+  </si>
+  <si>
+    <t>Worldwide cargo &amp; combi charters for freight as well as US DoD. Leasing (Prime Air etc.)</t>
   </si>
 </sst>
 </file>
@@ -2080,14 +2144,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;0&quot;#"/>
     <numFmt numFmtId="168" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2187,8 +2251,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2222,12 +2306,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2324,9 +2402,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2348,7 +2426,7 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2377,7 +2455,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2391,6 +2469,10 @@
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2419,10 +2501,9 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2681,7 +2762,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2802,6 +2883,91 @@
       </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>28.47</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>73.98</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>2106.2105999999999</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>-1312.325</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>3418.5356000000002</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="D23">
+            <v>117</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="D24">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="D25" t="str">
+            <v>N/A</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>Wilmington, OH</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30">
+            <v>1980</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33" t="str">
+            <v>Q222</v>
+          </cell>
+          <cell r="D33">
+            <v>44777</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>1.4921863586996182</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="37">
+          <cell r="T37">
+            <v>0.33796510669690843</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3183,13 +3349,13 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="20"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="20"/>
+    <col min="2" max="2" width="42.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
         <v>27</v>
@@ -3231,7 +3397,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
@@ -3275,7 +3441,7 @@
         <v>-1.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>48</v>
       </c>
@@ -3319,7 +3485,7 @@
         <v>-1.49E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>53</v>
       </c>
@@ -3363,7 +3529,7 @@
         <v>-9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>57</v>
       </c>
@@ -3407,7 +3573,7 @@
         <v>-3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>63</v>
       </c>
@@ -3451,7 +3617,7 @@
         <v>-2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>70</v>
       </c>
@@ -3495,7 +3661,7 @@
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>75</v>
       </c>
@@ -3539,7 +3705,7 @@
         <v>1.11E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>75</v>
       </c>
@@ -3583,7 +3749,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>82</v>
       </c>
@@ -3627,7 +3793,7 @@
         <v>2.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>753</v>
       </c>
@@ -3671,7 +3837,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>93</v>
       </c>
@@ -3715,7 +3881,7 @@
         <v>-2.93E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>93</v>
       </c>
@@ -3759,7 +3925,7 @@
         <v>-2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>103</v>
       </c>
@@ -3803,7 +3969,7 @@
         <v>-1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>1055</v>
       </c>
@@ -3847,7 +4013,7 @@
         <v>-9.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>112</v>
       </c>
@@ -3891,7 +4057,7 @@
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>670</v>
       </c>
@@ -3935,7 +4101,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>122</v>
       </c>
@@ -3979,7 +4145,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>127</v>
       </c>
@@ -4023,7 +4189,7 @@
         <v>-2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>132</v>
       </c>
@@ -4067,7 +4233,7 @@
         <v>-2.07E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>138</v>
       </c>
@@ -4111,7 +4277,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>145</v>
       </c>
@@ -4155,7 +4321,7 @@
         <v>-2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>138</v>
       </c>
@@ -4199,7 +4365,7 @@
         <v>-7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>12</v>
       </c>
@@ -4243,7 +4409,7 @@
         <v>-4.53E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>158</v>
       </c>
@@ -4287,7 +4453,7 @@
         <v>-2.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>162</v>
       </c>
@@ -4332,7 +4498,7 @@
         <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>293</v>
       </c>
@@ -4376,7 +4542,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>173</v>
       </c>
@@ -4420,7 +4586,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>178</v>
       </c>
@@ -4464,7 +4630,7 @@
         <v>-3.04E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>184</v>
       </c>
@@ -4509,7 +4675,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>11</v>
       </c>
@@ -4553,7 +4719,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>10</v>
       </c>
@@ -4597,7 +4763,7 @@
         <v>-6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>196</v>
       </c>
@@ -4641,7 +4807,7 @@
         <v>7.5399999999999995E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>201</v>
       </c>
@@ -4685,7 +4851,7 @@
         <v>-9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>207</v>
       </c>
@@ -4729,7 +4895,7 @@
         <v>-1.61E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>211</v>
       </c>
@@ -4773,7 +4939,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>217</v>
       </c>
@@ -4817,7 +4983,7 @@
         <v>-4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>223</v>
       </c>
@@ -4861,7 +5027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>227</v>
       </c>
@@ -4905,7 +5071,7 @@
         <v>-1.8200000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>231</v>
       </c>
@@ -4949,7 +5115,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>231</v>
       </c>
@@ -4993,7 +5159,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>242</v>
       </c>
@@ -5037,7 +5203,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>248</v>
       </c>
@@ -5081,7 +5247,7 @@
         <v>-3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>254</v>
       </c>
@@ -5125,7 +5291,7 @@
         <v>-4.36E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>258</v>
       </c>
@@ -5169,7 +5335,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>264</v>
       </c>
@@ -5213,7 +5379,7 @@
         <v>-4.1200000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>269</v>
       </c>
@@ -5257,7 +5423,7 @@
         <v>-5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>275</v>
       </c>
@@ -5301,7 +5467,7 @@
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>278</v>
       </c>
@@ -5345,7 +5511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>283</v>
       </c>
@@ -5390,7 +5556,7 @@
         <v>-1.4E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>288</v>
       </c>
@@ -5435,7 +5601,7 @@
         <v>-3.3300000000000003E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>293</v>
       </c>
@@ -5479,7 +5645,7 @@
         <v>-5.5E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>299</v>
       </c>
@@ -5523,7 +5689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>304</v>
       </c>
@@ -5567,7 +5733,7 @@
         <v>2.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>310</v>
       </c>
@@ -5611,7 +5777,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>316</v>
       </c>
@@ -5655,7 +5821,7 @@
         <v>-1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>316</v>
       </c>
@@ -5699,7 +5865,7 @@
         <v>-2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>326</v>
       </c>
@@ -5743,7 +5909,7 @@
         <v>-2.7799999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>332</v>
       </c>
@@ -5787,7 +5953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>337</v>
       </c>
@@ -5831,7 +5997,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>343</v>
       </c>
@@ -5875,7 +6041,7 @@
         <v>-3.7199999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>348</v>
       </c>
@@ -5920,7 +6086,7 @@
         <v>-4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
         <v>353</v>
       </c>
@@ -5964,7 +6130,7 @@
         <v>-4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>359</v>
       </c>
@@ -6008,7 +6174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>365</v>
       </c>
@@ -6052,7 +6218,7 @@
         <v>-0.88419999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>371</v>
       </c>
@@ -6192,14 +6358,14 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="20"/>
-    <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="20"/>
+    <col min="2" max="2" width="53.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="48"/>
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="38"/>
       <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
@@ -6240,24 +6406,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>164</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>444</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>446</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>67</v>
@@ -6278,30 +6444,30 @@
         <v>67</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="N2" s="9">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>67</v>
@@ -6322,30 +6488,30 @@
         <v>67</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="N3" s="11">
         <v>-0.11940000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>67</v>
@@ -6357,7 +6523,7 @@
         <v>4.22</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K4" s="13">
         <v>0.1336</v>
@@ -6372,24 +6538,24 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G5" s="7">
         <v>7.14</v>
@@ -6401,7 +6567,7 @@
         <v>3.5</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K5" s="9">
         <v>1</v>
@@ -6410,27 +6576,27 @@
         <v>67</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N5" s="9">
         <v>3.2800000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>67</v>
@@ -6445,7 +6611,7 @@
         <v>1.81</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K6" s="13">
         <v>0.17630000000000001</v>
@@ -6454,30 +6620,30 @@
         <v>67</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="N6" s="9">
         <v>4.6100000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>164</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G7" s="8">
         <v>138.6</v>
@@ -6489,7 +6655,7 @@
         <v>0.25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="K7" s="13">
         <v>0.21</v>
@@ -6498,27 +6664,27 @@
         <v>67</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N7" s="9">
         <v>5.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>67</v>
@@ -6533,7 +6699,7 @@
         <v>0.54</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K8" s="13">
         <v>0.22090000000000001</v>
@@ -6542,30 +6708,30 @@
         <v>67</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N8" s="9">
         <v>2.46E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G9" s="8">
         <v>56.34</v>
@@ -6586,30 +6752,30 @@
         <v>67</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="N9" s="11">
         <v>-1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>2588</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G10" s="7">
         <v>9.24</v>
@@ -6621,7 +6787,7 @@
         <v>3.53</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="K10" s="9">
         <v>0.91400000000000003</v>
@@ -6630,30 +6796,30 @@
         <v>44791</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="N10" s="9">
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G11" s="8">
         <v>50.5</v>
@@ -6674,30 +6840,30 @@
         <v>67</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="N11" s="9">
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>67</v>
@@ -6718,24 +6884,24 @@
         <v>67</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="N12" s="9">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>198</v>
@@ -6753,7 +6919,7 @@
         <v>1.05</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K13" s="11">
         <v>9.4200000000000006E-2</v>
@@ -6762,30 +6928,30 @@
         <v>67</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="N13" s="9">
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>209</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="G14" s="7">
         <v>7.1</v>
@@ -6797,7 +6963,7 @@
         <v>1.29</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="K14" s="9">
         <v>1</v>
@@ -6806,30 +6972,30 @@
         <v>67</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="N14" s="9">
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>213</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="G15" s="7">
         <v>5.96</v>
@@ -6850,30 +7016,30 @@
         <v>67</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N15" s="9">
         <v>0.1346</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>694</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="G16" s="7">
         <v>7.55</v>
@@ -6885,7 +7051,7 @@
         <v>0.74</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="K16" s="9">
         <v>0.71799999999999997</v>
@@ -6894,30 +7060,30 @@
         <v>44803</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="N16" s="9">
         <v>6.4199999999999993E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G17" s="7">
         <v>9.92</v>
@@ -6929,7 +7095,7 @@
         <v>1.47</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="K17" s="9">
         <v>0.99850000000000005</v>
@@ -6938,27 +7104,27 @@
         <v>67</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="N17" s="9">
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>67</v>
@@ -6973,39 +7139,39 @@
         <v>6.06</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="K18" s="13">
         <v>0.1188</v>
       </c>
-      <c r="L18" s="47">
+      <c r="L18" s="37">
         <v>44882</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="N18" s="11">
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>357</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="G19" s="7">
         <v>11</v>
@@ -7017,7 +7183,7 @@
         <v>1.46</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="K19" s="9">
         <v>0.58440000000000003</v>
@@ -7026,30 +7192,30 @@
         <v>44799</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N19" s="9">
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G20" s="7">
         <v>18.05</v>
@@ -7061,39 +7227,39 @@
         <v>0.19</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K20" s="9">
         <v>0.65839999999999999</v>
       </c>
-      <c r="L20" s="47">
+      <c r="L20" s="37">
         <v>44873</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="N20" s="9">
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="G21" s="7">
         <v>0.13</v>
@@ -7114,27 +7280,27 @@
         <v>67</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="N21" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>1848</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>67</v>
@@ -7149,7 +7315,7 @@
         <v>7.28</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="K22" s="13">
         <v>0.4017</v>
@@ -7158,27 +7324,27 @@
         <v>44862</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="N22" s="11">
         <v>-6.3E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>67</v>
@@ -7193,7 +7359,7 @@
         <v>67</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="K23" s="11">
         <v>0</v>
@@ -7202,30 +7368,30 @@
         <v>67</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="N23" s="11">
         <v>-0.16120000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G24" s="8">
         <v>31.13</v>
@@ -7246,30 +7412,30 @@
         <v>67</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="N24" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>67</v>
@@ -7281,7 +7447,7 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="K25" s="13">
         <v>0.48430000000000001</v>
@@ -7290,30 +7456,30 @@
         <v>44833</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="N25" s="9">
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>149</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="G26" s="8">
         <v>30.08</v>
@@ -7325,7 +7491,7 @@
         <v>0.9</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="K26" s="11">
         <v>0</v>
@@ -7334,30 +7500,30 @@
         <v>67</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="N26" s="9">
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="G27" s="7">
         <v>0.21</v>
@@ -7369,7 +7535,7 @@
         <v>-3.82</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="K27" s="11">
         <v>2.7000000000000001E-3</v>
@@ -7378,30 +7544,30 @@
         <v>44785</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="N27" s="9">
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>149</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>67</v>
@@ -7413,7 +7579,7 @@
         <v>971.61</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K28" s="11">
         <v>3.5900000000000001E-2</v>
@@ -7422,30 +7588,30 @@
         <v>67</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="N28" s="9">
         <v>2.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>67</v>
@@ -7457,7 +7623,7 @@
         <v>3.53</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="K29" s="11">
         <v>5.7099999999999998E-2</v>
@@ -7466,27 +7632,27 @@
         <v>44832</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="N29" s="11">
         <v>-3.8800000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>8620</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F30" s="8" t="e" cm="1" vm="3">
         <f t="array" ref="F30">-_FV(HKD$7,"22")</f>
@@ -7502,7 +7668,7 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="K30" s="11">
         <v>0</v>
@@ -7511,30 +7677,30 @@
         <v>44785</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="N30" s="11">
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>67</v>
@@ -7546,39 +7712,39 @@
         <v>15.56</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K31" s="11">
         <v>0</v>
       </c>
-      <c r="L31" s="47">
+      <c r="L31" s="37">
         <v>44874</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="N31" s="9">
         <v>2.63E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>149</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>67</v>
@@ -7590,7 +7756,7 @@
         <v>9.19</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="K32" s="11">
         <v>0</v>
@@ -7599,27 +7765,27 @@
         <v>67</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="N32" s="9">
         <v>2.3699999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>67</v>
@@ -7649,24 +7815,24 @@
         <v>6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>355</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="G34" s="8">
         <v>69.41</v>
@@ -7687,24 +7853,24 @@
         <v>67</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="N34" s="11">
         <v>-1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>67</v>
@@ -7731,7 +7897,7 @@
         <v>67</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="N35" s="9">
         <v>49.000100000000003</v>
@@ -7799,45 +7965,49 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16:D17"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="4"/>
-    <col min="5" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="8.83203125" style="1"/>
-    <col min="11" max="11" width="65.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.83203125" style="1"/>
-    <col min="15" max="15" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="1"/>
+    <col min="3" max="3" width="37.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="4"/>
+    <col min="5" max="5" width="8.875" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="8.875" style="1"/>
+    <col min="11" max="11" width="65.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.875" style="1"/>
+    <col min="15" max="15" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.375" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.83203125" style="1"/>
-    <col min="21" max="22" width="8.83203125" style="4"/>
-    <col min="23" max="23" width="8.83203125" style="1"/>
-    <col min="24" max="24" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.83203125" style="1"/>
+    <col min="18" max="18" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.875" style="1"/>
+    <col min="21" max="22" width="8.875" style="4"/>
+    <col min="23" max="23" width="8.875" style="1"/>
+    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="S1" s="49">
+        <f>AVERAGE(S3:S9)</f>
+        <v>1.3264810277491643</v>
+      </c>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7854,7 +8024,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>5</v>
@@ -7878,7 +8048,7 @@
         <v>386</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>23</v>
@@ -7887,36 +8057,36 @@
         <v>26</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="S2" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B3" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B3" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F3" s="28">
         <f>[1]Main!$C$6*H25</f>
@@ -7930,7 +8100,7 @@
         <f>[1]Main!$C$8*H25</f>
         <v>7539.5767259999993</v>
       </c>
-      <c r="I3" s="27">
+      <c r="I3" s="26">
         <f>[1]Main!$C$11*H25</f>
         <v>0</v>
       </c>
@@ -7939,7 +8109,7 @@
         <v>7539.5767259999993</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -7954,7 +8124,7 @@
         <v>Gurgaon, India</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
         <v>12</v>
       </c>
@@ -7979,7 +8149,7 @@
         <f>[2]Main!$C$8</f>
         <v>5543.5049999999992</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="26">
         <f>[2]Main!$C$11</f>
         <v>0</v>
       </c>
@@ -8008,12 +8178,12 @@
         <v>London/Madrid</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B5" s="25" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>42</v>
@@ -8023,7 +8193,7 @@
       </c>
       <c r="F5" s="26">
         <f>[3]Main!$C$6*H22</f>
-        <v>37.646999999999998</v>
+        <v>36.810400000000001</v>
       </c>
       <c r="G5" s="26">
         <f>[3]Main!$C$7</f>
@@ -8031,18 +8201,18 @@
       </c>
       <c r="H5" s="26">
         <f>[3]Main!$C$8*H22</f>
-        <v>4762.3455000000004</v>
-      </c>
-      <c r="I5" s="27">
+        <v>4656.5155999999997</v>
+      </c>
+      <c r="I5" s="26">
         <f>[3]Main!$C$11*H22</f>
-        <v>1009.8000000000001</v>
+        <v>987.36</v>
       </c>
       <c r="J5" s="26">
         <f>[3]Main!$C$12*H22</f>
-        <v>3752.5455000000002</v>
+        <v>3669.1556</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L5" s="22">
         <f>'[3]Financial Model'!$V$42</f>
@@ -8071,7 +8241,7 @@
         <v>Seattle, WA</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B6" s="25" t="s">
         <v>11</v>
       </c>
@@ -8142,401 +8312,451 @@
         <v>Luton, UK</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B7" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F7" s="1">
+        <f>[6]Main!$C$6</f>
+        <v>10.029999999999999</v>
+      </c>
+      <c r="G7" s="26">
+        <f>[6]Main!$C$7</f>
+        <v>214.62</v>
+      </c>
+      <c r="H7" s="26">
+        <f>[6]Main!$C$8</f>
+        <v>2152.6385999999998</v>
+      </c>
+      <c r="I7" s="26">
+        <f>[6]Main!$C$11</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="26">
+        <f>[6]Main!$C$12</f>
+        <v>2152.6385999999998</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="O7" s="4">
+        <v>96</v>
+      </c>
+      <c r="P7" s="4">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>82</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="W7" s="4">
+        <f>[6]Main!$C$28</f>
+        <v>1971</v>
+      </c>
+      <c r="X7" s="4" t="str">
+        <f>[6]Main!$C$27</f>
+        <v>Leeds, UK</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B8" s="25" t="s">
+        <v>438</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F8" s="48">
+        <f>[7]Main!$C$6*H22</f>
+        <v>25.053599999999999</v>
+      </c>
+      <c r="G8" s="1">
+        <f>[7]Main!$C$7</f>
+        <v>73.98</v>
+      </c>
+      <c r="H8" s="26">
+        <f>[7]Main!$C$8*H22</f>
+        <v>1853.465328</v>
+      </c>
+      <c r="I8" s="26">
+        <f>[7]Main!$C$11*H22</f>
+        <v>-1154.846</v>
+      </c>
+      <c r="J8" s="26">
+        <f>[7]Main!$C$12*H22</f>
+        <v>3008.3113280000002</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="L8" s="22">
+        <f>'[7]Financial Model'!$T$37</f>
+        <v>0.33796510669690843</v>
+      </c>
+      <c r="O8" s="4">
+        <f>[7]Main!$D$23</f>
+        <v>117</v>
+      </c>
+      <c r="P8" s="4">
+        <f>[7]Main!$D$24</f>
+        <v>2</v>
+      </c>
+      <c r="Q8" s="4" t="str">
+        <f>[7]Main!$D$25</f>
+        <v>N/A</v>
+      </c>
+      <c r="S8" s="35">
+        <f>[7]Main!$C$38</f>
+        <v>1.4921863586996182</v>
+      </c>
+      <c r="U8" s="4" t="str">
+        <f>[7]Main!$C$33</f>
+        <v>Q222</v>
+      </c>
+      <c r="V8" s="36">
+        <f>[7]Main!$D$33</f>
+        <v>44777</v>
+      </c>
+      <c r="W8" s="4">
+        <f>[7]Main!$C$30</f>
+        <v>1980</v>
+      </c>
+      <c r="X8" s="4" t="str">
+        <f>[7]Main!$C$29</f>
+        <v>Wilmington, OH</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F9" s="1">
         <f>[5]Main!$C$6</f>
         <v>17.350000000000001</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G9" s="26">
         <f>[5]Main!$C$7</f>
         <v>103.7</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H9" s="26">
         <f>[5]Main!$C$8</f>
         <v>1799.1950000000002</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I9" s="26">
         <f>[5]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J9" s="26">
         <f>[5]Main!$C$12</f>
         <v>1799.1950000000002</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L9" s="22">
         <f>'[5]Financial Model'!$L$25</f>
         <v>0.47730688307784791</v>
       </c>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="4">
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="4">
         <f>[5]Main!$D$21</f>
         <v>0</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P9" s="4">
         <f>[5]Main!$D$22</f>
         <v>153</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="W7" s="4">
+      <c r="Q9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="W9" s="4">
         <f>[5]Main!$C$29</f>
         <v>2003</v>
       </c>
-      <c r="X7" s="4" t="str">
+      <c r="X9" s="4" t="str">
         <f>[5]Main!$C$28</f>
         <v>Budapest, Hungary</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B8" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="F8" s="1">
-        <f>[6]Main!$C$6</f>
-        <v>10.029999999999999</v>
-      </c>
-      <c r="G8" s="26">
-        <f>[6]Main!$C$7</f>
-        <v>214.62</v>
-      </c>
-      <c r="H8" s="26">
-        <f>[6]Main!$C$8</f>
-        <v>2152.6385999999998</v>
-      </c>
-      <c r="I8" s="27">
-        <f>[6]Main!$C$11</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="26">
-        <f>[6]Main!$C$12</f>
-        <v>2152.6385999999998</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="O8" s="4">
-        <v>96</v>
-      </c>
-      <c r="P8" s="4">
-        <v>57</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>82</v>
-      </c>
-      <c r="S8" s="4"/>
-      <c r="W8" s="4">
-        <f>[6]Main!$C$28</f>
-        <v>1971</v>
-      </c>
-      <c r="X8" s="4" t="str">
-        <f>[6]Main!$C$27</f>
-        <v>Leeds, UK</v>
-      </c>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B9" s="25"/>
-      <c r="E9" s="4"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="S9" s="4"/>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B10" s="25"/>
+      <c r="E10" s="4"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="Q10" s="4"/>
       <c r="S10" s="4"/>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="S11" s="4"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="H11" s="31"/>
-      <c r="K11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="O11" s="4">
-        <v>130</v>
-      </c>
-      <c r="P11" s="4">
-        <v>44</v>
-      </c>
-      <c r="Q11" s="4"/>
-      <c r="S11" s="4"/>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B12" s="33">
-        <v>753</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>399</v>
       </c>
       <c r="H12" s="31"/>
       <c r="K12" s="1" t="s">
-        <v>400</v>
+        <v>24</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
+      <c r="O12" s="4">
+        <v>130</v>
+      </c>
+      <c r="P12" s="4">
+        <v>44</v>
+      </c>
       <c r="Q12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B13" s="1" t="s">
-        <v>382</v>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B13" s="33">
+        <v>753</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F13" s="1">
-        <v>40.14</v>
-      </c>
-      <c r="H13" s="32">
-        <f>(F13*H22)*592.96</f>
-        <v>21421.272960000006</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="H13" s="31"/>
       <c r="K13" s="1" t="s">
-        <v>397</v>
+        <v>608</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
+      <c r="Q13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>383</v>
       </c>
       <c r="F14" s="1">
-        <v>76.38</v>
+        <v>40.14</v>
       </c>
       <c r="H14" s="32">
-        <f>(F14*H22)*226.92</f>
-        <v>15598.934639999999</v>
+        <f>(F14*H22)*592.96</f>
+        <v>20945.244672000001</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B15" s="29">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F15" s="1">
+        <v>76.38</v>
+      </c>
+      <c r="H15" s="32">
+        <f>(F15*H22)*226.92</f>
+        <v>15252.291647999999</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B16" s="29">
         <v>9201</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F16" s="30">
         <v>2357</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="32">
-        <f>(F15*H24)*320.79</f>
+      <c r="G16" s="30"/>
+      <c r="H16" s="32">
+        <f>(F16*H24)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="S15" s="4"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B16" s="1" t="s">
+      <c r="L16" s="4"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F16" s="1">
-        <v>9.5399999999999991</v>
-      </c>
-      <c r="H16" s="32">
-        <f>(F16*H22)*320.79</f>
-        <v>2754.3029400000005</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="S16" s="4"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B17" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>383</v>
       </c>
+      <c r="F17" s="1">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="H17" s="32">
+        <f>(F17*H22)*320.79</f>
+        <v>2693.0962079999999</v>
+      </c>
       <c r="K17" s="1" t="s">
-        <v>402</v>
-      </c>
+        <v>395</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>439</v>
+        <v>400</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>440</v>
+        <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="F18" s="46">
-        <v>28.47</v>
-      </c>
-      <c r="H18" s="32">
-        <v>2117</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.15">
+        <v>401</v>
+      </c>
+      <c r="S18" s="4"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="H19" s="32"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D21" s="1"/>
-      <c r="F21" s="41" t="s">
+      <c r="F21" s="43" t="s">
         <v>378</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="43"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="45"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="41" t="s">
         <v>379</v>
       </c>
-      <c r="G22" s="40"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="23">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="41" t="s">
         <v>380</v>
       </c>
-      <c r="G23" s="40"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="23">
         <v>0.85</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="41" t="s">
         <v>391</v>
       </c>
-      <c r="G24" s="40"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="F25" s="37" t="s">
-        <v>436</v>
-      </c>
-      <c r="G25" s="38"/>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="F25" s="39" t="s">
+        <v>435</v>
+      </c>
+      <c r="G25" s="40"/>
       <c r="H25" s="24">
         <v>1.0999999999999999E-2</v>
       </c>
@@ -8546,22 +8766,23 @@
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="B11:Q11"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="F23:G23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{176C962A-9F96-4539-8149-82E34F7BBB40}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{56F8AAB4-AB88-4816-A70A-66823F4EBD86}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{56F8AAB4-AB88-4816-A70A-66823F4EBD86}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{593208B0-BF4C-4E7C-9DA3-9FABEC41EED7}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{5BD026C6-209C-4F8D-96F9-0D20474E4F7F}"/>
     <hyperlink ref="B3" r:id="rId6" xr:uid="{28605697-2E3F-4D0E-BA6A-013F294DB301}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{7F471098-FF05-4C1A-AA9F-8A6A66E1327B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -8573,73 +8794,73 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1"/>
-    <col min="7" max="7" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1"/>
-    <col min="10" max="10" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="1"/>
-    <col min="12" max="12" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>419</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B3" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>420</v>
       </c>
       <c r="F3" s="4">
         <v>2020</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
@@ -8651,27 +8872,27 @@
         <v>16</v>
       </c>
       <c r="K3" s="34" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F4" s="4">
         <v>1984</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H4" s="4">
         <v>36</v>
@@ -8683,21 +8904,21 @@
         <v>32</v>
       </c>
       <c r="K4" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F5" s="4">
         <v>1997</v>
@@ -8709,10 +8930,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create & start $RYAAY model
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE29E4A-4306-5E4B-8E99-8034FD9C7655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723351C2-F5CF-4ADD-970D-A0D8AC0A4C15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
+    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
   <sheets>
     <sheet name="Airlines Screening" sheetId="2" r:id="rId1"/>
@@ -26,21 +26,12 @@
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -53,7 +44,7 @@
     <author>me</author>
   </authors>
   <commentList>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
+    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
       <text>
         <r>
           <rPr>
@@ -66,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
+    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
       <text>
         <r>
           <rPr>
@@ -79,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
       <text>
         <r>
           <rPr>
@@ -92,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
+    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
       <text>
         <r>
           <rPr>
@@ -105,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
       <text>
         <r>
           <rPr>
@@ -118,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
+    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
       <text>
         <r>
           <rPr>
@@ -131,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="1" shapeId="0" xr:uid="{6707E1A1-B9D2-4817-8DE3-181D10B4D7FB}">
+    <comment ref="O9" authorId="1" shapeId="0" xr:uid="{6707E1A1-B9D2-4817-8DE3-181D10B4D7FB}">
       <text>
         <r>
           <rPr>
@@ -155,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="1" shapeId="0" xr:uid="{9CECB1AB-BF64-4D62-80D4-8FDC2F945662}">
+    <comment ref="P9" authorId="1" shapeId="0" xr:uid="{9CECB1AB-BF64-4D62-80D4-8FDC2F945662}">
       <text>
         <r>
           <rPr>
@@ -179,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="1" shapeId="0" xr:uid="{F023898F-9365-4C97-A256-586C010E62F1}">
+    <comment ref="Q9" authorId="1" shapeId="0" xr:uid="{F023898F-9365-4C97-A256-586C010E62F1}">
       <text>
         <r>
           <rPr>
@@ -203,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
       <text>
         <r>
           <rPr>
@@ -216,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P9" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
+    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
       <text>
         <r>
           <rPr>
@@ -229,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
+    <comment ref="O13" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
       <text>
         <r>
           <rPr>
@@ -242,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P12" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
+    <comment ref="P13" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
       <text>
         <r>
           <rPr>
@@ -260,7 +251,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -268,7 +259,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -277,21 +268,21 @@
   <futureMetadata name="XLRICHVALUE" count="3">
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
@@ -2156,13 +2147,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="7">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;0&quot;#"/>
     <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -2415,7 +2407,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2439,7 +2431,7 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2468,7 +2460,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2487,7 +2479,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2518,6 +2509,7 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2979,9 +2971,6 @@
             <v>1799.1950000000002</v>
           </cell>
         </row>
-        <row r="21">
-          <cell r="D21"/>
-        </row>
         <row r="22">
           <cell r="D22">
             <v>153</v>
@@ -3011,6 +3000,57 @@
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>69.05</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>227.43</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>15704.041499999999</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>Dublin, Ireland</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>1984</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32">
+            <v>1997</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3389,16 +3429,16 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B6" sqref="B6:L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="20"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="20"/>
+    <col min="2" max="2" width="42.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
         <v>27</v>
@@ -3440,7 +3480,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
@@ -3484,7 +3524,7 @@
         <v>-1.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>48</v>
       </c>
@@ -3528,7 +3568,7 @@
         <v>-1.49E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>53</v>
       </c>
@@ -3572,7 +3612,7 @@
         <v>-9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>57</v>
       </c>
@@ -3616,7 +3656,7 @@
         <v>-3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>63</v>
       </c>
@@ -3660,7 +3700,7 @@
         <v>-2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>70</v>
       </c>
@@ -3704,7 +3744,7 @@
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>75</v>
       </c>
@@ -3748,7 +3788,7 @@
         <v>1.11E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>75</v>
       </c>
@@ -3792,7 +3832,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>82</v>
       </c>
@@ -3836,7 +3876,7 @@
         <v>2.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>753</v>
       </c>
@@ -3880,7 +3920,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>93</v>
       </c>
@@ -3924,7 +3964,7 @@
         <v>-2.93E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>93</v>
       </c>
@@ -3968,7 +4008,7 @@
         <v>-2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>103</v>
       </c>
@@ -4012,7 +4052,7 @@
         <v>-1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>1055</v>
       </c>
@@ -4056,7 +4096,7 @@
         <v>-9.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>112</v>
       </c>
@@ -4100,7 +4140,7 @@
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>670</v>
       </c>
@@ -4144,7 +4184,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>122</v>
       </c>
@@ -4188,7 +4228,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>127</v>
       </c>
@@ -4232,7 +4272,7 @@
         <v>-2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>132</v>
       </c>
@@ -4276,7 +4316,7 @@
         <v>-2.07E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>138</v>
       </c>
@@ -4320,7 +4360,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>145</v>
       </c>
@@ -4364,7 +4404,7 @@
         <v>-2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>138</v>
       </c>
@@ -4408,7 +4448,7 @@
         <v>-7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>12</v>
       </c>
@@ -4452,7 +4492,7 @@
         <v>-4.53E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>158</v>
       </c>
@@ -4496,7 +4536,7 @@
         <v>-2.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>162</v>
       </c>
@@ -4541,7 +4581,7 @@
         <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>293</v>
       </c>
@@ -4585,7 +4625,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>173</v>
       </c>
@@ -4629,7 +4669,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>178</v>
       </c>
@@ -4673,7 +4713,7 @@
         <v>-3.04E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>184</v>
       </c>
@@ -4718,7 +4758,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>11</v>
       </c>
@@ -4762,7 +4802,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>10</v>
       </c>
@@ -4806,7 +4846,7 @@
         <v>-6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>196</v>
       </c>
@@ -4850,7 +4890,7 @@
         <v>7.5399999999999995E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>201</v>
       </c>
@@ -4894,7 +4934,7 @@
         <v>-9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>207</v>
       </c>
@@ -4938,7 +4978,7 @@
         <v>-1.61E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>211</v>
       </c>
@@ -4982,7 +5022,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>217</v>
       </c>
@@ -5026,7 +5066,7 @@
         <v>-4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>223</v>
       </c>
@@ -5070,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>227</v>
       </c>
@@ -5114,7 +5154,7 @@
         <v>-1.8200000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>231</v>
       </c>
@@ -5158,7 +5198,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>231</v>
       </c>
@@ -5202,7 +5242,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>242</v>
       </c>
@@ -5246,7 +5286,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>248</v>
       </c>
@@ -5290,7 +5330,7 @@
         <v>-3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>254</v>
       </c>
@@ -5334,7 +5374,7 @@
         <v>-4.36E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>258</v>
       </c>
@@ -5378,7 +5418,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>264</v>
       </c>
@@ -5422,7 +5462,7 @@
         <v>-4.1200000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>269</v>
       </c>
@@ -5466,7 +5506,7 @@
         <v>-5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>275</v>
       </c>
@@ -5510,7 +5550,7 @@
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>278</v>
       </c>
@@ -5554,7 +5594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>283</v>
       </c>
@@ -5599,7 +5639,7 @@
         <v>-1.4E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>288</v>
       </c>
@@ -5644,7 +5684,7 @@
         <v>-3.3300000000000003E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>293</v>
       </c>
@@ -5688,7 +5728,7 @@
         <v>-5.5E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>299</v>
       </c>
@@ -5732,7 +5772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>304</v>
       </c>
@@ -5776,7 +5816,7 @@
         <v>2.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>310</v>
       </c>
@@ -5820,7 +5860,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>316</v>
       </c>
@@ -5864,7 +5904,7 @@
         <v>-1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>316</v>
       </c>
@@ -5908,7 +5948,7 @@
         <v>-2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>326</v>
       </c>
@@ -5952,7 +5992,7 @@
         <v>-2.7799999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>332</v>
       </c>
@@ -5996,7 +6036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>337</v>
       </c>
@@ -6040,7 +6080,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>343</v>
       </c>
@@ -6084,7 +6124,7 @@
         <v>-3.7199999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>348</v>
       </c>
@@ -6129,7 +6169,7 @@
         <v>-4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
         <v>353</v>
       </c>
@@ -6173,7 +6213,7 @@
         <v>-4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>359</v>
       </c>
@@ -6217,7 +6257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>365</v>
       </c>
@@ -6261,7 +6301,7 @@
         <v>-0.88419999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>371</v>
       </c>
@@ -6401,13 +6441,13 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="20"/>
-    <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="20"/>
+    <col min="2" max="2" width="53.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
       <c r="B1" s="5" t="s">
         <v>27</v>
@@ -6449,7 +6489,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>440</v>
       </c>
@@ -6493,7 +6533,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>446</v>
       </c>
@@ -6537,7 +6577,7 @@
         <v>-0.11940000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>451</v>
       </c>
@@ -6581,7 +6621,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>456</v>
       </c>
@@ -6625,7 +6665,7 @@
         <v>3.2800000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>462</v>
       </c>
@@ -6669,7 +6709,7 @@
         <v>4.6100000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>467</v>
       </c>
@@ -6713,7 +6753,7 @@
         <v>5.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>473</v>
       </c>
@@ -6757,7 +6797,7 @@
         <v>2.46E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>478</v>
       </c>
@@ -6801,7 +6841,7 @@
         <v>-1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>2588</v>
       </c>
@@ -6845,7 +6885,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>487</v>
       </c>
@@ -6889,7 +6929,7 @@
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>492</v>
       </c>
@@ -6933,7 +6973,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>497</v>
       </c>
@@ -6977,7 +7017,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>501</v>
       </c>
@@ -7021,7 +7061,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>506</v>
       </c>
@@ -7065,7 +7105,7 @@
         <v>0.1346</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>694</v>
       </c>
@@ -7109,7 +7149,7 @@
         <v>6.4199999999999993E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>514</v>
       </c>
@@ -7153,7 +7193,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>520</v>
       </c>
@@ -7197,7 +7237,7 @@
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>357</v>
       </c>
@@ -7241,7 +7281,7 @@
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>530</v>
       </c>
@@ -7285,7 +7325,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>536</v>
       </c>
@@ -7329,7 +7369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>1848</v>
       </c>
@@ -7373,7 +7413,7 @@
         <v>-6.3E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>545</v>
       </c>
@@ -7417,7 +7457,7 @@
         <v>-0.16120000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>550</v>
       </c>
@@ -7461,7 +7501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>555</v>
       </c>
@@ -7505,7 +7545,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>561</v>
       </c>
@@ -7549,7 +7589,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>567</v>
       </c>
@@ -7593,7 +7633,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>567</v>
       </c>
@@ -7637,7 +7677,7 @@
         <v>2.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>577</v>
       </c>
@@ -7681,7 +7721,7 @@
         <v>-3.8800000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>8620</v>
       </c>
@@ -7726,7 +7766,7 @@
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>587</v>
       </c>
@@ -7770,7 +7810,7 @@
         <v>2.63E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>587</v>
       </c>
@@ -7814,7 +7854,7 @@
         <v>2.3699999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>597</v>
       </c>
@@ -7858,7 +7898,7 @@
         <v>6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>600</v>
       </c>
@@ -7902,7 +7942,7 @@
         <v>-1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>605</v>
       </c>
@@ -8008,49 +8048,49 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="4"/>
-    <col min="5" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="8.83203125" style="1"/>
-    <col min="11" max="11" width="65.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.83203125" style="1"/>
-    <col min="15" max="15" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="1"/>
+    <col min="3" max="3" width="37.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="4"/>
+    <col min="5" max="5" width="8.875" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="8.875" style="1"/>
+    <col min="11" max="11" width="65.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.875" style="1"/>
+    <col min="15" max="15" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.375" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.83203125" style="1"/>
-    <col min="21" max="22" width="8.83203125" style="4"/>
-    <col min="23" max="23" width="8.83203125" style="1"/>
-    <col min="24" max="24" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.83203125" style="1"/>
+    <col min="18" max="18" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="8.875" style="1"/>
+    <col min="21" max="22" width="8.875" style="4"/>
+    <col min="23" max="23" width="8.875" style="1"/>
+    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="48" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="S1" s="40">
-        <f>AVERAGE(S3:S9)</f>
+      <c r="S1" s="39">
+        <f>AVERAGE(S4:S10)</f>
         <v>1.3082569747231938</v>
       </c>
     </row>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8121,588 +8161,613 @@
         <v>610</v>
       </c>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F3" s="28">
+        <f>[8]Main!$C$6*H22</f>
+        <v>60.763999999999996</v>
+      </c>
+      <c r="G3" s="26">
+        <f>[8]Main!$C$7</f>
+        <v>227.43</v>
+      </c>
+      <c r="H3" s="26">
+        <f>[8]Main!$C$12*H22</f>
+        <v>13819.55652</v>
+      </c>
+      <c r="I3" s="49">
+        <f>[8]Main!$C$11*H22</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="26">
+        <f>[8]Main!$C$12*H22</f>
+        <v>13819.55652</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="W3" s="4">
+        <f>[8]Main!$C$31</f>
+        <v>1984</v>
+      </c>
+      <c r="X3" s="4" t="str">
+        <f>[8]Main!$C$30</f>
+        <v>Dublin, Ireland</v>
+      </c>
+      <c r="Y3" s="4">
+        <f>[8]Main!$C$32</f>
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B4" s="25" t="s">
         <v>433</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F4" s="28">
         <f>[1]Main!$C$6*H25</f>
         <v>19.570099999999996</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G4" s="26">
         <f>[1]Main!$C$7</f>
         <v>385.26</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H4" s="26">
         <f>[1]Main!$C$8*H25</f>
         <v>7539.5767259999993</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I4" s="26">
         <f>[1]Main!$C$11*H25</f>
         <v>0</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J4" s="26">
         <f>[1]Main!$C$12*H25</f>
         <v>7539.5767259999993</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="W3" s="4">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="W4" s="4">
         <f>[1]Main!$C$25</f>
         <v>2005</v>
       </c>
-      <c r="X3" s="4" t="str">
+      <c r="X4" s="4" t="str">
         <f>[1]Main!$C$24</f>
         <v>Gurgaon, India</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y4" s="4">
         <f>[1]Main!$C$26</f>
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B4" s="25" t="s">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F5" s="28">
         <f>[2]Main!$C$6</f>
         <v>1.1198999999999999</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G5" s="26">
         <f>[2]Main!$C$7</f>
         <v>4950</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H5" s="26">
         <f>[2]Main!$C$8</f>
         <v>5543.5049999999992</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I5" s="26">
         <f>[2]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J5" s="26">
         <f>[2]Main!$C$12</f>
         <v>5543.5049999999992</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="O4" s="4">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="O5" s="4">
         <v>531</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q5" s="4">
         <v>200</v>
       </c>
-      <c r="S4" s="4"/>
-      <c r="W4" s="4">
+      <c r="S5" s="4"/>
+      <c r="W5" s="4">
         <f>[2]Main!$C$28</f>
         <v>2011</v>
       </c>
-      <c r="X4" s="4" t="str">
+      <c r="X5" s="4" t="str">
         <f>[2]Main!$C$27</f>
         <v>London/Madrid</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="Y5" s="4">
         <f>[2]Main!$C$29</f>
         <v>2011</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B5" s="25" t="s">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
         <v>425</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F6" s="28">
         <f>[3]Main!$C$6*H22</f>
         <v>36.810400000000001</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G6" s="26">
         <f>[3]Main!$C$7</f>
         <v>126.5</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H6" s="26">
         <f>[3]Main!$C$8*H22</f>
         <v>4656.5155999999997</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I6" s="26">
         <f>[3]Main!$C$11*H22</f>
         <v>987.36</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J6" s="26">
         <f>[3]Main!$C$12*H22</f>
         <v>3669.1556</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L6" s="22">
         <f>'[3]Financial Model'!$V$42</f>
         <v>0.26862302483069977</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="S5" s="35">
+      <c r="M6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="S6" s="35">
         <f>[3]Main!$C$35</f>
         <v>1.3933386917609896</v>
       </c>
-      <c r="U5" s="4" t="str">
+      <c r="U6" s="4" t="str">
         <f>[3]Main!$C$30</f>
         <v>Q222</v>
       </c>
-      <c r="V5" s="36">
+      <c r="V6" s="36">
         <f>[3]Main!$D$30</f>
         <v>44378</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W6" s="4">
         <f>[3]Main!$C$23</f>
         <v>1932</v>
       </c>
-      <c r="X5" s="4" t="str">
+      <c r="X6" s="4" t="str">
         <f>[3]Main!$C$24</f>
         <v>Seattle, WA</v>
       </c>
-      <c r="Y5" s="4"/>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B6" s="25" t="s">
+      <c r="Y6" s="4"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="28">
         <f>[4]Main!$C$6</f>
         <v>3.54</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G7" s="26">
         <f>[4]Main!$C$7</f>
         <v>758</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H7" s="26">
         <f>[4]Main!$C$8</f>
         <v>2683.32</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I7" s="26">
         <f>[4]Main!$C$11</f>
         <v>478</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J7" s="26">
         <f>[4]Main!$C$12</f>
         <v>2205.3200000000002</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L7" s="22">
         <f>'[4]Financial Model'!$I$31</f>
         <v>2.4699599465954607E-2</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="O6" s="4">
+      <c r="M7" s="4"/>
+      <c r="O7" s="4">
         <v>310</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P7" s="4">
         <v>106</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q7" s="4">
         <v>136</v>
       </c>
-      <c r="S6" s="35">
+      <c r="S7" s="35">
         <f>[4]Main!$C$37</f>
         <v>1.0939180327868854</v>
       </c>
-      <c r="U6" s="4" t="str">
+      <c r="U7" s="4" t="str">
         <f>[4]Main!$C$31</f>
         <v>H122</v>
       </c>
-      <c r="V6" s="36">
+      <c r="V7" s="36">
         <f>[4]Main!$D$31</f>
         <v>44700</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W7" s="4">
         <f>[4]Main!$C$28</f>
         <v>1995</v>
       </c>
-      <c r="X6" s="4" t="str">
+      <c r="X7" s="4" t="str">
         <f>[4]Main!$C$27</f>
         <v>Luton, UK</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y7" s="4">
         <f>[4]Main!$C$29</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B7" s="25" t="s">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B8" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="28">
         <f>[5]Main!$C$6</f>
         <v>10.029999999999999</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G8" s="26">
         <f>[5]Main!$C$7</f>
         <v>214.62</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H8" s="26">
         <f>[5]Main!$C$8</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I8" s="26">
         <f>[5]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J8" s="26">
         <f>[5]Main!$C$12</f>
         <v>2152.6385999999998</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="O7" s="4">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="O8" s="4">
         <v>96</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P8" s="4">
         <v>57</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q8" s="4">
         <v>82</v>
       </c>
-      <c r="S7" s="4"/>
-      <c r="W7" s="4">
+      <c r="S8" s="4"/>
+      <c r="W8" s="4">
         <f>[5]Main!$C$28</f>
         <v>1971</v>
       </c>
-      <c r="X7" s="4" t="str">
+      <c r="X8" s="4" t="str">
         <f>[5]Main!$C$27</f>
         <v>Leeds, UK</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y8" s="4">
         <f>[5]Main!$C$29</f>
         <v>1988</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B8" s="25" t="s">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B9" s="25" t="s">
         <v>438</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F9" s="28">
         <f>[6]Main!$C$6*H22</f>
         <v>25.053599999999999</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G9" s="26">
         <f>[6]Main!$C$7</f>
         <v>73.998000000000005</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H9" s="26">
         <f>[6]Main!$C$8*H22</f>
         <v>1853.9162928000003</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I9" s="26">
         <f>[6]Main!$C$11*H22</f>
         <v>-1157.33816</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J9" s="26">
         <f>[6]Main!$C$12*H22</f>
         <v>3011.2544528000003</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L9" s="22">
         <f>'[6]Financial Model'!$U$37</f>
         <v>0.33604299344574362</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O9" s="4">
         <f>[6]Main!$D$23</f>
         <v>117</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P9" s="4">
         <f>[6]Main!$D$24</f>
         <v>2</v>
       </c>
-      <c r="Q8" s="4" t="str">
+      <c r="Q9" s="4" t="str">
         <f>[6]Main!$D$25</f>
         <v>N/A</v>
       </c>
-      <c r="S8" s="35">
+      <c r="S9" s="35">
         <f>[6]Main!$C$38</f>
         <v>1.4375141996217067</v>
       </c>
-      <c r="U8" s="4" t="str">
+      <c r="U9" s="4" t="str">
         <f>[6]Main!$C$33</f>
         <v>Q322</v>
       </c>
-      <c r="V8" s="36">
+      <c r="V9" s="36">
         <f>[6]Main!$D$33</f>
         <v>44868</v>
       </c>
-      <c r="W8" s="4">
+      <c r="W9" s="4">
         <f>[6]Main!$C$30</f>
         <v>1980</v>
       </c>
-      <c r="X8" s="4" t="str">
+      <c r="X9" s="4" t="str">
         <f>[6]Main!$C$29</f>
         <v>Wilmington, OH</v>
       </c>
-      <c r="Y8" s="4">
+      <c r="Y9" s="4">
         <f>[6]Main!$C$31</f>
         <v>2003</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B9" s="25" t="s">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="28">
         <f>[7]Main!$C$6</f>
         <v>17.350000000000001</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G10" s="26">
         <f>[7]Main!$C$7</f>
         <v>103.7</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H10" s="26">
         <f>[7]Main!$C$8</f>
         <v>1799.1950000000002</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I10" s="26">
         <f>[7]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J10" s="26">
         <f>[7]Main!$C$12</f>
         <v>1799.1950000000002</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L10" s="22">
         <f>'[7]Financial Model'!$L$25</f>
         <v>0.47730688307784791</v>
       </c>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="4">
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="4">
         <f>[7]Main!$D$21</f>
         <v>0</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P10" s="4">
         <f>[7]Main!$D$22</f>
         <v>153</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="W9" s="4">
+      <c r="Q10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="W10" s="4">
         <f>[7]Main!$C$29</f>
         <v>2003</v>
       </c>
-      <c r="X9" s="4" t="str">
+      <c r="X10" s="4" t="str">
         <f>[7]Main!$C$28</f>
         <v>Budapest, Hungary</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y10" s="4">
         <f>[7]Main!$C$30</f>
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B10" s="25"/>
-      <c r="E10" s="4"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="S10" s="4"/>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B11" s="25"/>
+      <c r="E11" s="4"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="Q11" s="4"/>
       <c r="S11" s="4"/>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="H12" s="31"/>
-      <c r="K12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="O12" s="4">
-        <v>130</v>
-      </c>
-      <c r="P12" s="4">
-        <v>44</v>
-      </c>
-      <c r="Q12" s="4"/>
-      <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B13" s="33">
-        <v>753</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>399</v>
       </c>
       <c r="H13" s="31"/>
       <c r="K13" s="1" t="s">
-        <v>608</v>
+        <v>24</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
+      <c r="O13" s="4">
+        <v>130</v>
+      </c>
+      <c r="P13" s="4">
+        <v>44</v>
+      </c>
       <c r="Q13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.15">
-      <c r="B14" s="1" t="s">
-        <v>382</v>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B14" s="33">
+        <v>753</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F14" s="1">
-        <v>40.14</v>
-      </c>
-      <c r="H14" s="32">
-        <f>(F14*H22)*592.96</f>
-        <v>20945.244672000001</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="H14" s="31"/>
       <c r="K14" s="1" t="s">
-        <v>397</v>
+        <v>608</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
+      <c r="Q14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>383</v>
       </c>
       <c r="F15" s="1">
-        <v>76.38</v>
+        <v>40.14</v>
       </c>
       <c r="H15" s="32">
-        <f>(F15*H22)*226.92</f>
-        <v>15252.291647999999</v>
+        <f>(F15*H22)*592.96</f>
+        <v>20945.244672000001</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="S15" s="4"/>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B16" s="29">
         <v>9201</v>
       </c>
@@ -8729,7 +8794,7 @@
       <c r="L16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>385</v>
       </c>
@@ -8756,7 +8821,7 @@
       <c r="M17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>400</v>
       </c>
@@ -8774,60 +8839,60 @@
       </c>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="H19" s="32"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D21" s="1"/>
-      <c r="F21" s="45" t="s">
+      <c r="F21" s="44" t="s">
         <v>378</v>
       </c>
-      <c r="G21" s="46"/>
-      <c r="H21" s="47"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
-      <c r="F22" s="43" t="s">
+      <c r="F22" s="42" t="s">
         <v>379</v>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="43"/>
       <c r="H22" s="23">
         <v>0.88</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="F23" s="43" t="s">
+      <c r="F23" s="42" t="s">
         <v>380</v>
       </c>
-      <c r="G23" s="44"/>
+      <c r="G23" s="43"/>
       <c r="H23" s="23">
         <v>0.85</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
-      <c r="F24" s="43" t="s">
+      <c r="F24" s="42" t="s">
         <v>391</v>
       </c>
-      <c r="G24" s="44"/>
+      <c r="G24" s="43"/>
       <c r="H24" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="F25" s="41" t="s">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="F25" s="40" t="s">
         <v>435</v>
       </c>
-      <c r="G25" s="42"/>
+      <c r="G25" s="41"/>
       <c r="H25" s="24">
         <v>1.0999999999999999E-2</v>
       </c>
@@ -8837,23 +8902,24 @@
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q12"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="F23:G23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{176C962A-9F96-4539-8149-82E34F7BBB40}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{56F8AAB4-AB88-4816-A70A-66823F4EBD86}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{593208B0-BF4C-4E7C-9DA3-9FABEC41EED7}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{5BD026C6-209C-4F8D-96F9-0D20474E4F7F}"/>
-    <hyperlink ref="B3" r:id="rId6" xr:uid="{28605697-2E3F-4D0E-BA6A-013F294DB301}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{7F471098-FF05-4C1A-AA9F-8A6A66E1327B}"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{176C962A-9F96-4539-8149-82E34F7BBB40}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{56F8AAB4-AB88-4816-A70A-66823F4EBD86}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{593208B0-BF4C-4E7C-9DA3-9FABEC41EED7}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{5BD026C6-209C-4F8D-96F9-0D20474E4F7F}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{28605697-2E3F-4D0E-BA6A-013F294DB301}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{7F471098-FF05-4C1A-AA9F-8A6A66E1327B}"/>
+    <hyperlink ref="B3" r:id="rId8" xr:uid="{340E3559-5E25-4E5A-9CCF-84716432B315}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId8"/>
-  <legacyDrawing r:id="rId9"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -8868,24 +8934,24 @@
       <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1"/>
-    <col min="7" max="7" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1"/>
-    <col min="10" max="10" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="1"/>
-    <col min="12" max="12" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>403</v>
       </c>
@@ -8920,7 +8986,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>407</v>
       </c>
@@ -8949,7 +9015,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>412</v>
       </c>
@@ -8981,7 +9047,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>420</v>
       </c>

</xml_diff>

<commit_message>
Add average fleet ages
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723351C2-F5CF-4ADD-970D-A0D8AC0A4C15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460D2B0B-7CE1-45F7-A68E-A8FA281F98F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
+    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="3" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
   <sheets>
     <sheet name="Airlines Screening" sheetId="2" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="614">
   <si>
     <t>Ticker</t>
   </si>
@@ -2141,6 +2141,15 @@
   </si>
   <si>
     <t>IPO</t>
+  </si>
+  <si>
+    <t>Avg Age</t>
+  </si>
+  <si>
+    <t>Fleet Age</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -2154,9 +2163,9 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;0&quot;#"/>
     <numFmt numFmtId="168" formatCode="0.0\x"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2273,6 +2282,12 @@
       <i/>
       <sz val="10"/>
       <color theme="8" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2409,7 +2424,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2482,6 +2497,28 @@
     <xf numFmtId="168" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2494,22 +2531,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2530,6 +2557,57 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>69.05</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>227.43</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>15704.041499999999</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>Dublin, Ireland</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>1984</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32">
+            <v>1997</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2583,7 +2661,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2617,6 +2695,9 @@
           <cell r="C12">
             <v>5543.5049999999992</v>
           </cell>
+          <cell r="V12">
+            <v>13.233333333333334</v>
+          </cell>
         </row>
         <row r="27">
           <cell r="C27" t="str">
@@ -2641,7 +2722,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2711,7 +2792,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2788,7 +2869,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2846,7 +2927,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2936,7 +3017,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2971,6 +3052,9 @@
             <v>1799.1950000000002</v>
           </cell>
         </row>
+        <row r="21">
+          <cell r="D21"/>
+        </row>
         <row r="22">
           <cell r="D22">
             <v>153</v>
@@ -3000,57 +3084,6 @@
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Financial Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>69.05</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>227.43</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>15704.041499999999</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30" t="str">
-            <v>Dublin, Ireland</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>1984</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>1997</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8042,13 +8075,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:Y25"/>
+  <dimension ref="B1:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8067,30 +8100,35 @@
     <col min="16" max="16" width="13.375" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="8.875" style="1"/>
-    <col min="21" max="22" width="8.875" style="4"/>
-    <col min="23" max="23" width="8.875" style="1"/>
-    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.875" style="1"/>
+    <col min="19" max="19" width="9.875" style="1" customWidth="1"/>
+    <col min="20" max="21" width="8.875" style="1"/>
+    <col min="22" max="23" width="8.875" style="4"/>
+    <col min="24" max="24" width="8.875" style="1"/>
+    <col min="25" max="25" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:26" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="53" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="S1" s="39">
-        <f>AVERAGE(S4:S10)</f>
+      <c r="S1" s="43">
+        <f>AVERAGE(S3:S10)</f>
+        <v>10.144047619047617</v>
+      </c>
+      <c r="T1" s="39">
+        <f>AVERAGE(T4:T10)</f>
         <v>1.3082569747231938</v>
       </c>
     </row>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8143,25 +8181,28 @@
         <v>437</v>
       </c>
       <c r="S2" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>384</v>
       </c>
@@ -8175,23 +8216,23 @@
         <v>383</v>
       </c>
       <c r="F3" s="28">
-        <f>[8]Main!$C$6*H22</f>
+        <f>[1]Main!$C$6*H22</f>
         <v>60.763999999999996</v>
       </c>
       <c r="G3" s="26">
-        <f>[8]Main!$C$7</f>
+        <f>[1]Main!$C$7</f>
         <v>227.43</v>
       </c>
       <c r="H3" s="26">
-        <f>[8]Main!$C$12*H22</f>
+        <f>[1]Main!$C$12*H22</f>
         <v>13819.55652</v>
       </c>
-      <c r="I3" s="49">
-        <f>[8]Main!$C$11*H22</f>
+      <c r="I3" s="40">
+        <f>[1]Main!$C$11*H22</f>
         <v>0</v>
       </c>
       <c r="J3" s="26">
-        <f>[8]Main!$C$12*H22</f>
+        <f>[1]Main!$C$12*H22</f>
         <v>13819.55652</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -8199,21 +8240,25 @@
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="W3" s="4">
-        <f>[8]Main!$C$31</f>
+      <c r="S3" s="41">
+        <f>AVERAGE(12.8,4.6,11.7)</f>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="T3" s="4"/>
+      <c r="X3" s="4">
+        <f>[1]Main!$C$31</f>
         <v>1984</v>
       </c>
-      <c r="X3" s="4" t="str">
-        <f>[8]Main!$C$30</f>
+      <c r="Y3" s="4" t="str">
+        <f>[1]Main!$C$30</f>
         <v>Dublin, Ireland</v>
       </c>
-      <c r="Y3" s="4">
-        <f>[8]Main!$C$32</f>
+      <c r="Z3" s="4">
+        <f>[1]Main!$C$32</f>
         <v>1997</v>
       </c>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
         <v>433</v>
       </c>
@@ -8227,23 +8272,23 @@
         <v>434</v>
       </c>
       <c r="F4" s="28">
-        <f>[1]Main!$C$6*H25</f>
+        <f>[2]Main!$C$6*H25</f>
         <v>19.570099999999996</v>
       </c>
       <c r="G4" s="26">
-        <f>[1]Main!$C$7</f>
+        <f>[2]Main!$C$7</f>
         <v>385.26</v>
       </c>
       <c r="H4" s="26">
-        <f>[1]Main!$C$8*H25</f>
+        <f>[2]Main!$C$8*H25</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="I4" s="26">
-        <f>[1]Main!$C$11*H25</f>
+        <f>[2]Main!$C$11*H25</f>
         <v>0</v>
       </c>
       <c r="J4" s="26">
-        <f>[1]Main!$C$12*H25</f>
+        <f>[2]Main!$C$12*H25</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -8252,21 +8297,24 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="W4" s="4">
-        <f>[1]Main!$C$25</f>
+      <c r="S4" s="4">
+        <v>10.7</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="X4" s="4">
+        <f>[2]Main!$C$25</f>
         <v>2005</v>
       </c>
-      <c r="X4" s="4" t="str">
-        <f>[1]Main!$C$24</f>
+      <c r="Y4" s="4" t="str">
+        <f>[2]Main!$C$24</f>
         <v>Gurgaon, India</v>
       </c>
-      <c r="Y4" s="4">
-        <f>[1]Main!$C$26</f>
+      <c r="Z4" s="4">
+        <f>[2]Main!$C$26</f>
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B5" s="25" t="s">
         <v>12</v>
       </c>
@@ -8280,23 +8328,23 @@
         <v>377</v>
       </c>
       <c r="F5" s="28">
-        <f>[2]Main!$C$6</f>
+        <f>[3]Main!$C$6</f>
         <v>1.1198999999999999</v>
       </c>
       <c r="G5" s="26">
-        <f>[2]Main!$C$7</f>
+        <f>[3]Main!$C$7</f>
         <v>4950</v>
       </c>
       <c r="H5" s="26">
-        <f>[2]Main!$C$8</f>
+        <f>[3]Main!$C$8</f>
         <v>5543.5049999999992</v>
       </c>
       <c r="I5" s="26">
-        <f>[2]Main!$C$11</f>
+        <f>[3]Main!$C$11</f>
         <v>0</v>
       </c>
       <c r="J5" s="26">
-        <f>[2]Main!$C$12</f>
+        <f>[3]Main!$C$12</f>
         <v>5543.5049999999992</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -8310,21 +8358,25 @@
       <c r="Q5" s="4">
         <v>200</v>
       </c>
-      <c r="S5" s="4"/>
-      <c r="W5" s="4">
-        <f>[2]Main!$C$28</f>
+      <c r="S5" s="42">
+        <f>[3]Main!$V$12</f>
+        <v>13.233333333333334</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="X5" s="4">
+        <f>[3]Main!$C$28</f>
         <v>2011</v>
       </c>
-      <c r="X5" s="4" t="str">
-        <f>[2]Main!$C$27</f>
+      <c r="Y5" s="4" t="str">
+        <f>[3]Main!$C$27</f>
         <v>London/Madrid</v>
       </c>
-      <c r="Y5" s="4">
-        <f>[2]Main!$C$29</f>
+      <c r="Z5" s="4">
+        <f>[3]Main!$C$29</f>
         <v>2011</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B6" s="25" t="s">
         <v>425</v>
       </c>
@@ -8338,57 +8390,60 @@
         <v>383</v>
       </c>
       <c r="F6" s="28">
-        <f>[3]Main!$C$6*H22</f>
+        <f>[4]Main!$C$6*H22</f>
         <v>36.810400000000001</v>
       </c>
       <c r="G6" s="26">
-        <f>[3]Main!$C$7</f>
+        <f>[4]Main!$C$7</f>
         <v>126.5</v>
       </c>
       <c r="H6" s="26">
-        <f>[3]Main!$C$8*H22</f>
+        <f>[4]Main!$C$8*H22</f>
         <v>4656.5155999999997</v>
       </c>
       <c r="I6" s="26">
-        <f>[3]Main!$C$11*H22</f>
+        <f>[4]Main!$C$11*H22</f>
         <v>987.36</v>
       </c>
       <c r="J6" s="26">
-        <f>[3]Main!$C$12*H22</f>
+        <f>[4]Main!$C$12*H22</f>
         <v>3669.1556</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>426</v>
       </c>
       <c r="L6" s="22">
-        <f>'[3]Financial Model'!$V$42</f>
+        <f>'[4]Financial Model'!$V$42</f>
         <v>0.26862302483069977</v>
       </c>
       <c r="M6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="S6" s="35">
-        <f>[3]Main!$C$35</f>
+      <c r="S6" s="4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="T6" s="35">
+        <f>[4]Main!$C$35</f>
         <v>1.3933386917609896</v>
       </c>
-      <c r="U6" s="4" t="str">
-        <f>[3]Main!$C$30</f>
+      <c r="V6" s="4" t="str">
+        <f>[4]Main!$C$30</f>
         <v>Q222</v>
       </c>
-      <c r="V6" s="36">
-        <f>[3]Main!$D$30</f>
+      <c r="W6" s="36">
+        <f>[4]Main!$D$30</f>
         <v>44378</v>
       </c>
-      <c r="W6" s="4">
-        <f>[3]Main!$C$23</f>
+      <c r="X6" s="4">
+        <f>[4]Main!$C$23</f>
         <v>1932</v>
       </c>
-      <c r="X6" s="4" t="str">
-        <f>[3]Main!$C$24</f>
+      <c r="Y6" s="4" t="str">
+        <f>[4]Main!$C$24</f>
         <v>Seattle, WA</v>
       </c>
-      <c r="Y6" s="4"/>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Z6" s="4"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="25" t="s">
         <v>11</v>
       </c>
@@ -8402,30 +8457,30 @@
         <v>381</v>
       </c>
       <c r="F7" s="28">
-        <f>[4]Main!$C$6</f>
+        <f>[5]Main!$C$6</f>
         <v>3.54</v>
       </c>
       <c r="G7" s="26">
-        <f>[4]Main!$C$7</f>
+        <f>[5]Main!$C$7</f>
         <v>758</v>
       </c>
       <c r="H7" s="26">
-        <f>[4]Main!$C$8</f>
+        <f>[5]Main!$C$8</f>
         <v>2683.32</v>
       </c>
       <c r="I7" s="26">
-        <f>[4]Main!$C$11</f>
+        <f>[5]Main!$C$11</f>
         <v>478</v>
       </c>
       <c r="J7" s="26">
-        <f>[4]Main!$C$12</f>
+        <f>[5]Main!$C$12</f>
         <v>2205.3200000000002</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>394</v>
       </c>
       <c r="L7" s="22">
-        <f>'[4]Financial Model'!$I$31</f>
+        <f>'[5]Financial Model'!$I$31</f>
         <v>2.4699599465954607E-2</v>
       </c>
       <c r="M7" s="4"/>
@@ -8438,32 +8493,36 @@
       <c r="Q7" s="4">
         <v>136</v>
       </c>
-      <c r="S7" s="35">
-        <f>[4]Main!$C$37</f>
+      <c r="S7" s="4">
+        <f>AVERAGE(10,9.2,7.2)</f>
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="T7" s="35">
+        <f>[5]Main!$C$37</f>
         <v>1.0939180327868854</v>
       </c>
-      <c r="U7" s="4" t="str">
-        <f>[4]Main!$C$31</f>
+      <c r="V7" s="4" t="str">
+        <f>[5]Main!$C$31</f>
         <v>H122</v>
       </c>
-      <c r="V7" s="36">
-        <f>[4]Main!$D$31</f>
+      <c r="W7" s="36">
+        <f>[5]Main!$D$31</f>
         <v>44700</v>
       </c>
-      <c r="W7" s="4">
-        <f>[4]Main!$C$28</f>
+      <c r="X7" s="4">
+        <f>[5]Main!$C$28</f>
         <v>1995</v>
       </c>
-      <c r="X7" s="4" t="str">
-        <f>[4]Main!$C$27</f>
+      <c r="Y7" s="4" t="str">
+        <f>[5]Main!$C$27</f>
         <v>Luton, UK</v>
       </c>
-      <c r="Y7" s="4">
-        <f>[4]Main!$C$29</f>
+      <c r="Z7" s="4">
+        <f>[5]Main!$C$29</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8" s="25" t="s">
         <v>16</v>
       </c>
@@ -8477,23 +8536,23 @@
         <v>381</v>
       </c>
       <c r="F8" s="28">
-        <f>[5]Main!$C$6</f>
+        <f>[6]Main!$C$6</f>
         <v>10.029999999999999</v>
       </c>
       <c r="G8" s="26">
-        <f>[5]Main!$C$7</f>
+        <f>[6]Main!$C$7</f>
         <v>214.62</v>
       </c>
       <c r="H8" s="26">
-        <f>[5]Main!$C$8</f>
+        <f>[6]Main!$C$8</f>
         <v>2152.6385999999998</v>
       </c>
       <c r="I8" s="26">
-        <f>[5]Main!$C$11</f>
+        <f>[6]Main!$C$11</f>
         <v>0</v>
       </c>
       <c r="J8" s="26">
-        <f>[5]Main!$C$12</f>
+        <f>[6]Main!$C$12</f>
         <v>2152.6385999999998</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -8510,21 +8569,24 @@
       <c r="Q8" s="4">
         <v>82</v>
       </c>
-      <c r="S8" s="4"/>
-      <c r="W8" s="4">
-        <f>[5]Main!$C$28</f>
+      <c r="S8" s="44">
+        <v>15.3</v>
+      </c>
+      <c r="T8" s="4"/>
+      <c r="X8" s="4">
+        <f>[6]Main!$C$28</f>
         <v>1971</v>
       </c>
-      <c r="X8" s="4" t="str">
-        <f>[5]Main!$C$27</f>
+      <c r="Y8" s="4" t="str">
+        <f>[6]Main!$C$27</f>
         <v>Leeds, UK</v>
       </c>
-      <c r="Y8" s="4">
-        <f>[5]Main!$C$29</f>
+      <c r="Z8" s="4">
+        <f>[6]Main!$C$29</f>
         <v>1988</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" s="25" t="s">
         <v>438</v>
       </c>
@@ -8538,70 +8600,71 @@
         <v>383</v>
       </c>
       <c r="F9" s="28">
-        <f>[6]Main!$C$6*H22</f>
+        <f>[7]Main!$C$6*H22</f>
         <v>25.053599999999999</v>
       </c>
       <c r="G9" s="26">
-        <f>[6]Main!$C$7</f>
+        <f>[7]Main!$C$7</f>
         <v>73.998000000000005</v>
       </c>
       <c r="H9" s="26">
-        <f>[6]Main!$C$8*H22</f>
+        <f>[7]Main!$C$8*H22</f>
         <v>1853.9162928000003</v>
       </c>
       <c r="I9" s="26">
-        <f>[6]Main!$C$11*H22</f>
+        <f>[7]Main!$C$11*H22</f>
         <v>-1157.33816</v>
       </c>
       <c r="J9" s="26">
-        <f>[6]Main!$C$12*H22</f>
+        <f>[7]Main!$C$12*H22</f>
         <v>3011.2544528000003</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>609</v>
       </c>
       <c r="L9" s="22">
-        <f>'[6]Financial Model'!$U$37</f>
+        <f>'[7]Financial Model'!$U$37</f>
         <v>0.33604299344574362</v>
       </c>
       <c r="O9" s="4">
-        <f>[6]Main!$D$23</f>
+        <f>[7]Main!$D$23</f>
         <v>117</v>
       </c>
       <c r="P9" s="4">
-        <f>[6]Main!$D$24</f>
+        <f>[7]Main!$D$24</f>
         <v>2</v>
       </c>
       <c r="Q9" s="4" t="str">
-        <f>[6]Main!$D$25</f>
+        <f>[7]Main!$D$25</f>
         <v>N/A</v>
       </c>
-      <c r="S9" s="35">
-        <f>[6]Main!$C$38</f>
+      <c r="S9" s="4"/>
+      <c r="T9" s="35">
+        <f>[7]Main!$C$38</f>
         <v>1.4375141996217067</v>
       </c>
-      <c r="U9" s="4" t="str">
-        <f>[6]Main!$C$33</f>
+      <c r="V9" s="4" t="str">
+        <f>[7]Main!$C$33</f>
         <v>Q322</v>
       </c>
-      <c r="V9" s="36">
-        <f>[6]Main!$D$33</f>
+      <c r="W9" s="36">
+        <f>[7]Main!$D$33</f>
         <v>44868</v>
       </c>
-      <c r="W9" s="4">
-        <f>[6]Main!$C$30</f>
+      <c r="X9" s="4">
+        <f>[7]Main!$C$30</f>
         <v>1980</v>
       </c>
-      <c r="X9" s="4" t="str">
-        <f>[6]Main!$C$29</f>
+      <c r="Y9" s="4" t="str">
+        <f>[7]Main!$C$29</f>
         <v>Wilmington, OH</v>
       </c>
-      <c r="Y9" s="4">
-        <f>[6]Main!$C$31</f>
+      <c r="Z9" s="4">
+        <f>[7]Main!$C$31</f>
         <v>2003</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B10" s="25" t="s">
         <v>10</v>
       </c>
@@ -8615,58 +8678,62 @@
         <v>377</v>
       </c>
       <c r="F10" s="28">
-        <f>[7]Main!$C$6</f>
+        <f>[8]Main!$C$6</f>
         <v>17.350000000000001</v>
       </c>
       <c r="G10" s="26">
-        <f>[7]Main!$C$7</f>
+        <f>[8]Main!$C$7</f>
         <v>103.7</v>
       </c>
       <c r="H10" s="26">
-        <f>[7]Main!$C$8</f>
+        <f>[8]Main!$C$8</f>
         <v>1799.1950000000002</v>
       </c>
       <c r="I10" s="26">
-        <f>[7]Main!$C$11</f>
+        <f>[8]Main!$C$11</f>
         <v>0</v>
       </c>
       <c r="J10" s="26">
-        <f>[7]Main!$C$12</f>
+        <f>[8]Main!$C$12</f>
         <v>1799.1950000000002</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L10" s="22">
-        <f>'[7]Financial Model'!$L$25</f>
+        <f>'[8]Financial Model'!$L$25</f>
         <v>0.47730688307784791</v>
       </c>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
       <c r="O10" s="4">
-        <f>[7]Main!$D$21</f>
+        <f>[8]Main!$D$21</f>
         <v>0</v>
       </c>
       <c r="P10" s="4">
-        <f>[7]Main!$D$22</f>
+        <f>[8]Main!$D$22</f>
         <v>153</v>
       </c>
       <c r="Q10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="W10" s="4">
-        <f>[7]Main!$C$29</f>
+      <c r="S10" s="42">
+        <f>AVERAGE(5.2,3.7,0.7,2.7)</f>
+        <v>3.0750000000000002</v>
+      </c>
+      <c r="T10" s="4"/>
+      <c r="X10" s="4">
+        <f>[8]Main!$C$29</f>
         <v>2003</v>
       </c>
-      <c r="X10" s="4" t="str">
-        <f>[7]Main!$C$28</f>
+      <c r="Y10" s="4" t="str">
+        <f>[8]Main!$C$28</f>
         <v>Budapest, Hungary</v>
       </c>
-      <c r="Y10" s="4">
-        <f>[7]Main!$C$30</f>
+      <c r="Z10" s="4">
+        <f>[8]Main!$C$30</f>
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B11" s="25"/>
       <c r="E11" s="4"/>
       <c r="H11" s="28"/>
@@ -8675,28 +8742,28 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="S11" s="4"/>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
-      <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="T11" s="4"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
@@ -8719,9 +8786,9 @@
         <v>44</v>
       </c>
       <c r="Q13" s="4"/>
-      <c r="S13" s="4"/>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B14" s="33">
         <v>753</v>
       </c>
@@ -8738,9 +8805,9 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>382</v>
       </c>
@@ -8765,9 +8832,9 @@
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="S15" s="4"/>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B16" s="29">
         <v>9201</v>
       </c>
@@ -8792,9 +8859,9 @@
         <v>392</v>
       </c>
       <c r="L16" s="4"/>
-      <c r="S16" s="4"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>385</v>
       </c>
@@ -8819,9 +8886,9 @@
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="S17" s="4"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>400</v>
       </c>
@@ -8837,75 +8904,91 @@
       <c r="K18" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="S18" s="4"/>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="T18" s="4"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="H19" s="32"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D21" s="1"/>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="45" t="s">
         <v>378</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="50" t="s">
         <v>379</v>
       </c>
-      <c r="G22" s="43"/>
+      <c r="G22" s="51"/>
       <c r="H22" s="23">
         <v>0.88</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="F23" s="42" t="s">
+      <c r="F23" s="50" t="s">
         <v>380</v>
       </c>
-      <c r="G23" s="43"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="23">
         <v>0.85</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
-      <c r="F24" s="42" t="s">
+      <c r="F24" s="50" t="s">
         <v>391</v>
       </c>
-      <c r="G24" s="43"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F25" s="40" t="s">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="F25" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="G25" s="41"/>
+      <c r="G25" s="49"/>
       <c r="H25" s="24">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="F28" s="45" t="s">
+        <v>413</v>
+      </c>
+      <c r="G28" s="46"/>
+      <c r="H28" s="47"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>613</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F28:H28"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
@@ -8916,22 +8999,23 @@
     <hyperlink ref="B4" r:id="rId6" xr:uid="{28605697-2E3F-4D0E-BA6A-013F294DB301}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{7F471098-FF05-4C1A-AA9F-8A6A66E1327B}"/>
     <hyperlink ref="B3" r:id="rId8" xr:uid="{340E3559-5E25-4E5A-9CCF-84716432B315}"/>
+    <hyperlink ref="G29" r:id="rId9" xr:uid="{76EE83BD-7400-4A46-978B-D25721A01204}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA0EDE9-69E3-4DB1-A599-3D030985D0D0}">
-  <dimension ref="B2:L5"/>
+  <dimension ref="B1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8946,12 +9030,18 @@
     <col min="8" max="8" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1"/>
     <col min="10" max="10" width="13.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" style="1"/>
-    <col min="12" max="12" width="33.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8" style="1"/>
+    <col min="11" max="12" width="8" style="1"/>
+    <col min="13" max="13" width="33.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="K1" s="43">
+        <f>AVERAGE(K3:K5)</f>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>403</v>
       </c>
@@ -8980,13 +9070,16 @@
         <v>411</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>407</v>
       </c>
@@ -9008,14 +9101,17 @@
       <c r="J3" s="4">
         <v>16</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="K3" s="4">
+        <v>13.9</v>
+      </c>
+      <c r="L3" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>412</v>
       </c>
@@ -9040,14 +9136,17 @@
       <c r="J4" s="4">
         <v>32</v>
       </c>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="L4" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>420</v>
       </c>
@@ -9069,17 +9168,15 @@
       <c r="J5" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="L5" s="34" t="s">
         <v>414</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" display="Link" xr:uid="{705A33A3-71BB-4320-B698-2F78CD2A8AFC}"/>
-    <hyperlink ref="K4" r:id="rId2" xr:uid="{02883213-BF38-4D93-A318-299B713A430A}"/>
-    <hyperlink ref="K5" r:id="rId3" location="Fleet" xr:uid="{31B6035D-A419-4044-A1AE-78B68CC43A46}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Titan Airways (private equity) to Airlines
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC4E1A7-59BA-42BF-A1FD-CDE68A9CC946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3CE161-D1FD-4181-BC77-1D907DE77CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
@@ -27,6 +27,7 @@
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
     <author>me</author>
   </authors>
   <commentList>
-    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{61C10B76-0DAF-064D-AE3B-2214629883F5}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
+    <comment ref="S7" authorId="0" shapeId="0" xr:uid="{3E6B0981-0393-1A4E-86F7-17B4F0F10192}">
       <text>
         <r>
           <rPr>
@@ -70,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
+    <comment ref="T7" authorId="0" shapeId="0" xr:uid="{24C2E0AD-869F-F84E-B5B4-5D117694EC51}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R7" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
+    <comment ref="U7" authorId="0" shapeId="0" xr:uid="{462115FC-9958-DD4B-B923-8CDD5C93BD8C}">
       <text>
         <r>
           <rPr>
@@ -96,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
+    <comment ref="S8" authorId="0" shapeId="0" xr:uid="{A91C8AB2-451C-734F-9F12-C43C68128376}">
       <text>
         <r>
           <rPr>
@@ -109,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
+    <comment ref="T8" authorId="0" shapeId="0" xr:uid="{1EADED05-599C-2443-BAEA-A44BB8B69AF4}">
       <text>
         <r>
           <rPr>
@@ -122,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P9" authorId="1" shapeId="0" xr:uid="{6707E1A1-B9D2-4817-8DE3-181D10B4D7FB}">
+    <comment ref="S9" authorId="1" shapeId="0" xr:uid="{6707E1A1-B9D2-4817-8DE3-181D10B4D7FB}">
       <text>
         <r>
           <rPr>
@@ -146,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q9" authorId="1" shapeId="0" xr:uid="{9CECB1AB-BF64-4D62-80D4-8FDC2F945662}">
+    <comment ref="T9" authorId="1" shapeId="0" xr:uid="{9CECB1AB-BF64-4D62-80D4-8FDC2F945662}">
       <text>
         <r>
           <rPr>
@@ -170,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R9" authorId="1" shapeId="0" xr:uid="{F023898F-9365-4C97-A256-586C010E62F1}">
+    <comment ref="U9" authorId="1" shapeId="0" xr:uid="{F023898F-9365-4C97-A256-586C010E62F1}">
       <text>
         <r>
           <rPr>
@@ -194,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
+    <comment ref="S10" authorId="0" shapeId="0" xr:uid="{90DE1C05-F69E-C543-922A-43B295FED9FB}">
       <text>
         <r>
           <rPr>
@@ -207,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q10" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
+    <comment ref="T10" authorId="0" shapeId="0" xr:uid="{9C186867-46F1-7945-ACDC-7063A2FFD8AD}">
       <text>
         <r>
           <rPr>
@@ -220,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P13" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
+    <comment ref="S13" authorId="0" shapeId="0" xr:uid="{8D311092-A9DA-8243-AF71-951A4751D5E3}">
       <text>
         <r>
           <rPr>
@@ -233,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q13" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
+    <comment ref="T13" authorId="0" shapeId="0" xr:uid="{9DA0DD90-866B-8640-8262-B5FD9B7B259B}">
       <text>
         <r>
           <rPr>
@@ -308,7 +309,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="629">
   <si>
     <t>Ticker</t>
   </si>
@@ -1498,9 +1499,6 @@
     <t>Worlds largest low-cost carrier</t>
   </si>
   <si>
-    <t>(GBP)</t>
-  </si>
-  <si>
     <t>SEHK</t>
   </si>
   <si>
@@ -1576,9 +1574,6 @@
     <t>Long-haul airline</t>
   </si>
   <si>
-    <t xml:space="preserve">Flybe 1979-2020 collapsed in March 2020, brand bought out by Cyrus Capital with a plan to relaunch </t>
-  </si>
-  <si>
     <t>$ALK</t>
   </si>
   <si>
@@ -2153,6 +2148,54 @@
   </si>
   <si>
     <t>PAX 22</t>
+  </si>
+  <si>
+    <t>Hagondale Ltd. (Titan Airways)</t>
+  </si>
+  <si>
+    <t>Charter &amp; Specialist</t>
+  </si>
+  <si>
+    <t>Exeter</t>
+  </si>
+  <si>
+    <t>Flybe 1979-2020 collapsed in March 2020, brand bought out by Cyrus Capital with a plan to relaunch . Collapsed again in January 2023</t>
+  </si>
+  <si>
+    <t>Humberside Airport</t>
+  </si>
+  <si>
+    <t>Stanstead Airport</t>
+  </si>
+  <si>
+    <t>Crawley (Gatwick)</t>
+  </si>
+  <si>
+    <t>Private Equity</t>
+  </si>
+  <si>
+    <t>Titan Airways</t>
+  </si>
+  <si>
+    <t>Hagondale Limited</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>OM %</t>
+  </si>
+  <si>
+    <t>NM %</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>Charter &amp; specialist contract airline based in the UK + Aircraft Leasing</t>
+  </si>
+  <si>
+    <t>(Normalised to GBP)</t>
   </si>
 </sst>
 </file>
@@ -2295,7 +2338,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2329,6 +2372,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2427,7 +2482,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2540,6 +2595,21 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3055,6 +3125,9 @@
             <v>1799.1950000000002</v>
           </cell>
         </row>
+        <row r="21">
+          <cell r="D21"/>
+        </row>
         <row r="22">
           <cell r="D22">
             <v>153</v>
@@ -3083,7 +3156,77 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Accounts"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="13">
+          <cell r="C13" t="str">
+            <v>Stanstead Airport, UK</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14">
+            <v>1988</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17">
+            <v>14.4</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="C18">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20" t="str">
+            <v>FY21/22</v>
+          </cell>
+          <cell r="D20">
+            <v>45141</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="18">
+          <cell r="L18">
+            <v>3.7691802910883844E-2</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="L19">
+            <v>-7.2462158441842464E-2</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="L20">
+            <v>-8.0967153446236284E-2</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="K21">
+            <v>0.18785583230649008</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3461,7 +3604,7 @@
   </sheetPr>
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:L6"/>
     </sheetView>
   </sheetViews>
@@ -6524,22 +6667,22 @@
     </row>
     <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>164</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>440</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>442</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>67</v>
@@ -6560,7 +6703,7 @@
         <v>67</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="N2" s="9">
         <v>1.1000000000000001E-3</v>
@@ -6568,22 +6711,22 @@
     </row>
     <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>67</v>
@@ -6604,7 +6747,7 @@
         <v>67</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="N3" s="11">
         <v>-0.11940000000000001</v>
@@ -6612,22 +6755,22 @@
     </row>
     <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>67</v>
@@ -6639,7 +6782,7 @@
         <v>4.22</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="K4" s="13">
         <v>0.1336</v>
@@ -6656,22 +6799,22 @@
     </row>
     <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G5" s="7">
         <v>7.14</v>
@@ -6683,7 +6826,7 @@
         <v>3.5</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K5" s="9">
         <v>1</v>
@@ -6692,7 +6835,7 @@
         <v>67</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="N5" s="9">
         <v>3.2800000000000003E-2</v>
@@ -6700,19 +6843,19 @@
     </row>
     <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>67</v>
@@ -6727,7 +6870,7 @@
         <v>1.81</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K6" s="13">
         <v>0.17630000000000001</v>
@@ -6736,7 +6879,7 @@
         <v>67</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="N6" s="9">
         <v>4.6100000000000002E-2</v>
@@ -6744,22 +6887,22 @@
     </row>
     <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>164</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G7" s="8">
         <v>138.6</v>
@@ -6771,7 +6914,7 @@
         <v>0.25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K7" s="13">
         <v>0.21</v>
@@ -6780,7 +6923,7 @@
         <v>67</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="N7" s="9">
         <v>5.7999999999999996E-3</v>
@@ -6788,19 +6931,19 @@
     </row>
     <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>67</v>
@@ -6815,7 +6958,7 @@
         <v>0.54</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K8" s="13">
         <v>0.22090000000000001</v>
@@ -6824,7 +6967,7 @@
         <v>67</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="N8" s="9">
         <v>2.46E-2</v>
@@ -6832,22 +6975,22 @@
     </row>
     <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G9" s="8">
         <v>56.34</v>
@@ -6868,7 +7011,7 @@
         <v>67</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N9" s="11">
         <v>-1.5599999999999999E-2</v>
@@ -6879,19 +7022,19 @@
         <v>2588</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G10" s="7">
         <v>9.24</v>
@@ -6903,7 +7046,7 @@
         <v>3.53</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="K10" s="9">
         <v>0.91400000000000003</v>
@@ -6912,7 +7055,7 @@
         <v>44791</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="N10" s="9">
         <v>4.1599999999999998E-2</v>
@@ -6920,22 +7063,22 @@
     </row>
     <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G11" s="8">
         <v>50.5</v>
@@ -6956,7 +7099,7 @@
         <v>67</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="N11" s="9">
         <v>8.3999999999999995E-3</v>
@@ -6964,22 +7107,22 @@
     </row>
     <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>67</v>
@@ -7000,7 +7143,7 @@
         <v>67</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="N12" s="9">
         <v>5.0000000000000001E-4</v>
@@ -7008,16 +7151,16 @@
     </row>
     <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>198</v>
@@ -7035,7 +7178,7 @@
         <v>1.05</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="K13" s="11">
         <v>9.4200000000000006E-2</v>
@@ -7044,7 +7187,7 @@
         <v>67</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="N13" s="9">
         <v>1.5299999999999999E-2</v>
@@ -7052,22 +7195,22 @@
     </row>
     <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>209</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G14" s="7">
         <v>7.1</v>
@@ -7079,7 +7222,7 @@
         <v>1.29</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K14" s="9">
         <v>1</v>
@@ -7088,7 +7231,7 @@
         <v>67</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="N14" s="9">
         <v>1.9E-3</v>
@@ -7096,22 +7239,22 @@
     </row>
     <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>213</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G15" s="7">
         <v>5.96</v>
@@ -7132,7 +7275,7 @@
         <v>67</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="N15" s="9">
         <v>0.1346</v>
@@ -7143,19 +7286,19 @@
         <v>694</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G16" s="7">
         <v>7.55</v>
@@ -7167,7 +7310,7 @@
         <v>0.74</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="K16" s="9">
         <v>0.71799999999999997</v>
@@ -7176,7 +7319,7 @@
         <v>44803</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N16" s="9">
         <v>6.4199999999999993E-2</v>
@@ -7184,22 +7327,22 @@
     </row>
     <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="G17" s="7">
         <v>9.92</v>
@@ -7211,7 +7354,7 @@
         <v>1.47</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K17" s="9">
         <v>0.99850000000000005</v>
@@ -7220,7 +7363,7 @@
         <v>67</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="N17" s="9">
         <v>3.1099999999999999E-2</v>
@@ -7228,19 +7371,19 @@
     </row>
     <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>67</v>
@@ -7255,7 +7398,7 @@
         <v>6.06</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="K18" s="13">
         <v>0.1188</v>
@@ -7264,7 +7407,7 @@
         <v>44882</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="N18" s="11">
         <v>-8.5000000000000006E-3</v>
@@ -7275,19 +7418,19 @@
         <v>357</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G19" s="7">
         <v>11</v>
@@ -7299,7 +7442,7 @@
         <v>1.46</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K19" s="9">
         <v>0.58440000000000003</v>
@@ -7308,7 +7451,7 @@
         <v>44799</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N19" s="9">
         <v>6.8400000000000002E-2</v>
@@ -7316,22 +7459,22 @@
     </row>
     <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="G20" s="7">
         <v>18.05</v>
@@ -7343,7 +7486,7 @@
         <v>0.19</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K20" s="9">
         <v>0.65839999999999999</v>
@@ -7352,7 +7495,7 @@
         <v>44873</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="N20" s="9">
         <v>5.3E-3</v>
@@ -7360,22 +7503,22 @@
     </row>
     <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="G21" s="7">
         <v>0.13</v>
@@ -7396,7 +7539,7 @@
         <v>67</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="N21" s="9">
         <v>0</v>
@@ -7407,16 +7550,16 @@
         <v>1848</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>67</v>
@@ -7431,7 +7574,7 @@
         <v>7.28</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="K22" s="13">
         <v>0.4017</v>
@@ -7440,7 +7583,7 @@
         <v>44862</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="N22" s="11">
         <v>-6.3E-3</v>
@@ -7448,19 +7591,19 @@
     </row>
     <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>67</v>
@@ -7475,7 +7618,7 @@
         <v>67</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="K23" s="11">
         <v>0</v>
@@ -7484,7 +7627,7 @@
         <v>67</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="N23" s="11">
         <v>-0.16120000000000001</v>
@@ -7492,22 +7635,22 @@
     </row>
     <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G24" s="8">
         <v>31.13</v>
@@ -7528,7 +7671,7 @@
         <v>67</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="N24" s="9">
         <v>0</v>
@@ -7536,22 +7679,22 @@
     </row>
     <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>67</v>
@@ -7563,7 +7706,7 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="K25" s="13">
         <v>0.48430000000000001</v>
@@ -7572,7 +7715,7 @@
         <v>44833</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="N25" s="9">
         <v>3.0999999999999999E-3</v>
@@ -7580,22 +7723,22 @@
     </row>
     <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>149</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G26" s="8">
         <v>30.08</v>
@@ -7607,7 +7750,7 @@
         <v>0.9</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="K26" s="11">
         <v>0</v>
@@ -7616,7 +7759,7 @@
         <v>67</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="N26" s="9">
         <v>1.2E-2</v>
@@ -7624,22 +7767,22 @@
     </row>
     <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="G27" s="7">
         <v>0.21</v>
@@ -7651,7 +7794,7 @@
         <v>-3.82</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="K27" s="11">
         <v>2.7000000000000001E-3</v>
@@ -7660,7 +7803,7 @@
         <v>44785</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="N27" s="9">
         <v>3.5700000000000003E-2</v>
@@ -7668,22 +7811,22 @@
     </row>
     <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>149</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>67</v>
@@ -7695,7 +7838,7 @@
         <v>971.61</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="K28" s="11">
         <v>3.5900000000000001E-2</v>
@@ -7704,7 +7847,7 @@
         <v>67</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="N28" s="9">
         <v>2.8500000000000001E-2</v>
@@ -7712,22 +7855,22 @@
     </row>
     <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>67</v>
@@ -7739,7 +7882,7 @@
         <v>3.53</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="K29" s="11">
         <v>5.7099999999999998E-2</v>
@@ -7748,7 +7891,7 @@
         <v>44832</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="N29" s="11">
         <v>-3.8800000000000001E-2</v>
@@ -7759,16 +7902,16 @@
         <v>8620</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F30" s="8" t="e" cm="1" vm="3">
         <f t="array" ref="F30">-_FV(HKD$7,"22")</f>
@@ -7784,7 +7927,7 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="K30" s="11">
         <v>0</v>
@@ -7793,7 +7936,7 @@
         <v>44785</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="N30" s="11">
         <v>-4.4900000000000002E-2</v>
@@ -7801,22 +7944,22 @@
     </row>
     <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>67</v>
@@ -7828,7 +7971,7 @@
         <v>15.56</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="K31" s="11">
         <v>0</v>
@@ -7837,7 +7980,7 @@
         <v>44874</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="N31" s="9">
         <v>2.63E-2</v>
@@ -7845,22 +7988,22 @@
     </row>
     <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>149</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>67</v>
@@ -7872,7 +8015,7 @@
         <v>9.19</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K32" s="11">
         <v>0</v>
@@ -7881,7 +8024,7 @@
         <v>67</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="N32" s="9">
         <v>2.3699999999999999E-2</v>
@@ -7889,19 +8032,19 @@
     </row>
     <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>67</v>
@@ -7933,22 +8076,22 @@
     </row>
     <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>355</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="G34" s="8">
         <v>69.41</v>
@@ -7969,7 +8112,7 @@
         <v>67</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="N34" s="11">
         <v>-1.8599999999999998E-2</v>
@@ -7977,16 +8120,16 @@
     </row>
     <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>67</v>
@@ -8013,7 +8156,7 @@
         <v>67</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="N35" s="9">
         <v>49.000100000000003</v>
@@ -8075,19 +8218,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:AA29"/>
+  <dimension ref="B1:AD34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12:R25"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="1"/>
+    <col min="2" max="2" width="11.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.875" style="4"/>
     <col min="5" max="5" width="8.875" style="1"/>
@@ -8095,40 +8238,40 @@
     <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
     <col min="8" max="10" width="8.875" style="1"/>
     <col min="11" max="11" width="65.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="8.875" style="1"/>
-    <col min="16" max="16" width="10.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.875" style="1" customWidth="1"/>
-    <col min="21" max="22" width="8.875" style="1"/>
-    <col min="23" max="24" width="8.875" style="4"/>
-    <col min="25" max="25" width="8.875" style="1"/>
-    <col min="26" max="26" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.875" style="1"/>
+    <col min="12" max="18" width="8.875" style="1"/>
+    <col min="19" max="19" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.875" style="1" customWidth="1"/>
+    <col min="24" max="25" width="8.875" style="1"/>
+    <col min="26" max="27" width="8.875" style="4"/>
+    <col min="28" max="28" width="8.875" style="1"/>
+    <col min="29" max="29" width="16.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="F1" s="45" t="s">
-        <v>396</v>
+        <v>628</v>
       </c>
       <c r="G1" s="45"/>
       <c r="H1" s="45"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="T1" s="43">
-        <f>AVERAGE(T3:T10)</f>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="W1" s="43">
+        <f>AVERAGE(W3:W10)</f>
         <v>10.144047619047617</v>
       </c>
-      <c r="U1" s="39">
-        <f>AVERAGE(U4:U10)</f>
+      <c r="X1" s="39">
+        <f>AVERAGE(X4:X10)</f>
         <v>1.3082569747231938</v>
       </c>
     </row>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8145,7 +8288,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>5</v>
@@ -8163,49 +8306,58 @@
         <v>9</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>613</v>
+        <v>625</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="Q2" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AB2" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>384</v>
       </c>
@@ -8219,7 +8371,7 @@
         <v>383</v>
       </c>
       <c r="F3" s="28">
-        <f>[1]Main!$C$6*H22</f>
+        <f>[1]Main!$C$6*H27</f>
         <v>58.001999999999995</v>
       </c>
       <c r="G3" s="26">
@@ -8227,15 +8379,15 @@
         <v>227.43</v>
       </c>
       <c r="H3" s="26">
-        <f>[1]Main!$C$12*H22</f>
+        <f>[1]Main!$C$12*H27</f>
         <v>13191.394859999999</v>
       </c>
       <c r="I3" s="40">
-        <f>[1]Main!$C$11*H22</f>
+        <f>[1]Main!$C$11*H27</f>
         <v>0</v>
       </c>
       <c r="J3" s="26">
-        <f>[1]Main!$C$12*H22</f>
+        <f>[1]Main!$C$12*H27</f>
         <v>13191.394859999999</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -8244,39 +8396,42 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="T3" s="41">
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="W3" s="41">
         <f>AVERAGE(12.8,4.6,11.7)</f>
         <v>9.6999999999999993</v>
       </c>
-      <c r="U3" s="4"/>
-      <c r="Y3" s="4">
+      <c r="X3" s="4"/>
+      <c r="AB3" s="4">
         <f>[1]Main!$C$31</f>
         <v>1984</v>
       </c>
-      <c r="Z3" s="4" t="str">
+      <c r="AC3" s="4" t="str">
         <f>[1]Main!$C$30</f>
         <v>Dublin, Ireland</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="AD3" s="4">
         <f>[1]Main!$C$32</f>
         <v>1997</v>
       </c>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F4" s="28">
-        <f>[2]Main!$C$6*H25</f>
+        <f>[2]Main!$C$6*H30</f>
         <v>19.570099999999996</v>
       </c>
       <c r="G4" s="26">
@@ -8284,42 +8439,45 @@
         <v>385.26</v>
       </c>
       <c r="H4" s="26">
-        <f>[2]Main!$C$8*H25</f>
+        <f>[2]Main!$C$8*H30</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="I4" s="26">
-        <f>[2]Main!$C$11*H25</f>
+        <f>[2]Main!$C$11*H30</f>
         <v>0</v>
       </c>
       <c r="J4" s="26">
-        <f>[2]Main!$C$12*H25</f>
+        <f>[2]Main!$C$12*H30</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="T4" s="4">
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="W4" s="4">
         <v>10.7</v>
       </c>
-      <c r="U4" s="4"/>
-      <c r="Y4" s="4">
+      <c r="X4" s="4"/>
+      <c r="AB4" s="4">
         <f>[2]Main!$C$25</f>
         <v>2005</v>
       </c>
-      <c r="Z4" s="4" t="str">
+      <c r="AC4" s="4" t="str">
         <f>[2]Main!$C$24</f>
         <v>Gurgaon, India</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AD4" s="4">
         <f>[2]Main!$C$26</f>
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B5" s="25" t="s">
         <v>12</v>
       </c>
@@ -8358,36 +8516,39 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="P5" s="4">
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="S5" s="4">
         <v>531</v>
       </c>
-      <c r="R5" s="4">
+      <c r="U5" s="4">
         <v>200</v>
       </c>
-      <c r="T5" s="42">
+      <c r="W5" s="42">
         <f>[3]Main!$V$12</f>
         <v>13.233333333333334</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="Y5" s="4">
+      <c r="X5" s="4"/>
+      <c r="AB5" s="4">
         <f>[3]Main!$C$28</f>
         <v>2011</v>
       </c>
-      <c r="Z5" s="4" t="str">
+      <c r="AC5" s="4" t="str">
         <f>[3]Main!$C$27</f>
         <v>London/Madrid</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AD5" s="4">
         <f>[3]Main!$C$29</f>
         <v>2011</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B6" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>425</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>42</v>
@@ -8396,7 +8557,7 @@
         <v>383</v>
       </c>
       <c r="F6" s="28">
-        <f>[4]Main!$C$6*H22</f>
+        <f>[4]Main!$C$6*H27</f>
         <v>35.1372</v>
       </c>
       <c r="G6" s="26">
@@ -8404,53 +8565,56 @@
         <v>126.5</v>
       </c>
       <c r="H6" s="26">
-        <f>[4]Main!$C$8*H22</f>
+        <f>[4]Main!$C$8*H27</f>
         <v>4444.8557999999994</v>
       </c>
       <c r="I6" s="26">
-        <f>[4]Main!$C$11*H22</f>
+        <f>[4]Main!$C$11*H27</f>
         <v>942.48</v>
       </c>
       <c r="J6" s="26">
-        <f>[4]Main!$C$12*H22</f>
+        <f>[4]Main!$C$12*H27</f>
         <v>3502.3757999999998</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="L6" s="22">
         <f>'[4]Financial Model'!$V$42</f>
         <v>0.26862302483069977</v>
       </c>
       <c r="M6" s="22"/>
-      <c r="N6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="T6" s="4">
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="W6" s="4">
         <v>10.199999999999999</v>
       </c>
-      <c r="U6" s="35">
+      <c r="X6" s="35">
         <f>[4]Main!$C$35</f>
         <v>1.3933386917609896</v>
       </c>
-      <c r="W6" s="4" t="str">
+      <c r="Z6" s="4" t="str">
         <f>[4]Main!$C$30</f>
         <v>Q222</v>
       </c>
-      <c r="X6" s="36">
+      <c r="AA6" s="36">
         <f>[4]Main!$D$30</f>
         <v>44378</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="AB6" s="4">
         <f>[4]Main!$C$23</f>
         <v>1932</v>
       </c>
-      <c r="Z6" s="4" t="str">
+      <c r="AC6" s="4" t="str">
         <f>[4]Main!$C$24</f>
         <v>Seattle, WA</v>
       </c>
-      <c r="AA6" s="4"/>
-    </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AD6" s="4"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B7" s="25" t="s">
         <v>11</v>
       </c>
@@ -8491,46 +8655,49 @@
         <v>2.4699599465954607E-2</v>
       </c>
       <c r="M7" s="22"/>
-      <c r="N7" s="4"/>
-      <c r="P7" s="4">
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="4"/>
+      <c r="S7" s="4">
         <v>310</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="T7" s="4">
         <v>106</v>
       </c>
-      <c r="R7" s="4">
+      <c r="U7" s="4">
         <v>136</v>
       </c>
-      <c r="T7" s="4">
+      <c r="W7" s="4">
         <f>AVERAGE(10,9.2,7.2)</f>
         <v>8.7999999999999989</v>
       </c>
-      <c r="U7" s="35">
+      <c r="X7" s="35">
         <f>[5]Main!$C$37</f>
         <v>1.0939180327868854</v>
       </c>
-      <c r="W7" s="4" t="str">
+      <c r="Z7" s="4" t="str">
         <f>[5]Main!$C$31</f>
         <v>H122</v>
       </c>
-      <c r="X7" s="36">
+      <c r="AA7" s="36">
         <f>[5]Main!$D$31</f>
         <v>44700</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="AB7" s="4">
         <f>[5]Main!$C$28</f>
         <v>1995</v>
       </c>
-      <c r="Z7" s="4" t="str">
+      <c r="AC7" s="4" t="str">
         <f>[5]Main!$C$27</f>
         <v>Luton, UK</v>
       </c>
-      <c r="AA7" s="4">
+      <c r="AD7" s="4">
         <f>[5]Main!$C$29</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B8" s="25" t="s">
         <v>16</v>
       </c>
@@ -8569,38 +8736,41 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-      <c r="P8" s="4">
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="S8" s="4">
         <v>96</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="T8" s="4">
         <v>57</v>
       </c>
-      <c r="R8" s="4">
+      <c r="U8" s="4">
         <v>82</v>
       </c>
-      <c r="T8" s="44">
+      <c r="W8" s="44">
         <v>15.3</v>
       </c>
-      <c r="U8" s="4"/>
-      <c r="Y8" s="4">
+      <c r="X8" s="4"/>
+      <c r="AB8" s="4">
         <f>[6]Main!$C$28</f>
         <v>1971</v>
       </c>
-      <c r="Z8" s="4" t="str">
+      <c r="AC8" s="4" t="str">
         <f>[6]Main!$C$27</f>
         <v>Leeds, UK</v>
       </c>
-      <c r="AA8" s="4">
+      <c r="AD8" s="4">
         <f>[6]Main!$C$29</f>
         <v>1988</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B9" s="25" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>65</v>
@@ -8609,7 +8779,7 @@
         <v>383</v>
       </c>
       <c r="F9" s="28">
-        <f>[7]Main!$C$6*H22</f>
+        <f>[7]Main!$C$6*H27</f>
         <v>23.9148</v>
       </c>
       <c r="G9" s="26">
@@ -8617,64 +8787,67 @@
         <v>73.998000000000005</v>
       </c>
       <c r="H9" s="26">
-        <f>[7]Main!$C$8*H22</f>
+        <f>[7]Main!$C$8*H27</f>
         <v>1769.6473704000002</v>
       </c>
       <c r="I9" s="26">
-        <f>[7]Main!$C$11*H22</f>
+        <f>[7]Main!$C$11*H27</f>
         <v>-1104.7318799999998</v>
       </c>
       <c r="J9" s="26">
-        <f>[7]Main!$C$12*H22</f>
+        <f>[7]Main!$C$12*H27</f>
         <v>2874.3792504000003</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L9" s="22">
         <f>'[7]Financial Model'!$U$37</f>
         <v>0.33604299344574362</v>
       </c>
       <c r="M9" s="22"/>
-      <c r="P9" s="4">
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="S9" s="4">
         <f>[7]Main!$D$23</f>
         <v>117</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="T9" s="4">
         <f>[7]Main!$D$24</f>
         <v>2</v>
       </c>
-      <c r="R9" s="4" t="str">
+      <c r="U9" s="4" t="str">
         <f>[7]Main!$D$25</f>
         <v>N/A</v>
       </c>
-      <c r="T9" s="4"/>
-      <c r="U9" s="35">
+      <c r="W9" s="4"/>
+      <c r="X9" s="35">
         <f>[7]Main!$C$38</f>
         <v>1.4375141996217067</v>
       </c>
-      <c r="W9" s="4" t="str">
+      <c r="Z9" s="4" t="str">
         <f>[7]Main!$C$33</f>
         <v>Q322</v>
       </c>
-      <c r="X9" s="36">
+      <c r="AA9" s="36">
         <f>[7]Main!$D$33</f>
         <v>44868</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="AB9" s="4">
         <f>[7]Main!$C$30</f>
         <v>1980</v>
       </c>
-      <c r="Z9" s="4" t="str">
+      <c r="AC9" s="4" t="str">
         <f>[7]Main!$C$29</f>
         <v>Wilmington, OH</v>
       </c>
-      <c r="AA9" s="4">
+      <c r="AD9" s="4">
         <f>[7]Main!$C$31</f>
         <v>2003</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B10" s="25" t="s">
         <v>10</v>
       </c>
@@ -8717,34 +8890,37 @@
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
-      <c r="P10" s="4">
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="4">
         <f>[8]Main!$D$21</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="T10" s="4">
         <f>[8]Main!$D$22</f>
         <v>153</v>
       </c>
-      <c r="R10" s="4"/>
-      <c r="T10" s="42">
+      <c r="U10" s="4"/>
+      <c r="W10" s="42">
         <f>AVERAGE(5.2,3.7,0.7,2.7)</f>
         <v>3.0750000000000002</v>
       </c>
-      <c r="U10" s="4"/>
-      <c r="Y10" s="4">
+      <c r="X10" s="4"/>
+      <c r="AB10" s="4">
         <f>[8]Main!$C$29</f>
         <v>2003</v>
       </c>
-      <c r="Z10" s="4" t="str">
+      <c r="AC10" s="4" t="str">
         <f>[8]Main!$C$28</f>
         <v>Budapest, Hungary</v>
       </c>
-      <c r="AA10" s="4">
+      <c r="AD10" s="4">
         <f>[8]Main!$C$30</f>
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B11" s="25"/>
       <c r="E11" s="4"/>
       <c r="H11" s="28"/>
@@ -8753,10 +8929,13 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
       <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X11" s="4"/>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B12" s="53"/>
       <c r="C12" s="53"/>
       <c r="D12" s="53"/>
@@ -8774,9 +8953,12 @@
       <c r="P12" s="53"/>
       <c r="Q12" s="53"/>
       <c r="R12" s="53"/>
-      <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="S12" s="53"/>
+      <c r="T12" s="53"/>
+      <c r="U12" s="53"/>
+      <c r="X12" s="4"/>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
@@ -8793,16 +8975,19 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="P13" s="4">
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="S13" s="4">
         <v>130</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="T13" s="4">
         <v>44</v>
       </c>
-      <c r="R13" s="4"/>
       <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X13" s="4"/>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B14" s="33">
         <v>753</v>
       </c>
@@ -8810,19 +8995,22 @@
         <v>88</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H14" s="31"/>
       <c r="K14" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
       <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="X14" s="4"/>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>382</v>
       </c>
@@ -8839,7 +9027,7 @@
         <v>40.14</v>
       </c>
       <c r="H15" s="32">
-        <f>(F15*H22)*592.96</f>
+        <f>(F15*H27)*592.96</f>
         <v>19993.188095999998</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -8848,9 +9036,12 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="X15" s="4"/>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B16" s="29">
         <v>9201</v>
       </c>
@@ -8868,7 +9059,7 @@
       </c>
       <c r="G16" s="30"/>
       <c r="H16" s="32">
-        <f>(F16*H24)*320.79</f>
+        <f>(F16*H29)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -8876,9 +9067,12 @@
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="X16" s="4"/>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>385</v>
       </c>
@@ -8895,7 +9089,7 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="H17" s="32">
-        <f>(F17*H22)*320.79</f>
+        <f>(F17*H27)*320.79</f>
         <v>2570.6827439999997</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -8904,11 +9098,14 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="X17" s="4"/>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>41</v>
@@ -8920,93 +9117,208 @@
         <v>383</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+      <c r="X18" s="4"/>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.2">
       <c r="H19" s="32"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D21" s="1"/>
-      <c r="F21" s="48" t="s">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B21" s="58" t="s">
+        <v>620</v>
+      </c>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="60"/>
+      <c r="X21" s="60"/>
+      <c r="Y21" s="60"/>
+      <c r="Z21" s="59"/>
+      <c r="AA21" s="59"/>
+      <c r="AB21" s="60"/>
+      <c r="AC21" s="60"/>
+      <c r="AD21" s="60"/>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B22" s="25" t="s">
+        <v>621</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>623</v>
+      </c>
+      <c r="G22" s="57" t="s">
+        <v>623</v>
+      </c>
+      <c r="H22" s="57" t="s">
+        <v>623</v>
+      </c>
+      <c r="I22" s="57" t="s">
+        <v>623</v>
+      </c>
+      <c r="J22" s="57" t="s">
+        <v>623</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="L22" s="22">
+        <f>[9]Accounts!$L$18</f>
+        <v>3.7691802910883844E-2</v>
+      </c>
+      <c r="M22" s="22">
+        <f>[9]Accounts!$L$19</f>
+        <v>-7.2462158441842464E-2</v>
+      </c>
+      <c r="N22" s="22">
+        <f>[9]Accounts!$L$20</f>
+        <v>-8.0967153446236284E-2</v>
+      </c>
+      <c r="O22" s="22">
+        <f>[9]Accounts!$K$21</f>
+        <v>0.18785583230649008</v>
+      </c>
+      <c r="S22" s="4">
+        <f>[9]Main!$C$16</f>
+        <v>16</v>
+      </c>
+      <c r="T22" s="4">
+        <f>[9]Main!$C$18</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="W22" s="4">
+        <f>[9]Main!$C$17</f>
+        <v>14.4</v>
+      </c>
+      <c r="Z22" s="4" t="str">
+        <f>[9]Main!$C$20</f>
+        <v>FY21/22</v>
+      </c>
+      <c r="AA22" s="36">
+        <f>[9]Main!$D$20</f>
+        <v>45141</v>
+      </c>
+      <c r="AB22" s="4">
+        <f>[9]Main!$C$14</f>
+        <v>1988</v>
+      </c>
+      <c r="AC22" s="4" t="str">
+        <f>[9]Main!$C$13</f>
+        <v>Stanstead Airport, UK</v>
+      </c>
+      <c r="AD22" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D26" s="1"/>
+      <c r="F26" s="48" t="s">
         <v>378</v>
       </c>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D22" s="1"/>
-      <c r="F22" s="46" t="s">
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D27" s="1"/>
+      <c r="F27" s="46" t="s">
         <v>379</v>
       </c>
-      <c r="G22" s="47"/>
-      <c r="H22" s="23">
+      <c r="G27" s="47"/>
+      <c r="H27" s="23">
         <v>0.84</v>
       </c>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D23" s="1"/>
-      <c r="F23" s="46" t="s">
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D28" s="1"/>
+      <c r="F28" s="46" t="s">
         <v>380</v>
       </c>
-      <c r="G23" s="47"/>
-      <c r="H23" s="23">
+      <c r="G28" s="47"/>
+      <c r="H28" s="23">
         <v>0.85</v>
       </c>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D24" s="1"/>
-      <c r="F24" s="46" t="s">
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D29" s="1"/>
+      <c r="F29" s="46" t="s">
         <v>389</v>
       </c>
-      <c r="G24" s="47"/>
-      <c r="H24" s="23">
+      <c r="G29" s="47"/>
+      <c r="H29" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="F25" s="51" t="s">
-        <v>433</v>
-      </c>
-      <c r="G25" s="52"/>
-      <c r="H25" s="24">
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="F30" s="51" t="s">
+        <v>431</v>
+      </c>
+      <c r="G30" s="52"/>
+      <c r="H30" s="24">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="F28" s="48" t="s">
-        <v>411</v>
-      </c>
-      <c r="G28" s="49"/>
-      <c r="H28" s="50"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="F29" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>611</v>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F33" s="48" t="s">
+        <v>410</v>
+      </c>
+      <c r="G33" s="49"/>
+      <c r="H33" s="50"/>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>609</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B12:R12"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B12:U12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
@@ -9017,184 +9329,234 @@
     <hyperlink ref="B4" r:id="rId6" xr:uid="{28605697-2E3F-4D0E-BA6A-013F294DB301}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{7F471098-FF05-4C1A-AA9F-8A6A66E1327B}"/>
     <hyperlink ref="B3" r:id="rId8" xr:uid="{340E3559-5E25-4E5A-9CCF-84716432B315}"/>
-    <hyperlink ref="G29" r:id="rId9" xr:uid="{76EE83BD-7400-4A46-978B-D25721A01204}"/>
+    <hyperlink ref="G34" r:id="rId9" xr:uid="{76EE83BD-7400-4A46-978B-D25721A01204}"/>
+    <hyperlink ref="B22" r:id="rId10" xr:uid="{C5ACF554-92E1-4EE1-9BA9-3999DE03B357}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA0EDE9-69E3-4DB1-A599-3D030985D0D0}">
-  <dimension ref="B1:M5"/>
+  <dimension ref="B1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="1"/>
-    <col min="7" max="7" width="41.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="1"/>
-    <col min="10" max="10" width="13.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8" style="1"/>
-    <col min="13" max="13" width="33.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8" style="1"/>
+    <col min="6" max="6" width="14.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="1"/>
+    <col min="8" max="8" width="41.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="1"/>
+    <col min="11" max="11" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8" style="1"/>
+    <col min="14" max="14" width="33.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="K1" s="43">
-        <f>AVERAGE(K3:K5)</f>
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L1" s="43">
+        <f>AVERAGE(L3:L6)</f>
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="54" t="s">
+        <v>404</v>
+      </c>
+      <c r="E3" s="55" t="s">
         <v>416</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="F3" s="55" t="s">
+        <v>615</v>
+      </c>
+      <c r="G3" s="55">
+        <v>2020</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>405</v>
+      </c>
+      <c r="I3" s="55">
+        <v>7</v>
+      </c>
+      <c r="J3" s="55">
+        <v>5</v>
+      </c>
+      <c r="K3" s="55">
+        <v>16</v>
+      </c>
+      <c r="L3" s="55">
+        <v>13.9</v>
+      </c>
+      <c r="M3" s="56" t="s">
+        <v>411</v>
+      </c>
+      <c r="N3" s="54" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="D4" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1984</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="I4" s="4">
+        <v>36</v>
+      </c>
+      <c r="J4" s="4">
+        <v>21</v>
+      </c>
+      <c r="K4" s="4">
+        <v>32</v>
+      </c>
+      <c r="L4" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="M4" s="34" t="s">
         <v>411</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="N4" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="F3" s="4">
-        <v>2020</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="H3" s="4">
-        <v>7</v>
-      </c>
-      <c r="I3" s="4">
-        <v>5</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="D5" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1997</v>
+      </c>
+      <c r="I5" s="4">
+        <v>14</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="L5" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="M5" s="34" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
+        <v>613</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1988</v>
+      </c>
+      <c r="I6" s="4">
+        <f>[9]Main!$C$16</f>
         <v>16</v>
       </c>
-      <c r="K3" s="4">
-        <v>13.9</v>
-      </c>
-      <c r="L3" s="34" t="s">
-        <v>412</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1984</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="H4" s="4">
-        <v>36</v>
-      </c>
-      <c r="I4" s="4">
-        <v>21</v>
-      </c>
-      <c r="J4" s="4">
-        <v>32</v>
-      </c>
-      <c r="K4" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="L4" s="34" t="s">
-        <v>412</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1997</v>
-      </c>
-      <c r="H5" s="4">
-        <v>14</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="J6" s="4">
+        <f>[9]Main!$C$18</f>
         <v>0</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="K5" s="4">
-        <v>7.8</v>
-      </c>
-      <c r="L5" s="34" t="s">
-        <v>412</v>
+      <c r="L6" s="4">
+        <f>[9]Main!$C$17</f>
+        <v>14.4</v>
+      </c>
+      <c r="M6" s="34" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M6" r:id="rId1" xr:uid="{7158A053-BE5F-4646-8E0B-5F3D64A099E7}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{1F071127-866B-4B01-A882-6893B122F78A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prelim work to restart looking at Airlines
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3CE161-D1FD-4181-BC77-1D907DE77CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EADF51A-C380-4085-84EB-55F9888C5D3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18900" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
@@ -28,6 +28,7 @@
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -309,7 +310,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="640">
   <si>
     <t>Ticker</t>
   </si>
@@ -2196,6 +2197,39 @@
   </si>
   <si>
     <t>(Normalised to GBP)</t>
+  </si>
+  <si>
+    <t>Regional &amp; short-haul</t>
+  </si>
+  <si>
+    <t>$SKYW</t>
+  </si>
+  <si>
+    <t>SkyWest, Inc.</t>
+  </si>
+  <si>
+    <t>$SAVE</t>
+  </si>
+  <si>
+    <t>$FDX</t>
+  </si>
+  <si>
+    <t>FedEx Corporation</t>
+  </si>
+  <si>
+    <t>$UPS</t>
+  </si>
+  <si>
+    <t>United Postal Service, Inc.</t>
+  </si>
+  <si>
+    <t>Freight &amp; Cargo</t>
+  </si>
+  <si>
+    <t>Ultra-low cost carrier covering North America</t>
+  </si>
+  <si>
+    <t>Regional airline operating flights scheduled, maintained &amp; sold by partner 'mailine' airlines</t>
   </si>
 </sst>
 </file>
@@ -2482,7 +2516,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2568,6 +2602,22 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2595,21 +2645,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2675,6 +2710,76 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Accounts"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="13">
+          <cell r="C13" t="str">
+            <v>Stanstead Airport, UK</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14">
+            <v>1988</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17">
+            <v>14.4</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="C18">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20" t="str">
+            <v>FY21/22</v>
+          </cell>
+          <cell r="D20">
+            <v>45141</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="18">
+          <cell r="L18">
+            <v>3.7691802910883844E-2</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="L19">
+            <v>-7.2462158441842464E-2</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="L20">
+            <v>-8.0967153446236284E-2</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="K21">
+            <v>0.18785583230649008</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3167,66 +3272,30 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Accounts"/>
+      <sheetName val="Financial Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="13">
-          <cell r="C13" t="str">
-            <v>Stanstead Airport, UK</v>
+        <row r="6">
+          <cell r="C6">
+            <v>33.74</v>
           </cell>
         </row>
-        <row r="14">
-          <cell r="C14">
-            <v>1988</v>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Atlanta, GA</v>
           </cell>
         </row>
-        <row r="16">
-          <cell r="C16">
-            <v>16</v>
+        <row r="24">
+          <cell r="C24">
+            <v>1924</v>
           </cell>
         </row>
-        <row r="17">
-          <cell r="C17">
-            <v>14.4</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20" t="str">
-            <v>FY21/22</v>
-          </cell>
-          <cell r="D20">
-            <v>45141</v>
-          </cell>
+        <row r="25">
+          <cell r="C25"/>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="18">
-          <cell r="L18">
-            <v>3.7691802910883844E-2</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="L19">
-            <v>-7.2462158441842464E-2</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="L20">
-            <v>-8.0967153446236284E-2</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="K21">
-            <v>0.18785583230649008</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8218,13 +8287,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:AD34"/>
+  <dimension ref="B1:AD40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="B9:U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8253,13 +8322,13 @@
   <sheetData>
     <row r="1" spans="2:30" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="53" t="s">
         <v>628</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="W1" s="43">
@@ -8371,7 +8440,7 @@
         <v>383</v>
       </c>
       <c r="F3" s="28">
-        <f>[1]Main!$C$6*H27</f>
+        <f>[1]Main!$C$6*H33</f>
         <v>58.001999999999995</v>
       </c>
       <c r="G3" s="26">
@@ -8379,15 +8448,15 @@
         <v>227.43</v>
       </c>
       <c r="H3" s="26">
-        <f>[1]Main!$C$12*H27</f>
+        <f>[1]Main!$C$12*H33</f>
         <v>13191.394859999999</v>
       </c>
       <c r="I3" s="40">
-        <f>[1]Main!$C$11*H27</f>
+        <f>[1]Main!$C$11*H33</f>
         <v>0</v>
       </c>
       <c r="J3" s="26">
-        <f>[1]Main!$C$12*H27</f>
+        <f>[1]Main!$C$12*H33</f>
         <v>13191.394859999999</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -8431,7 +8500,7 @@
         <v>430</v>
       </c>
       <c r="F4" s="28">
-        <f>[2]Main!$C$6*H30</f>
+        <f>[2]Main!$C$6*H36</f>
         <v>19.570099999999996</v>
       </c>
       <c r="G4" s="26">
@@ -8439,15 +8508,15 @@
         <v>385.26</v>
       </c>
       <c r="H4" s="26">
-        <f>[2]Main!$C$8*H30</f>
+        <f>[2]Main!$C$8*H36</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="I4" s="26">
-        <f>[2]Main!$C$11*H30</f>
+        <f>[2]Main!$C$11*H36</f>
         <v>0</v>
       </c>
       <c r="J4" s="26">
-        <f>[2]Main!$C$12*H30</f>
+        <f>[2]Main!$C$12*H36</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -8557,7 +8626,7 @@
         <v>383</v>
       </c>
       <c r="F6" s="28">
-        <f>[4]Main!$C$6*H27</f>
+        <f>[4]Main!$C$6*H33</f>
         <v>35.1372</v>
       </c>
       <c r="G6" s="26">
@@ -8565,15 +8634,15 @@
         <v>126.5</v>
       </c>
       <c r="H6" s="26">
-        <f>[4]Main!$C$8*H27</f>
+        <f>[4]Main!$C$8*H33</f>
         <v>4444.8557999999994</v>
       </c>
       <c r="I6" s="26">
-        <f>[4]Main!$C$11*H27</f>
+        <f>[4]Main!$C$11*H33</f>
         <v>942.48</v>
       </c>
       <c r="J6" s="26">
-        <f>[4]Main!$C$12*H27</f>
+        <f>[4]Main!$C$12*H33</f>
         <v>3502.3757999999998</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -8779,7 +8848,7 @@
         <v>383</v>
       </c>
       <c r="F9" s="28">
-        <f>[7]Main!$C$6*H27</f>
+        <f>[7]Main!$C$6*H33</f>
         <v>23.9148</v>
       </c>
       <c r="G9" s="26">
@@ -8787,15 +8856,15 @@
         <v>73.998000000000005</v>
       </c>
       <c r="H9" s="26">
-        <f>[7]Main!$C$8*H27</f>
+        <f>[7]Main!$C$8*H33</f>
         <v>1769.6473704000002</v>
       </c>
       <c r="I9" s="26">
-        <f>[7]Main!$C$11*H27</f>
+        <f>[7]Main!$C$11*H33</f>
         <v>-1104.7318799999998</v>
       </c>
       <c r="J9" s="26">
-        <f>[7]Main!$C$12*H27</f>
+        <f>[7]Main!$C$12*H33</f>
         <v>2874.3792504000003</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -8936,26 +9005,26 @@
       <c r="X11" s="4"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="53"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="61"/>
+      <c r="U12" s="61"/>
       <c r="X12" s="4"/>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.2">
@@ -9027,7 +9096,7 @@
         <v>40.14</v>
       </c>
       <c r="H15" s="32">
-        <f>(F15*H27)*592.96</f>
+        <f>(F15*H33)*592.96</f>
         <v>19993.188095999998</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -9059,7 +9128,7 @@
       </c>
       <c r="G16" s="30"/>
       <c r="H16" s="32">
-        <f>(F16*H29)*320.79</f>
+        <f>(F16*H35)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -9089,7 +9158,7 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="H17" s="32">
-        <f>(F17*H27)*320.79</f>
+        <f>(F17*H33)*320.79</f>
         <v>2570.6827439999997</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -9104,7 +9173,7 @@
       <c r="X17" s="4"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="25" t="s">
         <v>397</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -9116,208 +9185,329 @@
       <c r="E18" s="4" t="s">
         <v>383</v>
       </c>
+      <c r="F18" s="52">
+        <f>[9]Main!$C$6*H33</f>
+        <v>28.3416</v>
+      </c>
       <c r="K18" s="1" t="s">
         <v>398</v>
       </c>
       <c r="X18" s="4"/>
+      <c r="AB18" s="4">
+        <f>[9]Main!$C$24</f>
+        <v>1924</v>
+      </c>
+      <c r="AC18" s="4" t="str">
+        <f>[9]Main!$C$23</f>
+        <v>Atlanta, GA</v>
+      </c>
+      <c r="AD18" s="4">
+        <f>[9]Main!$C$25</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="H19" s="32"/>
+      <c r="B19" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F19" s="52"/>
+      <c r="K19" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="X19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F20" s="52"/>
+      <c r="K20" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="X20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F21" s="52"/>
+      <c r="K21" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="X21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F22" s="52"/>
+      <c r="K22" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="X22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="E23" s="4"/>
+      <c r="F23" s="52"/>
+      <c r="X23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B24" s="25"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="52"/>
+      <c r="X24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="H25" s="32"/>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B27" s="49" t="s">
         <v>620</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="60"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="60"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="59"/>
-      <c r="T21" s="59"/>
-      <c r="U21" s="60"/>
-      <c r="V21" s="60"/>
-      <c r="W21" s="60"/>
-      <c r="X21" s="60"/>
-      <c r="Y21" s="60"/>
-      <c r="Z21" s="59"/>
-      <c r="AA21" s="59"/>
-      <c r="AB21" s="60"/>
-      <c r="AC21" s="60"/>
-      <c r="AD21" s="60"/>
-    </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B22" s="25" t="s">
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="51"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="51"/>
+      <c r="V27" s="51"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="51"/>
+      <c r="Z27" s="50"/>
+      <c r="AA27" s="50"/>
+      <c r="AB27" s="51"/>
+      <c r="AC27" s="51"/>
+      <c r="AD27" s="51"/>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B28" s="25" t="s">
         <v>621</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="D28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F28" s="48" t="s">
         <v>623</v>
       </c>
-      <c r="G22" s="57" t="s">
+      <c r="G28" s="48" t="s">
         <v>623</v>
       </c>
-      <c r="H22" s="57" t="s">
+      <c r="H28" s="48" t="s">
         <v>623</v>
       </c>
-      <c r="I22" s="57" t="s">
+      <c r="I28" s="48" t="s">
         <v>623</v>
       </c>
-      <c r="J22" s="57" t="s">
+      <c r="J28" s="48" t="s">
         <v>623</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="L22" s="22">
-        <f>[9]Accounts!$L$18</f>
+      <c r="L28" s="22">
+        <f>[10]Accounts!$L$18</f>
         <v>3.7691802910883844E-2</v>
       </c>
-      <c r="M22" s="22">
-        <f>[9]Accounts!$L$19</f>
+      <c r="M28" s="22">
+        <f>[10]Accounts!$L$19</f>
         <v>-7.2462158441842464E-2</v>
       </c>
-      <c r="N22" s="22">
-        <f>[9]Accounts!$L$20</f>
+      <c r="N28" s="22">
+        <f>[10]Accounts!$L$20</f>
         <v>-8.0967153446236284E-2</v>
       </c>
-      <c r="O22" s="22">
-        <f>[9]Accounts!$K$21</f>
+      <c r="O28" s="22">
+        <f>[10]Accounts!$K$21</f>
         <v>0.18785583230649008</v>
       </c>
-      <c r="S22" s="4">
-        <f>[9]Main!$C$16</f>
+      <c r="S28" s="4">
+        <f>[10]Main!$C$16</f>
         <v>16</v>
       </c>
-      <c r="T22" s="4">
-        <f>[9]Main!$C$18</f>
+      <c r="T28" s="4">
+        <f>[10]Main!$C$18</f>
         <v>0</v>
       </c>
-      <c r="U22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="W22" s="4">
-        <f>[9]Main!$C$17</f>
+      <c r="U28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="W28" s="4">
+        <f>[10]Main!$C$17</f>
         <v>14.4</v>
       </c>
-      <c r="Z22" s="4" t="str">
-        <f>[9]Main!$C$20</f>
+      <c r="Z28" s="4" t="str">
+        <f>[10]Main!$C$20</f>
         <v>FY21/22</v>
       </c>
-      <c r="AA22" s="36">
-        <f>[9]Main!$D$20</f>
+      <c r="AA28" s="36">
+        <f>[10]Main!$D$20</f>
         <v>45141</v>
       </c>
-      <c r="AB22" s="4">
-        <f>[9]Main!$C$14</f>
+      <c r="AB28" s="4">
+        <f>[10]Main!$C$14</f>
         <v>1988</v>
       </c>
-      <c r="AC22" s="4" t="str">
-        <f>[9]Main!$C$13</f>
+      <c r="AC28" s="4" t="str">
+        <f>[10]Main!$C$13</f>
         <v>Stanstead Airport, UK</v>
       </c>
-      <c r="AD22" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="D26" s="1"/>
-      <c r="F26" s="48" t="s">
+      <c r="AD28" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D32" s="1"/>
+      <c r="F32" s="56" t="s">
         <v>378</v>
       </c>
-      <c r="G26" s="49"/>
-      <c r="H26" s="50"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-    </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="D27" s="1"/>
-      <c r="F27" s="46" t="s">
+      <c r="G32" s="57"/>
+      <c r="H32" s="58"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+    </row>
+    <row r="33" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D33" s="1"/>
+      <c r="F33" s="54" t="s">
         <v>379</v>
       </c>
-      <c r="G27" s="47"/>
-      <c r="H27" s="23">
+      <c r="G33" s="55"/>
+      <c r="H33" s="23">
         <v>0.84</v>
       </c>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="D28" s="1"/>
-      <c r="F28" s="46" t="s">
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D34" s="1"/>
+      <c r="F34" s="54" t="s">
         <v>380</v>
       </c>
-      <c r="G28" s="47"/>
-      <c r="H28" s="23">
+      <c r="G34" s="55"/>
+      <c r="H34" s="23">
         <v>0.85</v>
       </c>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-    </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="D29" s="1"/>
-      <c r="F29" s="46" t="s">
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+    </row>
+    <row r="35" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D35" s="1"/>
+      <c r="F35" s="54" t="s">
         <v>389</v>
       </c>
-      <c r="G29" s="47"/>
-      <c r="H29" s="23">
+      <c r="G35" s="55"/>
+      <c r="H35" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-    </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="F30" s="51" t="s">
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+    </row>
+    <row r="36" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F36" s="59" t="s">
         <v>431</v>
       </c>
-      <c r="G30" s="52"/>
-      <c r="H30" s="24">
+      <c r="G36" s="60"/>
+      <c r="H36" s="24">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F33" s="48" t="s">
+    <row r="39" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F39" s="56" t="s">
         <v>410</v>
       </c>
-      <c r="G33" s="49"/>
-      <c r="H33" s="50"/>
-    </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F34" s="1" t="s">
+      <c r="G39" s="57"/>
+      <c r="H39" s="58"/>
+    </row>
+    <row r="40" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="G34" s="34" t="s">
+      <c r="G40" s="34" t="s">
         <v>609</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F32:H32"/>
     <mergeCell ref="B12:U12"/>
   </mergeCells>
   <hyperlinks>
@@ -9329,12 +9519,13 @@
     <hyperlink ref="B4" r:id="rId6" xr:uid="{28605697-2E3F-4D0E-BA6A-013F294DB301}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{7F471098-FF05-4C1A-AA9F-8A6A66E1327B}"/>
     <hyperlink ref="B3" r:id="rId8" xr:uid="{340E3559-5E25-4E5A-9CCF-84716432B315}"/>
-    <hyperlink ref="G34" r:id="rId9" xr:uid="{76EE83BD-7400-4A46-978B-D25721A01204}"/>
-    <hyperlink ref="B22" r:id="rId10" xr:uid="{C5ACF554-92E1-4EE1-9BA9-3999DE03B357}"/>
+    <hyperlink ref="G40" r:id="rId9" xr:uid="{76EE83BD-7400-4A46-978B-D25721A01204}"/>
+    <hyperlink ref="B28" r:id="rId10" xr:uid="{C5ACF554-92E1-4EE1-9BA9-3999DE03B357}"/>
+    <hyperlink ref="B18" r:id="rId11" xr:uid="{D7C56EA9-B97D-4FCE-9474-2C5FB0F6C524}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId12"/>
+  <legacyDrawing r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -9346,7 +9537,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9414,38 +9605,41 @@
         <v>403</v>
       </c>
     </row>
-    <row r="3" spans="2:14" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="54" t="s">
+    <row r="3" spans="2:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="45" t="s">
         <v>404</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="D3" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="E3" s="46" t="s">
         <v>416</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="46" t="s">
         <v>615</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="46">
         <v>2020</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="45" t="s">
         <v>405</v>
       </c>
-      <c r="I3" s="55">
+      <c r="I3" s="46">
         <v>7</v>
       </c>
-      <c r="J3" s="55">
+      <c r="J3" s="46">
         <v>5</v>
       </c>
-      <c r="K3" s="55">
+      <c r="K3" s="46">
         <v>16</v>
       </c>
-      <c r="L3" s="55">
+      <c r="L3" s="46">
         <v>13.9</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="47" t="s">
         <v>411</v>
       </c>
-      <c r="N3" s="54" t="s">
+      <c r="N3" s="45" t="s">
         <v>616</v>
       </c>
     </row>
@@ -9536,15 +9730,15 @@
         <v>1988</v>
       </c>
       <c r="I6" s="4">
-        <f>[9]Main!$C$16</f>
+        <f>[10]Main!$C$16</f>
         <v>16</v>
       </c>
       <c r="J6" s="4">
-        <f>[9]Main!$C$18</f>
+        <f>[10]Main!$C$18</f>
         <v>0</v>
       </c>
       <c r="L6" s="4">
-        <f>[9]Main!$C$17</f>
+        <f>[10]Main!$C$17</f>
         <v>14.4</v>
       </c>
       <c r="M6" s="34" t="s">

</xml_diff>

<commit_message>
£HLMA latest FY results
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AC84BD-88C4-164C-BDF6-29EB9765FDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC85C29-BE69-4184-BFE6-8FB1EC4F6FE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="32400" windowHeight="18800" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
+    <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18795" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
   <sheets>
     <sheet name="Airlines Screening" sheetId="2" r:id="rId1"/>
@@ -29,20 +29,12 @@
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -262,7 +254,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
@@ -270,7 +262,7 @@
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -279,21 +271,21 @@
   <futureMetadata name="XLRICHVALUE" count="3">
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="2"/>
         </ext>
       </extLst>
@@ -319,7 +311,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="651">
   <si>
     <t>Ticker</t>
   </si>
@@ -2133,9 +2125,6 @@
     <t>$0.01</t>
   </si>
   <si>
-    <t>Flag carrier for China, 1/3 of "Big Three" Chinese airlines</t>
-  </si>
-  <si>
     <t>Worldwide cargo &amp; combi charters for freight as well as US DoD. Leasing (Prime Air etc.)</t>
   </si>
   <si>
@@ -2271,10 +2260,10 @@
     <t>Polish charter airline operating holiday &amp; charter flights from Polish hubs</t>
   </si>
   <si>
-    <t>Warsaw, Poland</t>
-  </si>
-  <si>
     <t>WSE</t>
+  </si>
+  <si>
+    <t>Flag carrier for China, 1 of "Big Three" Chinese airlines</t>
   </si>
 </sst>
 </file>
@@ -2282,8 +2271,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;0&quot;#"/>
@@ -2559,7 +2548,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2583,7 +2572,7 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2612,7 +2601,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2672,10 +2661,22 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2687,25 +2688,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2728,7 +2717,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -2779,7 +2768,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -2843,8 +2832,72 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>48.6</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>17.54</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>852.44399999999996</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>852.44399999999996</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Warsaw, Poland</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>2009</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>2015</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>26</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>6</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -2898,7 +2951,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -2959,7 +3012,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -3029,7 +3082,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -3106,7 +3159,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -3164,7 +3217,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -3254,7 +3307,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -3326,7 +3379,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -3735,13 +3788,13 @@
       <selection activeCell="B6" sqref="B6:L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="20"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="20"/>
+    <col min="2" max="2" width="42.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
         <v>27</v>
@@ -3783,7 +3836,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
@@ -3827,7 +3880,7 @@
         <v>-1.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>48</v>
       </c>
@@ -3871,7 +3924,7 @@
         <v>-1.49E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>53</v>
       </c>
@@ -3915,7 +3968,7 @@
         <v>-9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>57</v>
       </c>
@@ -3959,7 +4012,7 @@
         <v>-3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>63</v>
       </c>
@@ -4003,7 +4056,7 @@
         <v>-2.86E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>70</v>
       </c>
@@ -4047,7 +4100,7 @@
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>75</v>
       </c>
@@ -4091,7 +4144,7 @@
         <v>1.11E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>75</v>
       </c>
@@ -4135,7 +4188,7 @@
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>82</v>
       </c>
@@ -4179,7 +4232,7 @@
         <v>2.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>753</v>
       </c>
@@ -4223,7 +4276,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>93</v>
       </c>
@@ -4267,7 +4320,7 @@
         <v>-2.93E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>93</v>
       </c>
@@ -4311,7 +4364,7 @@
         <v>-2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>103</v>
       </c>
@@ -4355,7 +4408,7 @@
         <v>-1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>1055</v>
       </c>
@@ -4399,7 +4452,7 @@
         <v>-9.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>112</v>
       </c>
@@ -4443,7 +4496,7 @@
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>670</v>
       </c>
@@ -4487,7 +4540,7 @@
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>122</v>
       </c>
@@ -4531,7 +4584,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>127</v>
       </c>
@@ -4575,7 +4628,7 @@
         <v>-2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>132</v>
       </c>
@@ -4619,7 +4672,7 @@
         <v>-2.07E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>138</v>
       </c>
@@ -4663,7 +4716,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>145</v>
       </c>
@@ -4707,7 +4760,7 @@
         <v>-2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>138</v>
       </c>
@@ -4751,7 +4804,7 @@
         <v>-7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>12</v>
       </c>
@@ -4795,7 +4848,7 @@
         <v>-4.53E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>158</v>
       </c>
@@ -4839,7 +4892,7 @@
         <v>-2.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>162</v>
       </c>
@@ -4884,7 +4937,7 @@
         <v>-3.1E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>293</v>
       </c>
@@ -4928,7 +4981,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>173</v>
       </c>
@@ -4972,7 +5025,7 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>178</v>
       </c>
@@ -5016,7 +5069,7 @@
         <v>-3.04E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>184</v>
       </c>
@@ -5061,7 +5114,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>11</v>
       </c>
@@ -5105,7 +5158,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>10</v>
       </c>
@@ -5149,7 +5202,7 @@
         <v>-6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>196</v>
       </c>
@@ -5193,7 +5246,7 @@
         <v>7.5399999999999995E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>201</v>
       </c>
@@ -5237,7 +5290,7 @@
         <v>-9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>207</v>
       </c>
@@ -5281,7 +5334,7 @@
         <v>-1.61E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>211</v>
       </c>
@@ -5325,7 +5378,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>217</v>
       </c>
@@ -5369,7 +5422,7 @@
         <v>-4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>223</v>
       </c>
@@ -5413,7 +5466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>227</v>
       </c>
@@ -5457,7 +5510,7 @@
         <v>-1.8200000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>231</v>
       </c>
@@ -5501,7 +5554,7 @@
         <v>1.84E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>231</v>
       </c>
@@ -5545,7 +5598,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>242</v>
       </c>
@@ -5589,7 +5642,7 @@
         <v>-3.85E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>248</v>
       </c>
@@ -5633,7 +5686,7 @@
         <v>-3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>254</v>
       </c>
@@ -5677,7 +5730,7 @@
         <v>-4.36E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>258</v>
       </c>
@@ -5721,7 +5774,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>264</v>
       </c>
@@ -5765,7 +5818,7 @@
         <v>-4.1200000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>269</v>
       </c>
@@ -5809,7 +5862,7 @@
         <v>-5.2600000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>275</v>
       </c>
@@ -5853,7 +5906,7 @@
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>278</v>
       </c>
@@ -5897,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>283</v>
       </c>
@@ -5942,7 +5995,7 @@
         <v>-1.4E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>288</v>
       </c>
@@ -5987,7 +6040,7 @@
         <v>-3.3300000000000003E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>293</v>
       </c>
@@ -6031,7 +6084,7 @@
         <v>-5.5E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>299</v>
       </c>
@@ -6075,7 +6128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>304</v>
       </c>
@@ -6119,7 +6172,7 @@
         <v>2.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>310</v>
       </c>
@@ -6163,7 +6216,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>316</v>
       </c>
@@ -6207,7 +6260,7 @@
         <v>-1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>316</v>
       </c>
@@ -6251,7 +6304,7 @@
         <v>-2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>326</v>
       </c>
@@ -6295,7 +6348,7 @@
         <v>-2.7799999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>332</v>
       </c>
@@ -6339,7 +6392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>337</v>
       </c>
@@ -6383,7 +6436,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>343</v>
       </c>
@@ -6427,7 +6480,7 @@
         <v>-3.7199999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>348</v>
       </c>
@@ -6472,7 +6525,7 @@
         <v>-4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
         <v>353</v>
       </c>
@@ -6516,7 +6569,7 @@
         <v>-4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>359</v>
       </c>
@@ -6560,7 +6613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>365</v>
       </c>
@@ -6604,7 +6657,7 @@
         <v>-0.88419999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>371</v>
       </c>
@@ -6744,13 +6797,13 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="20"/>
-    <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="20"/>
+    <col min="2" max="2" width="53.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="37"/>
       <c r="B1" s="5" t="s">
         <v>27</v>
@@ -6792,7 +6845,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>436</v>
       </c>
@@ -6836,7 +6889,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>442</v>
       </c>
@@ -6880,7 +6933,7 @@
         <v>-0.11940000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>447</v>
       </c>
@@ -6924,7 +6977,7 @@
         <v>-1.8E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>452</v>
       </c>
@@ -6968,7 +7021,7 @@
         <v>3.2800000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>458</v>
       </c>
@@ -7012,7 +7065,7 @@
         <v>4.6100000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>463</v>
       </c>
@@ -7056,7 +7109,7 @@
         <v>5.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>469</v>
       </c>
@@ -7100,7 +7153,7 @@
         <v>2.46E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>474</v>
       </c>
@@ -7144,7 +7197,7 @@
         <v>-1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>2588</v>
       </c>
@@ -7188,7 +7241,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>483</v>
       </c>
@@ -7232,7 +7285,7 @@
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>488</v>
       </c>
@@ -7276,7 +7329,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>493</v>
       </c>
@@ -7320,7 +7373,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>497</v>
       </c>
@@ -7364,7 +7417,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>502</v>
       </c>
@@ -7408,7 +7461,7 @@
         <v>0.1346</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>694</v>
       </c>
@@ -7452,7 +7505,7 @@
         <v>6.4199999999999993E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>510</v>
       </c>
@@ -7496,7 +7549,7 @@
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>516</v>
       </c>
@@ -7540,7 +7593,7 @@
         <v>-8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>357</v>
       </c>
@@ -7584,7 +7637,7 @@
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>526</v>
       </c>
@@ -7628,7 +7681,7 @@
         <v>5.3E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>532</v>
       </c>
@@ -7672,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>1848</v>
       </c>
@@ -7716,7 +7769,7 @@
         <v>-6.3E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>541</v>
       </c>
@@ -7760,7 +7813,7 @@
         <v>-0.16120000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>546</v>
       </c>
@@ -7804,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>551</v>
       </c>
@@ -7848,7 +7901,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>557</v>
       </c>
@@ -7892,7 +7945,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>563</v>
       </c>
@@ -7936,7 +7989,7 @@
         <v>3.5700000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>563</v>
       </c>
@@ -7980,7 +8033,7 @@
         <v>2.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>573</v>
       </c>
@@ -8024,7 +8077,7 @@
         <v>-3.8800000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>8620</v>
       </c>
@@ -8069,7 +8122,7 @@
         <v>-4.4900000000000002E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>583</v>
       </c>
@@ -8113,7 +8166,7 @@
         <v>2.63E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>583</v>
       </c>
@@ -8157,7 +8210,7 @@
         <v>2.3699999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>593</v>
       </c>
@@ -8201,7 +8254,7 @@
         <v>6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>596</v>
       </c>
@@ -8245,7 +8298,7 @@
         <v>-1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>601</v>
       </c>
@@ -8351,42 +8404,42 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q17" sqref="Q17"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="4"/>
-    <col min="5" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="8.83203125" style="1"/>
-    <col min="11" max="11" width="71.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="18" width="8.83203125" style="1"/>
-    <col min="19" max="19" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="4"/>
+    <col min="5" max="5" width="8.875" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="8.875" style="1"/>
+    <col min="11" max="11" width="71.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="8.875" style="1"/>
+    <col min="19" max="19" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.375" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.83203125" style="1" customWidth="1"/>
-    <col min="24" max="25" width="8.83203125" style="1"/>
-    <col min="26" max="27" width="8.83203125" style="4"/>
-    <col min="28" max="28" width="8.83203125" style="1"/>
-    <col min="29" max="29" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.83203125" style="1"/>
+    <col min="22" max="22" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.875" style="1" customWidth="1"/>
+    <col min="24" max="25" width="8.875" style="1"/>
+    <col min="26" max="27" width="8.875" style="4"/>
+    <col min="28" max="28" width="8.875" style="1"/>
+    <col min="29" max="29" width="16.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
-      <c r="F1" s="58" t="s">
-        <v>628</v>
-      </c>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="F1" s="59" t="s">
+        <v>627</v>
+      </c>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="W1" s="41">
@@ -8398,7 +8451,7 @@
         <v>1.3082569747231938</v>
       </c>
     </row>
-    <row r="2" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8433,22 +8486,22 @@
         <v>9</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>626</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>406</v>
@@ -8463,7 +8516,7 @@
         <v>433</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>424</v>
@@ -8481,10 +8534,10 @@
         <v>432</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="3" spans="2:30" x14ac:dyDescent="0.15">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>384</v>
       </c>
@@ -8544,7 +8597,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="4" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="50" t="s">
         <v>429</v>
       </c>
@@ -8608,7 +8661,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="50" t="s">
         <v>12</v>
       </c>
@@ -8677,7 +8730,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="6" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="50" t="s">
         <v>421</v>
       </c>
@@ -8750,7 +8803,7 @@
       </c>
       <c r="AD6" s="43"/>
     </row>
-    <row r="7" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="50" t="s">
         <v>11</v>
       </c>
@@ -8833,7 +8886,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="50" t="s">
         <v>16</v>
       </c>
@@ -8903,7 +8956,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="9" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="50" t="s">
         <v>434</v>
       </c>
@@ -8937,7 +8990,7 @@
         <v>2874.3792504000003</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="L9" s="54">
         <f>'[7]Financial Model'!$U$37</f>
@@ -8985,7 +9038,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="10" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="50" t="s">
         <v>10</v>
       </c>
@@ -9060,7 +9113,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B11" s="25"/>
       <c r="E11" s="4"/>
       <c r="H11" s="28"/>
@@ -9075,30 +9128,30 @@
       <c r="U11" s="4"/>
       <c r="X11" s="4"/>
     </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.15">
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="65"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
-      <c r="U12" s="65"/>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="67"/>
+      <c r="T12" s="67"/>
+      <c r="U12" s="67"/>
       <c r="X12" s="4"/>
     </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
@@ -9109,6 +9162,8 @@
         <v>18</v>
       </c>
       <c r="H13" s="31"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
       <c r="K13" s="1" t="s">
         <v>24</v>
       </c>
@@ -9127,7 +9182,7 @@
       <c r="U13" s="4"/>
       <c r="X13" s="4"/>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B14" s="33">
         <v>753</v>
       </c>
@@ -9138,8 +9193,10 @@
         <v>396</v>
       </c>
       <c r="H14" s="31"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
       <c r="K14" s="1" t="s">
-        <v>604</v>
+        <v>650</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -9150,7 +9207,7 @@
       <c r="U14" s="4"/>
       <c r="X14" s="4"/>
     </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>382</v>
       </c>
@@ -9170,6 +9227,8 @@
         <f>(F15*H33)*592.96</f>
         <v>19993.188095999998</v>
       </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
       <c r="K15" s="1" t="s">
         <v>395</v>
       </c>
@@ -9181,7 +9240,7 @@
       <c r="Q15" s="4"/>
       <c r="X15" s="4"/>
     </row>
-    <row r="16" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B16" s="29">
         <v>9201</v>
       </c>
@@ -9202,6 +9261,8 @@
         <f>(F16*H35)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
       <c r="K16" s="1" t="s">
         <v>390</v>
       </c>
@@ -9212,7 +9273,7 @@
       <c r="P16" s="4"/>
       <c r="X16" s="4"/>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>385</v>
       </c>
@@ -9232,6 +9293,8 @@
         <f>(F17*H33)*320.79</f>
         <v>2570.6827439999997</v>
       </c>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
       <c r="K17" s="1" t="s">
         <v>393</v>
       </c>
@@ -9243,7 +9306,7 @@
       <c r="Q17" s="4"/>
       <c r="X17" s="4"/>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="s">
         <v>397</v>
       </c>
@@ -9260,6 +9323,8 @@
         <f>[9]Main!$C$6*H33</f>
         <v>28.3416</v>
       </c>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
       <c r="K18" s="1" t="s">
         <v>398</v>
       </c>
@@ -9277,12 +9342,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>630</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>631</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>65</v>
@@ -9291,17 +9356,19 @@
         <v>383</v>
       </c>
       <c r="F19" s="49"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
       <c r="K19" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="X19" s="4"/>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
       <c r="AD19" s="4"/>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>232</v>
@@ -9313,20 +9380,22 @@
         <v>383</v>
       </c>
       <c r="F20" s="49"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
       <c r="K20" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="X20" s="4"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
       <c r="AD20" s="4"/>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>634</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>42</v>
@@ -9335,20 +9404,22 @@
         <v>383</v>
       </c>
       <c r="F21" s="49"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
       <c r="K21" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="X21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>635</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>636</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>42</v>
@@ -9357,23 +9428,25 @@
         <v>383</v>
       </c>
       <c r="F22" s="49"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
       <c r="K22" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="X22" s="4"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
       <c r="AD22" s="4"/>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>208</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>377</v>
@@ -9388,67 +9461,84 @@
         <f>(F23*G23)*H34</f>
         <v>3122.7427499999999</v>
       </c>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
       <c r="K23" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="X23" s="4"/>
       <c r="AB23" s="4">
         <v>2004</v>
       </c>
       <c r="AC23" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AD23" s="4"/>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.15">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B24" s="25" t="s">
+        <v>645</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>651</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>647</v>
-      </c>
       <c r="F24" s="49">
-        <v>49.5</v>
+        <f>[11]Main!$C$6*H37</f>
+        <v>9.234</v>
       </c>
       <c r="G24" s="1">
+        <f>[11]Main!$C$7</f>
         <v>17.54</v>
       </c>
       <c r="H24" s="32">
-        <f>(F24*G24)*H37</f>
-        <v>164.96369999999999</v>
+        <f>[11]Main!$C$8*H37</f>
+        <v>161.96436</v>
+      </c>
+      <c r="I24" s="26">
+        <f>[11]Main!$C$11*H37</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="26">
+        <f>[11]Main!$C$12*H37</f>
+        <v>161.96436</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="S24" s="4">
+        <f>[11]Main!$C$27</f>
         <v>26</v>
       </c>
       <c r="T24" s="4">
+        <f>[11]Main!$C$28</f>
         <v>6</v>
       </c>
       <c r="X24" s="4"/>
       <c r="AB24" s="4">
+        <f>[11]Main!$C$24</f>
         <v>2009</v>
       </c>
-      <c r="AC24" s="4" t="s">
-        <v>650</v>
+      <c r="AC24" s="4" t="str">
+        <f>[11]Main!$C$23</f>
+        <v>Warsaw, Poland</v>
       </c>
       <c r="AD24" s="4">
+        <f>[11]Main!$C$25</f>
         <v>2015</v>
       </c>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.2">
       <c r="H25" s="32"/>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B27" s="46" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="47"/>
@@ -9479,12 +9569,12 @@
       <c r="AC27" s="48"/>
       <c r="AD27" s="48"/>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B28" s="25" t="s">
+        <v>620</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>621</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>622</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>67</v>
@@ -9493,22 +9583,22 @@
         <v>381</v>
       </c>
       <c r="F28" s="45" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G28" s="45" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H28" s="45" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I28" s="45" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="J28" s="45" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="L28" s="22">
         <f>[10]Accounts!$L$18</f>
@@ -9554,89 +9644,89 @@
         <v>1988</v>
       </c>
       <c r="AC28" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AD28" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.2">
       <c r="D32" s="1"/>
-      <c r="F32" s="60" t="s">
+      <c r="F32" s="64" t="s">
         <v>378</v>
       </c>
-      <c r="G32" s="61"/>
-      <c r="H32" s="62"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="66"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="4:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D33" s="1"/>
-      <c r="F33" s="66" t="s">
+      <c r="F33" s="60" t="s">
         <v>379</v>
       </c>
-      <c r="G33" s="67"/>
-      <c r="H33" s="68">
+      <c r="G33" s="61"/>
+      <c r="H33" s="58">
         <v>0.84</v>
       </c>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="4:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D34" s="1"/>
-      <c r="F34" s="59" t="s">
+      <c r="F34" s="62" t="s">
         <v>380</v>
       </c>
-      <c r="G34" s="69"/>
+      <c r="G34" s="63"/>
       <c r="H34" s="23">
         <v>0.85</v>
       </c>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="4:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D35" s="1"/>
-      <c r="F35" s="59" t="s">
+      <c r="F35" s="62" t="s">
         <v>389</v>
       </c>
-      <c r="G35" s="69"/>
+      <c r="G35" s="63"/>
       <c r="H35" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="4:20" x14ac:dyDescent="0.15">
-      <c r="F36" s="59" t="s">
+    <row r="36" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F36" s="62" t="s">
         <v>431</v>
       </c>
-      <c r="G36" s="69"/>
+      <c r="G36" s="63"/>
       <c r="H36" s="23">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="4:20" x14ac:dyDescent="0.15">
-      <c r="F37" s="63" t="s">
-        <v>648</v>
-      </c>
-      <c r="G37" s="64"/>
+    <row r="37" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F37" s="68" t="s">
+        <v>647</v>
+      </c>
+      <c r="G37" s="69"/>
       <c r="H37" s="24">
         <v>0.19</v>
       </c>
     </row>
-    <row r="39" spans="4:20" x14ac:dyDescent="0.15">
-      <c r="F39" s="60" t="s">
+    <row r="39" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F39" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="G39" s="61"/>
-      <c r="H39" s="62"/>
-    </row>
-    <row r="40" spans="4:20" x14ac:dyDescent="0.15">
+      <c r="G39" s="65"/>
+      <c r="H39" s="66"/>
+    </row>
+    <row r="40" spans="4:20" x14ac:dyDescent="0.2">
       <c r="F40" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="G40" s="34" t="s">
         <v>608</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -9663,10 +9753,11 @@
     <hyperlink ref="G40" r:id="rId9" xr:uid="{76EE83BD-7400-4A46-978B-D25721A01204}"/>
     <hyperlink ref="B28" r:id="rId10" xr:uid="{C5ACF554-92E1-4EE1-9BA9-3999DE03B357}"/>
     <hyperlink ref="B18" r:id="rId11" xr:uid="{D7C56EA9-B97D-4FCE-9474-2C5FB0F6C524}"/>
+    <hyperlink ref="B24" r:id="rId12" xr:uid="{F05F2EE6-3271-4BA2-A513-8FF980C184CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId12"/>
-  <legacyDrawing r:id="rId13"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId13"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -9681,31 +9772,31 @@
       <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1"/>
-    <col min="8" max="8" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1"/>
-    <col min="11" max="11" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="8" style="1"/>
-    <col min="14" max="14" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L1" s="41">
         <f>AVERAGE(L3:L6)</f>
         <v>10.8</v>
       </c>
     </row>
-    <row r="2" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>400</v>
       </c>
@@ -9737,7 +9828,7 @@
         <v>408</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>410</v>
@@ -9746,18 +9837,18 @@
         <v>403</v>
       </c>
     </row>
-    <row r="3" spans="2:14" s="42" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="42" t="s">
         <v>404</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E3" s="43" t="s">
         <v>416</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G3" s="43">
         <v>2020</v>
@@ -9781,10 +9872,10 @@
         <v>411</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.15">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>409</v>
       </c>
@@ -9795,7 +9886,7 @@
         <v>416</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G4" s="4">
         <v>1984</v>
@@ -9822,7 +9913,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>417</v>
       </c>
@@ -9833,7 +9924,7 @@
         <v>416</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G5" s="4">
         <v>1997</v>
@@ -9854,18 +9945,18 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>613</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>614</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>416</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G6" s="4">
         <v>1988</v>

</xml_diff>

<commit_message>
Add NORSE to Overview - Airlines
</commit_message>
<xml_diff>
--- a/Overview - Airlines.xlsx
+++ b/Overview - Airlines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC85C29-BE69-4184-BFE6-8FB1EC4F6FE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D42383F-D9A6-4E8B-B0AE-CE53199338D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="495" windowWidth="32400" windowHeight="18795" activeTab="2" xr2:uid="{B2904301-D094-B04B-9DD3-24058A51C014}"/>
   </bookViews>
@@ -311,7 +311,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="658">
   <si>
     <t>Ticker</t>
   </si>
@@ -2264,6 +2264,27 @@
   </si>
   <si>
     <t>Flag carrier for China, 1 of "Big Three" Chinese airlines</t>
+  </si>
+  <si>
+    <t>OSE</t>
+  </si>
+  <si>
+    <t>NORSE.OL</t>
+  </si>
+  <si>
+    <t>Norse Atlantic ASA</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>NOKGBP</t>
+  </si>
+  <si>
+    <t>Norwegian low-cost long-haul airline operating fleet of 787 between North America &amp; Europe</t>
+  </si>
+  <si>
+    <t>Arendal, Norway</t>
   </si>
 </sst>
 </file>
@@ -2772,58 +2793,57 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Accounts"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="14">
-          <cell r="C14">
-            <v>1988</v>
+        <row r="6">
+          <cell r="C6">
+            <v>48.6</v>
           </cell>
         </row>
-        <row r="16">
-          <cell r="C16">
-            <v>16</v>
+        <row r="7">
+          <cell r="C7">
+            <v>17.54</v>
           </cell>
         </row>
-        <row r="17">
-          <cell r="C17">
-            <v>14.4</v>
+        <row r="8">
+          <cell r="C8">
+            <v>852.44399999999996</v>
           </cell>
         </row>
-        <row r="18">
-          <cell r="C18">
+        <row r="11">
+          <cell r="C11">
             <v>0</v>
           </cell>
         </row>
-        <row r="20">
-          <cell r="C20" t="str">
-            <v>FY21/22</v>
-          </cell>
-          <cell r="D20">
-            <v>45141</v>
+        <row r="12">
+          <cell r="C12">
+            <v>852.44399999999996</v>
           </cell>
         </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="18">
-          <cell r="L18">
-            <v>3.7691802910883844E-2</v>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Warsaw, Poland</v>
           </cell>
         </row>
-        <row r="19">
-          <cell r="L19">
-            <v>-7.2462158441842464E-2</v>
+        <row r="24">
+          <cell r="C24">
+            <v>2009</v>
           </cell>
         </row>
-        <row r="20">
-          <cell r="L20">
-            <v>-8.0967153446236284E-2</v>
+        <row r="25">
+          <cell r="C25">
+            <v>2015</v>
           </cell>
         </row>
-        <row r="21">
-          <cell r="K21">
-            <v>0.18785583230649008</v>
+        <row r="27">
+          <cell r="C27">
+            <v>26</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>6</v>
           </cell>
         </row>
       </sheetData>
@@ -2837,57 +2857,58 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Accounts"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>48.6</v>
+        <row r="14">
+          <cell r="C14">
+            <v>1988</v>
           </cell>
         </row>
-        <row r="7">
-          <cell r="C7">
-            <v>17.54</v>
+        <row r="16">
+          <cell r="C16">
+            <v>16</v>
           </cell>
         </row>
-        <row r="8">
-          <cell r="C8">
-            <v>852.44399999999996</v>
+        <row r="17">
+          <cell r="C17">
+            <v>14.4</v>
           </cell>
         </row>
-        <row r="11">
-          <cell r="C11">
+        <row r="18">
+          <cell r="C18">
             <v>0</v>
           </cell>
         </row>
-        <row r="12">
-          <cell r="C12">
-            <v>852.44399999999996</v>
+        <row r="20">
+          <cell r="C20" t="str">
+            <v>FY21/22</v>
+          </cell>
+          <cell r="D20">
+            <v>45141</v>
           </cell>
         </row>
-        <row r="23">
-          <cell r="C23" t="str">
-            <v>Warsaw, Poland</v>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="18">
+          <cell r="L18">
+            <v>3.7691802910883844E-2</v>
           </cell>
         </row>
-        <row r="24">
-          <cell r="C24">
-            <v>2009</v>
+        <row r="19">
+          <cell r="L19">
+            <v>-7.2462158441842464E-2</v>
           </cell>
         </row>
-        <row r="25">
-          <cell r="C25">
-            <v>2015</v>
+        <row r="20">
+          <cell r="L20">
+            <v>-8.0967153446236284E-2</v>
           </cell>
         </row>
-        <row r="27">
-          <cell r="C27">
-            <v>26</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>6</v>
+        <row r="21">
+          <cell r="K21">
+            <v>0.18785583230649008</v>
           </cell>
         </row>
       </sheetData>
@@ -8398,13 +8419,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EFA335-9DBB-3F42-9865-C3FC493C69CD}">
-  <dimension ref="B1:AD40"/>
+  <dimension ref="B1:AD42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8551,7 +8572,7 @@
         <v>383</v>
       </c>
       <c r="F3" s="28">
-        <f>[1]Main!$C$6*H33</f>
+        <f>[1]Main!$C$6*H34</f>
         <v>58.001999999999995</v>
       </c>
       <c r="G3" s="26">
@@ -8559,15 +8580,15 @@
         <v>227.43</v>
       </c>
       <c r="H3" s="26">
-        <f>[1]Main!$C$12*H33</f>
+        <f>[1]Main!$C$12*H34</f>
         <v>13191.394859999999</v>
       </c>
       <c r="I3" s="39">
-        <f>[1]Main!$C$11*H33</f>
+        <f>[1]Main!$C$11*H34</f>
         <v>0</v>
       </c>
       <c r="J3" s="26">
-        <f>[1]Main!$C$12*H33</f>
+        <f>[1]Main!$C$12*H34</f>
         <v>13191.394859999999</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -8611,7 +8632,7 @@
         <v>430</v>
       </c>
       <c r="F4" s="51">
-        <f>[2]Main!$C$6*H36</f>
+        <f>[2]Main!$C$6*H37</f>
         <v>19.570099999999996</v>
       </c>
       <c r="G4" s="52">
@@ -8619,15 +8640,15 @@
         <v>385.26</v>
       </c>
       <c r="H4" s="52">
-        <f>[2]Main!$C$8*H36</f>
+        <f>[2]Main!$C$8*H37</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="I4" s="52">
-        <f>[2]Main!$C$11*H36</f>
+        <f>[2]Main!$C$11*H37</f>
         <v>0</v>
       </c>
       <c r="J4" s="52">
-        <f>[2]Main!$C$12*H36</f>
+        <f>[2]Main!$C$12*H37</f>
         <v>7539.5767259999993</v>
       </c>
       <c r="K4" s="42" t="s">
@@ -8744,7 +8765,7 @@
         <v>383</v>
       </c>
       <c r="F6" s="51">
-        <f>[4]Main!$C$6*H33</f>
+        <f>[4]Main!$C$6*H34</f>
         <v>35.1372</v>
       </c>
       <c r="G6" s="52">
@@ -8752,15 +8773,15 @@
         <v>126.5</v>
       </c>
       <c r="H6" s="52">
-        <f>[4]Main!$C$8*H33</f>
+        <f>[4]Main!$C$8*H34</f>
         <v>4444.8557999999994</v>
       </c>
       <c r="I6" s="52">
-        <f>[4]Main!$C$11*H33</f>
+        <f>[4]Main!$C$11*H34</f>
         <v>942.48</v>
       </c>
       <c r="J6" s="52">
-        <f>[4]Main!$C$12*H33</f>
+        <f>[4]Main!$C$12*H34</f>
         <v>3502.3757999999998</v>
       </c>
       <c r="K6" s="42" t="s">
@@ -8970,7 +8991,7 @@
         <v>383</v>
       </c>
       <c r="F9" s="51">
-        <f>[7]Main!$C$6*H33</f>
+        <f>[7]Main!$C$6*H34</f>
         <v>23.9148</v>
       </c>
       <c r="G9" s="52">
@@ -8978,15 +8999,15 @@
         <v>73.998000000000005</v>
       </c>
       <c r="H9" s="52">
-        <f>[7]Main!$C$8*H33</f>
+        <f>[7]Main!$C$8*H34</f>
         <v>1769.6473704000002</v>
       </c>
       <c r="I9" s="52">
-        <f>[7]Main!$C$11*H33</f>
+        <f>[7]Main!$C$11*H34</f>
         <v>-1104.7318799999998</v>
       </c>
       <c r="J9" s="52">
-        <f>[7]Main!$C$12*H33</f>
+        <f>[7]Main!$C$12*H34</f>
         <v>2874.3792504000003</v>
       </c>
       <c r="K9" s="42" t="s">
@@ -9224,7 +9245,7 @@
         <v>40.14</v>
       </c>
       <c r="H15" s="32">
-        <f>(F15*H33)*592.96</f>
+        <f>(F15*H34)*592.96</f>
         <v>19993.188095999998</v>
       </c>
       <c r="I15" s="26"/>
@@ -9258,7 +9279,7 @@
       </c>
       <c r="G16" s="30"/>
       <c r="H16" s="32">
-        <f>(F16*H35)*320.79</f>
+        <f>(F16*H36)*320.79</f>
         <v>4536.6121800000001</v>
       </c>
       <c r="I16" s="26"/>
@@ -9290,7 +9311,7 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="H17" s="32">
-        <f>(F17*H33)*320.79</f>
+        <f>(F17*H34)*320.79</f>
         <v>2570.6827439999997</v>
       </c>
       <c r="I17" s="26"/>
@@ -9320,7 +9341,7 @@
         <v>383</v>
       </c>
       <c r="F18" s="49">
-        <f>[9]Main!$C$6*H33</f>
+        <f>[9]Main!$C$6*H34</f>
         <v>28.3416</v>
       </c>
       <c r="I18" s="26"/>
@@ -9458,7 +9479,7 @@
         <v>2570</v>
       </c>
       <c r="H23" s="32">
-        <f>(F23*G23)*H34</f>
+        <f>(F23*G23)*H35</f>
         <v>3122.7427499999999</v>
       </c>
       <c r="I23" s="26"/>
@@ -9489,197 +9510,222 @@
         <v>646</v>
       </c>
       <c r="F24" s="49">
-        <f>[11]Main!$C$6*H37</f>
+        <f>[10]Main!$C$6*H38</f>
         <v>9.234</v>
       </c>
       <c r="G24" s="1">
-        <f>[11]Main!$C$7</f>
+        <f>[10]Main!$C$7</f>
         <v>17.54</v>
       </c>
       <c r="H24" s="32">
-        <f>[11]Main!$C$8*H37</f>
+        <f>[10]Main!$C$8*H38</f>
         <v>161.96436</v>
       </c>
       <c r="I24" s="26">
-        <f>[11]Main!$C$11*H37</f>
+        <f>[10]Main!$C$11*H38</f>
         <v>0</v>
       </c>
       <c r="J24" s="26">
-        <f>[11]Main!$C$12*H37</f>
+        <f>[10]Main!$C$12*H38</f>
         <v>161.96436</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>648</v>
       </c>
       <c r="S24" s="4">
-        <f>[11]Main!$C$27</f>
+        <f>[10]Main!$C$27</f>
         <v>26</v>
       </c>
       <c r="T24" s="4">
-        <f>[11]Main!$C$28</f>
+        <f>[10]Main!$C$28</f>
         <v>6</v>
       </c>
       <c r="X24" s="4"/>
       <c r="AB24" s="4">
-        <f>[11]Main!$C$24</f>
+        <f>[10]Main!$C$24</f>
         <v>2009</v>
       </c>
       <c r="AC24" s="4" t="str">
-        <f>[11]Main!$C$23</f>
+        <f>[10]Main!$C$23</f>
         <v>Warsaw, Poland</v>
       </c>
       <c r="AD24" s="4">
-        <f>[11]Main!$C$25</f>
+        <f>[10]Main!$C$25</f>
         <v>2015</v>
       </c>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="H25" s="32"/>
-    </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B27" s="46" t="s">
+      <c r="B25" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="F25" s="1">
+        <f>21.8*H39</f>
+        <v>1.5913999999999999</v>
+      </c>
+      <c r="G25" s="1">
+        <v>66.52</v>
+      </c>
+      <c r="H25" s="32">
+        <f>G25*F25</f>
+        <v>105.85992799999998</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="AB25" s="4">
+        <v>2021</v>
+      </c>
+      <c r="AC25" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="AD25" s="4">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="H26" s="32"/>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B28" s="46" t="s">
         <v>619</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="48"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="48"/>
-      <c r="R27" s="48"/>
-      <c r="S27" s="47"/>
-      <c r="T27" s="47"/>
-      <c r="U27" s="48"/>
-      <c r="V27" s="48"/>
-      <c r="W27" s="48"/>
-      <c r="X27" s="48"/>
-      <c r="Y27" s="48"/>
-      <c r="Z27" s="47"/>
-      <c r="AA27" s="47"/>
-      <c r="AB27" s="48"/>
-      <c r="AC27" s="48"/>
-      <c r="AD27" s="48"/>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B28" s="25" t="s">
+      <c r="C28" s="46"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="47"/>
+      <c r="T28" s="47"/>
+      <c r="U28" s="48"/>
+      <c r="V28" s="48"/>
+      <c r="W28" s="48"/>
+      <c r="X28" s="48"/>
+      <c r="Y28" s="48"/>
+      <c r="Z28" s="47"/>
+      <c r="AA28" s="47"/>
+      <c r="AB28" s="48"/>
+      <c r="AC28" s="48"/>
+      <c r="AD28" s="48"/>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B29" s="25" t="s">
         <v>620</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="D29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F28" s="45" t="s">
+      <c r="F29" s="45" t="s">
         <v>622</v>
       </c>
-      <c r="G28" s="45" t="s">
+      <c r="G29" s="45" t="s">
         <v>622</v>
       </c>
-      <c r="H28" s="45" t="s">
+      <c r="H29" s="45" t="s">
         <v>622</v>
       </c>
-      <c r="I28" s="45" t="s">
+      <c r="I29" s="45" t="s">
         <v>622</v>
       </c>
-      <c r="J28" s="45" t="s">
+      <c r="J29" s="45" t="s">
         <v>622</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="L28" s="22">
-        <f>[10]Accounts!$L$18</f>
+      <c r="L29" s="22">
+        <f>[11]Accounts!$L$18</f>
         <v>3.7691802910883844E-2</v>
       </c>
-      <c r="M28" s="22">
-        <f>[10]Accounts!$L$19</f>
+      <c r="M29" s="22">
+        <f>[11]Accounts!$L$19</f>
         <v>-7.2462158441842464E-2</v>
       </c>
-      <c r="N28" s="22">
-        <f>[10]Accounts!$L$20</f>
+      <c r="N29" s="22">
+        <f>[11]Accounts!$L$20</f>
         <v>-8.0967153446236284E-2</v>
       </c>
-      <c r="O28" s="22">
-        <f>[10]Accounts!$K$21</f>
+      <c r="O29" s="22">
+        <f>[11]Accounts!$K$21</f>
         <v>0.18785583230649008</v>
       </c>
-      <c r="S28" s="4">
-        <f>[10]Main!$C$16</f>
+      <c r="S29" s="4">
+        <f>[11]Main!$C$16</f>
         <v>16</v>
       </c>
-      <c r="T28" s="4">
-        <f>[10]Main!$C$18</f>
+      <c r="T29" s="4">
+        <f>[11]Main!$C$18</f>
         <v>0</v>
       </c>
-      <c r="U28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="W28" s="4">
-        <f>[10]Main!$C$17</f>
+      <c r="U29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="W29" s="4">
+        <f>[11]Main!$C$17</f>
         <v>14.4</v>
       </c>
-      <c r="Z28" s="4" t="str">
-        <f>[10]Main!$C$20</f>
+      <c r="Z29" s="4" t="str">
+        <f>[11]Main!$C$20</f>
         <v>FY21/22</v>
       </c>
-      <c r="AA28" s="35">
-        <f>[10]Main!$D$20</f>
+      <c r="AA29" s="35">
+        <f>[11]Main!$D$20</f>
         <v>45141</v>
       </c>
-      <c r="AB28" s="4">
-        <f>[10]Main!$C$14</f>
+      <c r="AB29" s="4">
+        <f>[11]Main!$C$14</f>
         <v>1988</v>
       </c>
-      <c r="AC28" s="4" t="s">
+      <c r="AC29" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="AD28" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="D32" s="1"/>
-      <c r="F32" s="64" t="s">
-        <v>378</v>
-      </c>
-      <c r="G32" s="65"/>
-      <c r="H32" s="66"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
+      <c r="AD29" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="33" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D33" s="1"/>
-      <c r="F33" s="60" t="s">
-        <v>379</v>
-      </c>
-      <c r="G33" s="61"/>
-      <c r="H33" s="58">
-        <v>0.84</v>
-      </c>
+      <c r="F33" s="64" t="s">
+        <v>378</v>
+      </c>
+      <c r="G33" s="65"/>
+      <c r="H33" s="66"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
     <row r="34" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D34" s="1"/>
-      <c r="F34" s="62" t="s">
-        <v>380</v>
-      </c>
-      <c r="G34" s="63"/>
-      <c r="H34" s="23">
-        <v>0.85</v>
+      <c r="F34" s="60" t="s">
+        <v>379</v>
+      </c>
+      <c r="G34" s="61"/>
+      <c r="H34" s="58">
+        <v>0.84</v>
       </c>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
@@ -9687,59 +9733,81 @@
     <row r="35" spans="4:20" x14ac:dyDescent="0.2">
       <c r="D35" s="1"/>
       <c r="F35" s="62" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="G35" s="63"/>
       <c r="H35" s="23">
-        <v>6.0000000000000001E-3</v>
+        <v>0.85</v>
       </c>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D36" s="1"/>
       <c r="F36" s="62" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="G36" s="63"/>
       <c r="H36" s="23">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+    </row>
+    <row r="37" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F37" s="62" t="s">
+        <v>431</v>
+      </c>
+      <c r="G37" s="63"/>
+      <c r="H37" s="23">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="F37" s="68" t="s">
+    <row r="38" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F38" s="62" t="s">
         <v>647</v>
       </c>
-      <c r="G37" s="69"/>
-      <c r="H37" s="24">
+      <c r="G38" s="63"/>
+      <c r="H38" s="23">
         <v>0.19</v>
       </c>
     </row>
     <row r="39" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="F39" s="64" t="s">
+      <c r="F39" s="68" t="s">
+        <v>655</v>
+      </c>
+      <c r="G39" s="69"/>
+      <c r="H39" s="24">
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F41" s="64" t="s">
         <v>410</v>
       </c>
-      <c r="G39" s="65"/>
-      <c r="H39" s="66"/>
-    </row>
-    <row r="40" spans="4:20" x14ac:dyDescent="0.2">
-      <c r="F40" s="1" t="s">
+      <c r="G41" s="65"/>
+      <c r="H41" s="66"/>
+    </row>
+    <row r="42" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="G40" s="34" t="s">
+      <c r="G42" s="34" t="s">
         <v>608</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="F33:G33"/>
     <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F37:G37"/>
     <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
     <mergeCell ref="B12:U12"/>
-    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{3B58BCD6-42FB-9B41-82F9-2CB3C0FF35E5}"/>
@@ -9750,8 +9818,8 @@
     <hyperlink ref="B4" r:id="rId6" xr:uid="{28605697-2E3F-4D0E-BA6A-013F294DB301}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{7F471098-FF05-4C1A-AA9F-8A6A66E1327B}"/>
     <hyperlink ref="B3" r:id="rId8" xr:uid="{340E3559-5E25-4E5A-9CCF-84716432B315}"/>
-    <hyperlink ref="G40" r:id="rId9" xr:uid="{76EE83BD-7400-4A46-978B-D25721A01204}"/>
-    <hyperlink ref="B28" r:id="rId10" xr:uid="{C5ACF554-92E1-4EE1-9BA9-3999DE03B357}"/>
+    <hyperlink ref="G42" r:id="rId9" xr:uid="{76EE83BD-7400-4A46-978B-D25721A01204}"/>
+    <hyperlink ref="B29" r:id="rId10" xr:uid="{C5ACF554-92E1-4EE1-9BA9-3999DE03B357}"/>
     <hyperlink ref="B18" r:id="rId11" xr:uid="{D7C56EA9-B97D-4FCE-9474-2C5FB0F6C524}"/>
     <hyperlink ref="B24" r:id="rId12" xr:uid="{F05F2EE6-3271-4BA2-A513-8FF980C184CC}"/>
   </hyperlinks>
@@ -9962,15 +10030,15 @@
         <v>1988</v>
       </c>
       <c r="I6" s="4">
-        <f>[10]Main!$C$16</f>
+        <f>[11]Main!$C$16</f>
         <v>16</v>
       </c>
       <c r="J6" s="4">
-        <f>[10]Main!$C$18</f>
+        <f>[11]Main!$C$18</f>
         <v>0</v>
       </c>
       <c r="L6" s="4">
-        <f>[10]Main!$C$17</f>
+        <f>[11]Main!$C$17</f>
         <v>14.4</v>
       </c>
       <c r="M6" s="34" t="s">

</xml_diff>